<commit_message>
feat: add task which missed in Task template to `lazy` students
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/rawSource/Mentor score.xlsx
+++ b/mentor-dashboard/src/rawSource/Mentor score.xlsx
@@ -9646,7 +9646,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -9703,6 +9703,16 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -9727,10 +9737,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -9743,8 +9757,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10042,9 +10058,9 @@
   </sheetPr>
   <dimension ref="A1:H1865"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1214" sqref="E1214"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1252" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1300" sqref="D1300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -37341,7 +37357,7 @@
       <c r="B1214" s="11" t="s">
         <v>2952</v>
       </c>
-      <c r="C1214" s="11" t="s">
+      <c r="C1214" s="12" t="s">
         <v>2953</v>
       </c>
       <c r="D1214" s="2" t="s">
@@ -53083,7 +53099,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <phoneticPr fontId="0" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
@@ -56971,1705 +56987,1705 @@
     <hyperlink ref="B1299" r:id="rId3884"/>
     <hyperlink ref="C1299" r:id="rId3885"/>
     <hyperlink ref="E1299" r:id="rId3886" location="pullrequestreview-180533410"/>
-    <hyperlink ref="B1300" r:id="rId3887"/>
-    <hyperlink ref="C1300" r:id="rId3888"/>
-    <hyperlink ref="E1300" r:id="rId3889"/>
-    <hyperlink ref="B1301" r:id="rId3890"/>
-    <hyperlink ref="C1301" r:id="rId3891"/>
-    <hyperlink ref="E1301" r:id="rId3892"/>
-    <hyperlink ref="B1302" r:id="rId3893"/>
-    <hyperlink ref="C1302" r:id="rId3894"/>
-    <hyperlink ref="E1302" r:id="rId3895"/>
-    <hyperlink ref="B1303" r:id="rId3896"/>
-    <hyperlink ref="C1303" r:id="rId3897"/>
-    <hyperlink ref="E1303" r:id="rId3898" location="pullrequestreview-180535268"/>
-    <hyperlink ref="B1304" r:id="rId3899"/>
-    <hyperlink ref="C1304" r:id="rId3900"/>
-    <hyperlink ref="E1304" r:id="rId3901" location="pullrequestreview-180527806"/>
-    <hyperlink ref="B1305" r:id="rId3902"/>
-    <hyperlink ref="C1305" r:id="rId3903"/>
-    <hyperlink ref="E1305" r:id="rId3904" location="pullrequestreview-180537012"/>
-    <hyperlink ref="B1306" r:id="rId3905"/>
-    <hyperlink ref="C1306" r:id="rId3906"/>
-    <hyperlink ref="E1306" r:id="rId3907"/>
-    <hyperlink ref="B1307" r:id="rId3908"/>
-    <hyperlink ref="C1307" r:id="rId3909"/>
-    <hyperlink ref="E1307" r:id="rId3910"/>
-    <hyperlink ref="B1308" r:id="rId3911"/>
-    <hyperlink ref="C1308" r:id="rId3912"/>
-    <hyperlink ref="E1308" r:id="rId3913"/>
-    <hyperlink ref="B1309" r:id="rId3914"/>
-    <hyperlink ref="C1309" r:id="rId3915"/>
-    <hyperlink ref="E1309" r:id="rId3916"/>
-    <hyperlink ref="B1310" r:id="rId3917"/>
-    <hyperlink ref="C1310" r:id="rId3918"/>
-    <hyperlink ref="E1310" r:id="rId3919"/>
-    <hyperlink ref="B1311" r:id="rId3920"/>
-    <hyperlink ref="C1311" r:id="rId3921"/>
-    <hyperlink ref="E1311" r:id="rId3922"/>
-    <hyperlink ref="B1312" r:id="rId3923"/>
-    <hyperlink ref="C1312" r:id="rId3924"/>
-    <hyperlink ref="E1312" r:id="rId3925"/>
-    <hyperlink ref="B1313" r:id="rId3926"/>
-    <hyperlink ref="C1313" r:id="rId3927"/>
-    <hyperlink ref="E1313" r:id="rId3928"/>
-    <hyperlink ref="B1314" r:id="rId3929"/>
-    <hyperlink ref="C1314" r:id="rId3930"/>
-    <hyperlink ref="E1314" r:id="rId3931"/>
-    <hyperlink ref="B1315" r:id="rId3932"/>
-    <hyperlink ref="C1315" r:id="rId3933"/>
-    <hyperlink ref="E1315" r:id="rId3934"/>
-    <hyperlink ref="B1316" r:id="rId3935"/>
-    <hyperlink ref="C1316" r:id="rId3936"/>
-    <hyperlink ref="E1316" r:id="rId3937"/>
-    <hyperlink ref="B1317" r:id="rId3938"/>
-    <hyperlink ref="C1317" r:id="rId3939"/>
-    <hyperlink ref="E1317" r:id="rId3940"/>
-    <hyperlink ref="B1318" r:id="rId3941"/>
-    <hyperlink ref="C1318" r:id="rId3942"/>
-    <hyperlink ref="E1318" r:id="rId3943"/>
-    <hyperlink ref="B1319" r:id="rId3944"/>
-    <hyperlink ref="C1319" r:id="rId3945"/>
-    <hyperlink ref="E1319" r:id="rId3946"/>
-    <hyperlink ref="B1320" r:id="rId3947"/>
-    <hyperlink ref="C1320" r:id="rId3948"/>
-    <hyperlink ref="E1320" r:id="rId3949"/>
-    <hyperlink ref="B1321" r:id="rId3950"/>
-    <hyperlink ref="C1321" r:id="rId3951"/>
-    <hyperlink ref="E1321" r:id="rId3952"/>
-    <hyperlink ref="B1322" r:id="rId3953"/>
-    <hyperlink ref="C1322" r:id="rId3954"/>
-    <hyperlink ref="E1322" r:id="rId3955"/>
-    <hyperlink ref="B1323" r:id="rId3956"/>
-    <hyperlink ref="C1323" r:id="rId3957"/>
-    <hyperlink ref="E1323" r:id="rId3958"/>
-    <hyperlink ref="B1324" r:id="rId3959"/>
-    <hyperlink ref="C1324" r:id="rId3960"/>
-    <hyperlink ref="E1324" r:id="rId3961"/>
-    <hyperlink ref="B1325" r:id="rId3962"/>
-    <hyperlink ref="C1325" r:id="rId3963"/>
-    <hyperlink ref="E1325" r:id="rId3964"/>
-    <hyperlink ref="B1326" r:id="rId3965"/>
-    <hyperlink ref="C1326" r:id="rId3966"/>
-    <hyperlink ref="E1326" r:id="rId3967"/>
-    <hyperlink ref="B1327" r:id="rId3968"/>
-    <hyperlink ref="C1327" r:id="rId3969"/>
-    <hyperlink ref="E1327" r:id="rId3970"/>
-    <hyperlink ref="B1328" r:id="rId3971"/>
-    <hyperlink ref="C1328" r:id="rId3972"/>
-    <hyperlink ref="E1328" r:id="rId3973"/>
-    <hyperlink ref="B1329" r:id="rId3974"/>
-    <hyperlink ref="C1329" r:id="rId3975"/>
-    <hyperlink ref="E1329" r:id="rId3976"/>
-    <hyperlink ref="B1330" r:id="rId3977"/>
-    <hyperlink ref="C1330" r:id="rId3978"/>
-    <hyperlink ref="E1330" r:id="rId3979"/>
-    <hyperlink ref="B1331" r:id="rId3980"/>
-    <hyperlink ref="C1331" r:id="rId3981"/>
-    <hyperlink ref="E1331" r:id="rId3982"/>
-    <hyperlink ref="B1332" r:id="rId3983"/>
-    <hyperlink ref="C1332" r:id="rId3984"/>
-    <hyperlink ref="E1332" r:id="rId3985"/>
-    <hyperlink ref="B1333" r:id="rId3986"/>
-    <hyperlink ref="C1333" r:id="rId3987"/>
-    <hyperlink ref="E1333" r:id="rId3988"/>
-    <hyperlink ref="B1334" r:id="rId3989"/>
-    <hyperlink ref="C1334" r:id="rId3990"/>
-    <hyperlink ref="E1334" r:id="rId3991"/>
-    <hyperlink ref="B1335" r:id="rId3992"/>
-    <hyperlink ref="C1335" r:id="rId3993"/>
-    <hyperlink ref="E1335" r:id="rId3994"/>
-    <hyperlink ref="B1336" r:id="rId3995"/>
-    <hyperlink ref="C1336" r:id="rId3996"/>
-    <hyperlink ref="E1336" r:id="rId3997"/>
-    <hyperlink ref="B1337" r:id="rId3998"/>
-    <hyperlink ref="C1337" r:id="rId3999"/>
-    <hyperlink ref="E1337" r:id="rId4000"/>
-    <hyperlink ref="B1338" r:id="rId4001"/>
-    <hyperlink ref="C1338" r:id="rId4002"/>
-    <hyperlink ref="E1338" r:id="rId4003"/>
-    <hyperlink ref="B1339" r:id="rId4004"/>
-    <hyperlink ref="C1339" r:id="rId4005"/>
-    <hyperlink ref="E1339" r:id="rId4006"/>
-    <hyperlink ref="B1340" r:id="rId4007"/>
-    <hyperlink ref="C1340" r:id="rId4008"/>
-    <hyperlink ref="E1340" r:id="rId4009"/>
-    <hyperlink ref="B1341" r:id="rId4010"/>
-    <hyperlink ref="C1341" r:id="rId4011"/>
-    <hyperlink ref="E1341" r:id="rId4012"/>
-    <hyperlink ref="B1342" r:id="rId4013"/>
-    <hyperlink ref="C1342" r:id="rId4014"/>
-    <hyperlink ref="E1342" r:id="rId4015"/>
-    <hyperlink ref="B1343" r:id="rId4016"/>
-    <hyperlink ref="C1343" r:id="rId4017"/>
-    <hyperlink ref="E1343" r:id="rId4018"/>
-    <hyperlink ref="B1344" r:id="rId4019"/>
-    <hyperlink ref="C1344" r:id="rId4020"/>
-    <hyperlink ref="E1344" r:id="rId4021"/>
-    <hyperlink ref="B1345" r:id="rId4022"/>
-    <hyperlink ref="C1345" r:id="rId4023"/>
-    <hyperlink ref="E1345" r:id="rId4024"/>
-    <hyperlink ref="B1346" r:id="rId4025"/>
-    <hyperlink ref="C1346" r:id="rId4026"/>
-    <hyperlink ref="E1346" r:id="rId4027"/>
-    <hyperlink ref="B1347" r:id="rId4028"/>
-    <hyperlink ref="C1347" r:id="rId4029"/>
-    <hyperlink ref="E1347" r:id="rId4030"/>
-    <hyperlink ref="B1348" r:id="rId4031"/>
-    <hyperlink ref="C1348" r:id="rId4032"/>
-    <hyperlink ref="E1348" r:id="rId4033"/>
-    <hyperlink ref="B1349" r:id="rId4034"/>
-    <hyperlink ref="C1349" r:id="rId4035"/>
-    <hyperlink ref="E1349" r:id="rId4036"/>
-    <hyperlink ref="B1350" r:id="rId4037"/>
-    <hyperlink ref="C1350" r:id="rId4038"/>
-    <hyperlink ref="E1350" r:id="rId4039"/>
-    <hyperlink ref="B1351" r:id="rId4040"/>
-    <hyperlink ref="C1351" r:id="rId4041"/>
-    <hyperlink ref="E1351" r:id="rId4042"/>
-    <hyperlink ref="B1352" r:id="rId4043"/>
-    <hyperlink ref="C1352" r:id="rId4044"/>
-    <hyperlink ref="E1352" r:id="rId4045"/>
-    <hyperlink ref="B1353" r:id="rId4046"/>
-    <hyperlink ref="C1353" r:id="rId4047"/>
-    <hyperlink ref="E1353" r:id="rId4048"/>
-    <hyperlink ref="B1354" r:id="rId4049"/>
-    <hyperlink ref="C1354" r:id="rId4050"/>
-    <hyperlink ref="E1354" r:id="rId4051"/>
-    <hyperlink ref="B1355" r:id="rId4052"/>
-    <hyperlink ref="C1355" r:id="rId4053"/>
-    <hyperlink ref="E1355" r:id="rId4054"/>
-    <hyperlink ref="B1356" r:id="rId4055"/>
-    <hyperlink ref="C1356" r:id="rId4056"/>
-    <hyperlink ref="E1356" r:id="rId4057"/>
-    <hyperlink ref="G1356" r:id="rId4058"/>
-    <hyperlink ref="B1357" r:id="rId4059"/>
-    <hyperlink ref="C1357" r:id="rId4060"/>
-    <hyperlink ref="E1357" r:id="rId4061"/>
-    <hyperlink ref="B1358" r:id="rId4062"/>
-    <hyperlink ref="C1358" r:id="rId4063"/>
-    <hyperlink ref="E1358" r:id="rId4064"/>
-    <hyperlink ref="B1359" r:id="rId4065"/>
-    <hyperlink ref="C1359" r:id="rId4066"/>
-    <hyperlink ref="E1359" r:id="rId4067"/>
-    <hyperlink ref="B1360" r:id="rId4068"/>
-    <hyperlink ref="C1360" r:id="rId4069"/>
-    <hyperlink ref="E1360" r:id="rId4070"/>
-    <hyperlink ref="B1361" r:id="rId4071"/>
-    <hyperlink ref="C1361" r:id="rId4072"/>
-    <hyperlink ref="E1361" r:id="rId4073"/>
-    <hyperlink ref="B1362" r:id="rId4074"/>
-    <hyperlink ref="C1362" r:id="rId4075"/>
-    <hyperlink ref="E1362" r:id="rId4076"/>
-    <hyperlink ref="B1363" r:id="rId4077"/>
-    <hyperlink ref="C1363" r:id="rId4078"/>
-    <hyperlink ref="E1363" r:id="rId4079"/>
-    <hyperlink ref="B1364" r:id="rId4080"/>
-    <hyperlink ref="C1364" r:id="rId4081"/>
-    <hyperlink ref="E1364" r:id="rId4082"/>
-    <hyperlink ref="B1365" r:id="rId4083"/>
-    <hyperlink ref="C1365" r:id="rId4084"/>
-    <hyperlink ref="E1365" r:id="rId4085"/>
-    <hyperlink ref="B1366" r:id="rId4086"/>
-    <hyperlink ref="C1366" r:id="rId4087"/>
-    <hyperlink ref="E1366" r:id="rId4088"/>
-    <hyperlink ref="B1367" r:id="rId4089"/>
-    <hyperlink ref="C1367" r:id="rId4090"/>
-    <hyperlink ref="E1367" r:id="rId4091"/>
-    <hyperlink ref="B1368" r:id="rId4092"/>
-    <hyperlink ref="C1368" r:id="rId4093"/>
-    <hyperlink ref="E1368" r:id="rId4094"/>
-    <hyperlink ref="B1369" r:id="rId4095"/>
-    <hyperlink ref="C1369" r:id="rId4096"/>
-    <hyperlink ref="E1369" r:id="rId4097"/>
-    <hyperlink ref="B1370" r:id="rId4098"/>
-    <hyperlink ref="C1370" r:id="rId4099"/>
-    <hyperlink ref="E1370" r:id="rId4100"/>
-    <hyperlink ref="B1371" r:id="rId4101"/>
-    <hyperlink ref="C1371" r:id="rId4102"/>
-    <hyperlink ref="E1371" r:id="rId4103"/>
-    <hyperlink ref="B1372" r:id="rId4104"/>
-    <hyperlink ref="C1372" r:id="rId4105"/>
-    <hyperlink ref="E1372" r:id="rId4106"/>
-    <hyperlink ref="B1373" r:id="rId4107"/>
-    <hyperlink ref="C1373" r:id="rId4108"/>
-    <hyperlink ref="E1373" r:id="rId4109"/>
-    <hyperlink ref="B1374" r:id="rId4110"/>
-    <hyperlink ref="C1374" r:id="rId4111"/>
-    <hyperlink ref="E1374" r:id="rId4112"/>
-    <hyperlink ref="B1375" r:id="rId4113"/>
-    <hyperlink ref="C1375" r:id="rId4114"/>
-    <hyperlink ref="E1375" r:id="rId4115"/>
-    <hyperlink ref="B1376" r:id="rId4116"/>
-    <hyperlink ref="C1376" r:id="rId4117"/>
-    <hyperlink ref="E1376" r:id="rId4118"/>
-    <hyperlink ref="B1377" r:id="rId4119"/>
-    <hyperlink ref="C1377" r:id="rId4120"/>
-    <hyperlink ref="E1377" r:id="rId4121" location="pullrequestreview-181806388"/>
-    <hyperlink ref="B1378" r:id="rId4122"/>
-    <hyperlink ref="C1378" r:id="rId4123"/>
-    <hyperlink ref="E1378" r:id="rId4124"/>
-    <hyperlink ref="B1379" r:id="rId4125"/>
-    <hyperlink ref="C1379" r:id="rId4126"/>
-    <hyperlink ref="E1379" r:id="rId4127"/>
-    <hyperlink ref="B1380" r:id="rId4128"/>
-    <hyperlink ref="C1380" r:id="rId4129"/>
-    <hyperlink ref="E1380" r:id="rId4130"/>
-    <hyperlink ref="B1381" r:id="rId4131"/>
-    <hyperlink ref="C1381" r:id="rId4132"/>
-    <hyperlink ref="E1381" r:id="rId4133"/>
-    <hyperlink ref="B1382" r:id="rId4134"/>
-    <hyperlink ref="C1382" r:id="rId4135"/>
-    <hyperlink ref="E1382" r:id="rId4136"/>
-    <hyperlink ref="B1383" r:id="rId4137"/>
-    <hyperlink ref="C1383" r:id="rId4138"/>
-    <hyperlink ref="E1383" r:id="rId4139"/>
-    <hyperlink ref="B1384" r:id="rId4140"/>
-    <hyperlink ref="C1384" r:id="rId4141"/>
-    <hyperlink ref="E1384" r:id="rId4142"/>
-    <hyperlink ref="B1385" r:id="rId4143"/>
-    <hyperlink ref="C1385" r:id="rId4144"/>
-    <hyperlink ref="E1385" r:id="rId4145"/>
-    <hyperlink ref="B1386" r:id="rId4146"/>
-    <hyperlink ref="C1386" r:id="rId4147"/>
-    <hyperlink ref="E1386" r:id="rId4148"/>
-    <hyperlink ref="B1387" r:id="rId4149"/>
-    <hyperlink ref="C1387" r:id="rId4150"/>
-    <hyperlink ref="E1387" r:id="rId4151"/>
-    <hyperlink ref="B1388" r:id="rId4152"/>
-    <hyperlink ref="C1388" r:id="rId4153"/>
-    <hyperlink ref="E1388" r:id="rId4154"/>
-    <hyperlink ref="B1389" r:id="rId4155"/>
-    <hyperlink ref="C1389" r:id="rId4156"/>
-    <hyperlink ref="E1389" r:id="rId4157"/>
-    <hyperlink ref="B1390" r:id="rId4158"/>
-    <hyperlink ref="C1390" r:id="rId4159"/>
-    <hyperlink ref="E1390" r:id="rId4160"/>
-    <hyperlink ref="B1391" r:id="rId4161"/>
-    <hyperlink ref="C1391" r:id="rId4162"/>
-    <hyperlink ref="E1391" r:id="rId4163"/>
-    <hyperlink ref="B1392" r:id="rId4164"/>
-    <hyperlink ref="C1392" r:id="rId4165"/>
-    <hyperlink ref="E1392" r:id="rId4166"/>
-    <hyperlink ref="B1393" r:id="rId4167"/>
-    <hyperlink ref="C1393" r:id="rId4168"/>
-    <hyperlink ref="E1393" r:id="rId4169"/>
-    <hyperlink ref="B1394" r:id="rId4170"/>
-    <hyperlink ref="C1394" r:id="rId4171"/>
-    <hyperlink ref="E1394" r:id="rId4172"/>
-    <hyperlink ref="B1395" r:id="rId4173"/>
-    <hyperlink ref="C1395" r:id="rId4174"/>
-    <hyperlink ref="E1395" r:id="rId4175"/>
-    <hyperlink ref="B1396" r:id="rId4176"/>
-    <hyperlink ref="C1396" r:id="rId4177"/>
-    <hyperlink ref="E1396" r:id="rId4178"/>
-    <hyperlink ref="B1397" r:id="rId4179"/>
-    <hyperlink ref="C1397" r:id="rId4180"/>
-    <hyperlink ref="E1397" r:id="rId4181"/>
-    <hyperlink ref="B1398" r:id="rId4182"/>
-    <hyperlink ref="C1398" r:id="rId4183"/>
-    <hyperlink ref="E1398" r:id="rId4184"/>
-    <hyperlink ref="B1399" r:id="rId4185"/>
-    <hyperlink ref="C1399" r:id="rId4186"/>
-    <hyperlink ref="E1399" r:id="rId4187"/>
-    <hyperlink ref="B1400" r:id="rId4188"/>
-    <hyperlink ref="C1400" r:id="rId4189"/>
-    <hyperlink ref="E1400" r:id="rId4190"/>
-    <hyperlink ref="B1401" r:id="rId4191"/>
-    <hyperlink ref="C1401" r:id="rId4192"/>
-    <hyperlink ref="E1401" r:id="rId4193"/>
-    <hyperlink ref="B1402" r:id="rId4194"/>
-    <hyperlink ref="C1402" r:id="rId4195"/>
-    <hyperlink ref="E1402" r:id="rId4196"/>
-    <hyperlink ref="B1403" r:id="rId4197"/>
-    <hyperlink ref="C1403" r:id="rId4198"/>
-    <hyperlink ref="E1403" r:id="rId4199"/>
-    <hyperlink ref="B1404" r:id="rId4200"/>
-    <hyperlink ref="C1404" r:id="rId4201"/>
-    <hyperlink ref="E1404" r:id="rId4202"/>
-    <hyperlink ref="B1405" r:id="rId4203"/>
-    <hyperlink ref="C1405" r:id="rId4204"/>
-    <hyperlink ref="E1405" r:id="rId4205"/>
-    <hyperlink ref="B1406" r:id="rId4206"/>
-    <hyperlink ref="C1406" r:id="rId4207"/>
-    <hyperlink ref="E1406" r:id="rId4208"/>
-    <hyperlink ref="B1407" r:id="rId4209"/>
-    <hyperlink ref="C1407" r:id="rId4210"/>
-    <hyperlink ref="E1407" r:id="rId4211"/>
-    <hyperlink ref="B1408" r:id="rId4212"/>
-    <hyperlink ref="C1408" r:id="rId4213"/>
-    <hyperlink ref="E1408" r:id="rId4214"/>
-    <hyperlink ref="B1409" r:id="rId4215"/>
-    <hyperlink ref="C1409" r:id="rId4216"/>
-    <hyperlink ref="E1409" r:id="rId4217"/>
-    <hyperlink ref="B1410" r:id="rId4218"/>
-    <hyperlink ref="C1410" r:id="rId4219"/>
-    <hyperlink ref="E1410" r:id="rId4220"/>
-    <hyperlink ref="B1411" r:id="rId4221"/>
-    <hyperlink ref="C1411" r:id="rId4222"/>
-    <hyperlink ref="E1411" r:id="rId4223"/>
-    <hyperlink ref="B1412" r:id="rId4224"/>
-    <hyperlink ref="C1412" r:id="rId4225"/>
-    <hyperlink ref="E1412" r:id="rId4226"/>
-    <hyperlink ref="B1413" r:id="rId4227"/>
-    <hyperlink ref="C1413" r:id="rId4228"/>
-    <hyperlink ref="E1413" r:id="rId4229"/>
-    <hyperlink ref="B1414" r:id="rId4230"/>
-    <hyperlink ref="C1414" r:id="rId4231"/>
-    <hyperlink ref="E1414" r:id="rId4232"/>
-    <hyperlink ref="B1415" r:id="rId4233"/>
-    <hyperlink ref="C1415" r:id="rId4234"/>
-    <hyperlink ref="E1415" r:id="rId4235"/>
-    <hyperlink ref="B1416" r:id="rId4236"/>
-    <hyperlink ref="C1416" r:id="rId4237"/>
-    <hyperlink ref="E1416" r:id="rId4238"/>
-    <hyperlink ref="B1417" r:id="rId4239"/>
-    <hyperlink ref="C1417" r:id="rId4240"/>
-    <hyperlink ref="E1417" r:id="rId4241"/>
-    <hyperlink ref="B1418" r:id="rId4242"/>
-    <hyperlink ref="C1418" r:id="rId4243"/>
-    <hyperlink ref="E1418" r:id="rId4244"/>
-    <hyperlink ref="B1419" r:id="rId4245"/>
-    <hyperlink ref="C1419" r:id="rId4246"/>
-    <hyperlink ref="E1419" r:id="rId4247"/>
-    <hyperlink ref="B1420" r:id="rId4248"/>
-    <hyperlink ref="C1420" r:id="rId4249"/>
-    <hyperlink ref="E1420" r:id="rId4250"/>
-    <hyperlink ref="B1421" r:id="rId4251"/>
-    <hyperlink ref="C1421" r:id="rId4252"/>
-    <hyperlink ref="E1421" r:id="rId4253"/>
-    <hyperlink ref="B1422" r:id="rId4254"/>
-    <hyperlink ref="C1422" r:id="rId4255"/>
-    <hyperlink ref="E1422" r:id="rId4256"/>
-    <hyperlink ref="B1423" r:id="rId4257"/>
-    <hyperlink ref="C1423" r:id="rId4258"/>
-    <hyperlink ref="E1423" r:id="rId4259"/>
-    <hyperlink ref="B1424" r:id="rId4260"/>
-    <hyperlink ref="C1424" r:id="rId4261"/>
-    <hyperlink ref="E1424" r:id="rId4262"/>
-    <hyperlink ref="B1425" r:id="rId4263"/>
-    <hyperlink ref="C1425" r:id="rId4264"/>
-    <hyperlink ref="E1425" r:id="rId4265"/>
-    <hyperlink ref="B1426" r:id="rId4266"/>
-    <hyperlink ref="C1426" r:id="rId4267"/>
-    <hyperlink ref="E1426" r:id="rId4268"/>
-    <hyperlink ref="B1427" r:id="rId4269"/>
-    <hyperlink ref="C1427" r:id="rId4270"/>
-    <hyperlink ref="E1427" r:id="rId4271"/>
-    <hyperlink ref="B1428" r:id="rId4272"/>
-    <hyperlink ref="C1428" r:id="rId4273"/>
-    <hyperlink ref="E1428" r:id="rId4274"/>
-    <hyperlink ref="B1429" r:id="rId4275"/>
-    <hyperlink ref="C1429" r:id="rId4276"/>
-    <hyperlink ref="E1429" r:id="rId4277"/>
-    <hyperlink ref="B1430" r:id="rId4278"/>
-    <hyperlink ref="C1430" r:id="rId4279"/>
-    <hyperlink ref="E1430" r:id="rId4280"/>
-    <hyperlink ref="B1431" r:id="rId4281"/>
-    <hyperlink ref="C1431" r:id="rId4282"/>
-    <hyperlink ref="E1431" r:id="rId4283"/>
-    <hyperlink ref="B1432" r:id="rId4284"/>
-    <hyperlink ref="C1432" r:id="rId4285"/>
-    <hyperlink ref="E1432" r:id="rId4286"/>
-    <hyperlink ref="B1433" r:id="rId4287"/>
-    <hyperlink ref="C1433" r:id="rId4288"/>
-    <hyperlink ref="E1433" r:id="rId4289"/>
-    <hyperlink ref="B1434" r:id="rId4290"/>
-    <hyperlink ref="C1434" r:id="rId4291"/>
-    <hyperlink ref="E1434" r:id="rId4292"/>
-    <hyperlink ref="B1435" r:id="rId4293"/>
-    <hyperlink ref="C1435" r:id="rId4294"/>
-    <hyperlink ref="E1435" r:id="rId4295"/>
-    <hyperlink ref="B1436" r:id="rId4296"/>
-    <hyperlink ref="C1436" r:id="rId4297"/>
-    <hyperlink ref="E1436" r:id="rId4298"/>
-    <hyperlink ref="B1437" r:id="rId4299"/>
-    <hyperlink ref="C1437" r:id="rId4300"/>
-    <hyperlink ref="E1437" r:id="rId4301"/>
-    <hyperlink ref="B1438" r:id="rId4302"/>
-    <hyperlink ref="C1438" r:id="rId4303"/>
-    <hyperlink ref="E1438" r:id="rId4304"/>
-    <hyperlink ref="B1439" r:id="rId4305"/>
-    <hyperlink ref="C1439" r:id="rId4306"/>
-    <hyperlink ref="E1439" r:id="rId4307"/>
-    <hyperlink ref="B1440" r:id="rId4308"/>
-    <hyperlink ref="C1440" r:id="rId4309"/>
-    <hyperlink ref="E1440" r:id="rId4310"/>
-    <hyperlink ref="B1441" r:id="rId4311"/>
-    <hyperlink ref="C1441" r:id="rId4312"/>
-    <hyperlink ref="E1441" r:id="rId4313"/>
-    <hyperlink ref="B1442" r:id="rId4314"/>
-    <hyperlink ref="C1442" r:id="rId4315"/>
-    <hyperlink ref="E1442" r:id="rId4316"/>
-    <hyperlink ref="B1443" r:id="rId4317"/>
-    <hyperlink ref="C1443" r:id="rId4318"/>
-    <hyperlink ref="E1443" r:id="rId4319"/>
-    <hyperlink ref="B1444" r:id="rId4320"/>
-    <hyperlink ref="C1444" r:id="rId4321"/>
-    <hyperlink ref="E1444" r:id="rId4322"/>
-    <hyperlink ref="B1445" r:id="rId4323"/>
-    <hyperlink ref="C1445" r:id="rId4324"/>
-    <hyperlink ref="E1445" r:id="rId4325"/>
-    <hyperlink ref="B1446" r:id="rId4326"/>
-    <hyperlink ref="C1446" r:id="rId4327"/>
-    <hyperlink ref="E1446" r:id="rId4328"/>
-    <hyperlink ref="B1447" r:id="rId4329"/>
-    <hyperlink ref="C1447" r:id="rId4330"/>
-    <hyperlink ref="E1447" r:id="rId4331"/>
-    <hyperlink ref="B1448" r:id="rId4332"/>
-    <hyperlink ref="C1448" r:id="rId4333"/>
-    <hyperlink ref="E1448" r:id="rId4334"/>
-    <hyperlink ref="B1449" r:id="rId4335"/>
-    <hyperlink ref="C1449" r:id="rId4336"/>
-    <hyperlink ref="E1449" r:id="rId4337"/>
-    <hyperlink ref="B1450" r:id="rId4338"/>
-    <hyperlink ref="C1450" r:id="rId4339"/>
-    <hyperlink ref="E1450" r:id="rId4340"/>
-    <hyperlink ref="B1451" r:id="rId4341"/>
-    <hyperlink ref="C1451" r:id="rId4342"/>
-    <hyperlink ref="E1451" r:id="rId4343"/>
-    <hyperlink ref="B1452" r:id="rId4344"/>
-    <hyperlink ref="C1452" r:id="rId4345"/>
-    <hyperlink ref="E1452" r:id="rId4346"/>
-    <hyperlink ref="B1453" r:id="rId4347"/>
-    <hyperlink ref="C1453" r:id="rId4348"/>
-    <hyperlink ref="E1453" r:id="rId4349"/>
-    <hyperlink ref="B1454" r:id="rId4350"/>
-    <hyperlink ref="C1454" r:id="rId4351"/>
-    <hyperlink ref="E1454" r:id="rId4352"/>
-    <hyperlink ref="B1455" r:id="rId4353"/>
-    <hyperlink ref="C1455" r:id="rId4354"/>
-    <hyperlink ref="E1455" r:id="rId4355"/>
-    <hyperlink ref="B1456" r:id="rId4356"/>
-    <hyperlink ref="C1456" r:id="rId4357"/>
-    <hyperlink ref="E1456" r:id="rId4358"/>
-    <hyperlink ref="B1457" r:id="rId4359"/>
-    <hyperlink ref="C1457" r:id="rId4360"/>
-    <hyperlink ref="E1457" r:id="rId4361"/>
-    <hyperlink ref="B1458" r:id="rId4362"/>
-    <hyperlink ref="C1458" r:id="rId4363"/>
-    <hyperlink ref="E1458" r:id="rId4364"/>
-    <hyperlink ref="B1459" r:id="rId4365"/>
-    <hyperlink ref="C1459" r:id="rId4366"/>
-    <hyperlink ref="E1459" r:id="rId4367"/>
-    <hyperlink ref="B1460" r:id="rId4368"/>
-    <hyperlink ref="C1460" r:id="rId4369"/>
-    <hyperlink ref="E1460" r:id="rId4370"/>
-    <hyperlink ref="B1461" r:id="rId4371"/>
-    <hyperlink ref="C1461" r:id="rId4372"/>
-    <hyperlink ref="E1461" r:id="rId4373"/>
-    <hyperlink ref="B1462" r:id="rId4374"/>
-    <hyperlink ref="C1462" r:id="rId4375"/>
-    <hyperlink ref="E1462" r:id="rId4376"/>
-    <hyperlink ref="B1463" r:id="rId4377"/>
-    <hyperlink ref="C1463" r:id="rId4378"/>
-    <hyperlink ref="E1463" r:id="rId4379"/>
-    <hyperlink ref="B1464" r:id="rId4380"/>
-    <hyperlink ref="C1464" r:id="rId4381"/>
-    <hyperlink ref="E1464" r:id="rId4382"/>
-    <hyperlink ref="B1465" r:id="rId4383"/>
-    <hyperlink ref="C1465" r:id="rId4384"/>
-    <hyperlink ref="E1465" r:id="rId4385"/>
-    <hyperlink ref="B1466" r:id="rId4386"/>
-    <hyperlink ref="C1466" r:id="rId4387"/>
-    <hyperlink ref="E1466" r:id="rId4388"/>
-    <hyperlink ref="B1467" r:id="rId4389"/>
-    <hyperlink ref="C1467" r:id="rId4390"/>
-    <hyperlink ref="E1467" r:id="rId4391"/>
-    <hyperlink ref="B1468" r:id="rId4392"/>
-    <hyperlink ref="C1468" r:id="rId4393"/>
-    <hyperlink ref="E1468" r:id="rId4394"/>
-    <hyperlink ref="B1469" r:id="rId4395"/>
-    <hyperlink ref="C1469" r:id="rId4396"/>
-    <hyperlink ref="E1469" r:id="rId4397"/>
-    <hyperlink ref="B1470" r:id="rId4398"/>
-    <hyperlink ref="C1470" r:id="rId4399"/>
-    <hyperlink ref="E1470" r:id="rId4400"/>
-    <hyperlink ref="B1471" r:id="rId4401"/>
-    <hyperlink ref="C1471" r:id="rId4402"/>
-    <hyperlink ref="E1471" r:id="rId4403"/>
-    <hyperlink ref="B1472" r:id="rId4404"/>
-    <hyperlink ref="C1472" r:id="rId4405"/>
-    <hyperlink ref="E1472" r:id="rId4406"/>
-    <hyperlink ref="B1473" r:id="rId4407"/>
-    <hyperlink ref="C1473" r:id="rId4408"/>
-    <hyperlink ref="E1473" r:id="rId4409"/>
-    <hyperlink ref="B1474" r:id="rId4410"/>
-    <hyperlink ref="C1474" r:id="rId4411"/>
-    <hyperlink ref="E1474" r:id="rId4412"/>
-    <hyperlink ref="B1475" r:id="rId4413"/>
-    <hyperlink ref="C1475" r:id="rId4414"/>
-    <hyperlink ref="E1475" r:id="rId4415"/>
-    <hyperlink ref="B1476" r:id="rId4416"/>
-    <hyperlink ref="C1476" r:id="rId4417"/>
-    <hyperlink ref="E1476" r:id="rId4418"/>
-    <hyperlink ref="B1477" r:id="rId4419"/>
-    <hyperlink ref="C1477" r:id="rId4420"/>
-    <hyperlink ref="E1477" r:id="rId4421"/>
-    <hyperlink ref="B1478" r:id="rId4422"/>
-    <hyperlink ref="C1478" r:id="rId4423"/>
-    <hyperlink ref="E1478" r:id="rId4424"/>
-    <hyperlink ref="B1479" r:id="rId4425"/>
-    <hyperlink ref="C1479" r:id="rId4426"/>
-    <hyperlink ref="E1479" r:id="rId4427"/>
-    <hyperlink ref="B1480" r:id="rId4428"/>
-    <hyperlink ref="C1480" r:id="rId4429"/>
-    <hyperlink ref="E1480" r:id="rId4430"/>
-    <hyperlink ref="B1481" r:id="rId4431"/>
-    <hyperlink ref="C1481" r:id="rId4432"/>
-    <hyperlink ref="E1481" r:id="rId4433"/>
-    <hyperlink ref="B1482" r:id="rId4434"/>
-    <hyperlink ref="C1482" r:id="rId4435"/>
-    <hyperlink ref="E1482" r:id="rId4436"/>
-    <hyperlink ref="B1483" r:id="rId4437"/>
-    <hyperlink ref="C1483" r:id="rId4438"/>
-    <hyperlink ref="E1483" r:id="rId4439"/>
-    <hyperlink ref="B1484" r:id="rId4440"/>
-    <hyperlink ref="C1484" r:id="rId4441"/>
-    <hyperlink ref="E1484" r:id="rId4442"/>
-    <hyperlink ref="B1485" r:id="rId4443"/>
-    <hyperlink ref="C1485" r:id="rId4444"/>
-    <hyperlink ref="E1485" r:id="rId4445"/>
-    <hyperlink ref="B1486" r:id="rId4446"/>
-    <hyperlink ref="C1486" r:id="rId4447"/>
-    <hyperlink ref="E1486" r:id="rId4448"/>
-    <hyperlink ref="B1487" r:id="rId4449"/>
-    <hyperlink ref="C1487" r:id="rId4450"/>
-    <hyperlink ref="E1487" r:id="rId4451"/>
-    <hyperlink ref="B1488" r:id="rId4452"/>
-    <hyperlink ref="C1488" r:id="rId4453"/>
-    <hyperlink ref="E1488" r:id="rId4454" location="/"/>
-    <hyperlink ref="B1489" r:id="rId4455"/>
-    <hyperlink ref="C1489" r:id="rId4456"/>
-    <hyperlink ref="E1489" r:id="rId4457"/>
-    <hyperlink ref="B1490" r:id="rId4458"/>
-    <hyperlink ref="C1490" r:id="rId4459"/>
-    <hyperlink ref="E1490" r:id="rId4460"/>
-    <hyperlink ref="B1491" r:id="rId4461"/>
-    <hyperlink ref="C1491" r:id="rId4462"/>
-    <hyperlink ref="E1491" r:id="rId4463"/>
-    <hyperlink ref="B1492" r:id="rId4464"/>
-    <hyperlink ref="C1492" r:id="rId4465"/>
-    <hyperlink ref="E1492" r:id="rId4466"/>
-    <hyperlink ref="B1493" r:id="rId4467"/>
-    <hyperlink ref="C1493" r:id="rId4468"/>
-    <hyperlink ref="E1493" r:id="rId4469"/>
-    <hyperlink ref="B1494" r:id="rId4470"/>
-    <hyperlink ref="C1494" r:id="rId4471"/>
-    <hyperlink ref="E1494" r:id="rId4472"/>
-    <hyperlink ref="B1495" r:id="rId4473"/>
-    <hyperlink ref="C1495" r:id="rId4474"/>
-    <hyperlink ref="E1495" r:id="rId4475"/>
-    <hyperlink ref="B1496" r:id="rId4476"/>
-    <hyperlink ref="C1496" r:id="rId4477"/>
-    <hyperlink ref="E1496" r:id="rId4478"/>
-    <hyperlink ref="B1497" r:id="rId4479"/>
-    <hyperlink ref="C1497" r:id="rId4480"/>
-    <hyperlink ref="E1497" r:id="rId4481"/>
-    <hyperlink ref="B1498" r:id="rId4482"/>
-    <hyperlink ref="C1498" r:id="rId4483"/>
-    <hyperlink ref="E1498" r:id="rId4484"/>
-    <hyperlink ref="B1499" r:id="rId4485"/>
-    <hyperlink ref="C1499" r:id="rId4486"/>
-    <hyperlink ref="E1499" r:id="rId4487"/>
-    <hyperlink ref="B1500" r:id="rId4488"/>
-    <hyperlink ref="C1500" r:id="rId4489"/>
-    <hyperlink ref="E1500" r:id="rId4490"/>
-    <hyperlink ref="B1501" r:id="rId4491"/>
-    <hyperlink ref="C1501" r:id="rId4492"/>
-    <hyperlink ref="E1501" r:id="rId4493"/>
-    <hyperlink ref="B1502" r:id="rId4494"/>
-    <hyperlink ref="C1502" r:id="rId4495"/>
-    <hyperlink ref="E1502" r:id="rId4496"/>
-    <hyperlink ref="B1503" r:id="rId4497"/>
-    <hyperlink ref="C1503" r:id="rId4498"/>
-    <hyperlink ref="E1503" r:id="rId4499"/>
-    <hyperlink ref="B1504" r:id="rId4500"/>
-    <hyperlink ref="C1504" r:id="rId4501"/>
-    <hyperlink ref="E1504" r:id="rId4502"/>
-    <hyperlink ref="B1505" r:id="rId4503"/>
-    <hyperlink ref="C1505" r:id="rId4504"/>
-    <hyperlink ref="E1505" r:id="rId4505"/>
-    <hyperlink ref="B1506" r:id="rId4506"/>
-    <hyperlink ref="C1506" r:id="rId4507"/>
-    <hyperlink ref="E1506" r:id="rId4508"/>
-    <hyperlink ref="B1507" r:id="rId4509"/>
-    <hyperlink ref="C1507" r:id="rId4510"/>
-    <hyperlink ref="E1507" r:id="rId4511"/>
-    <hyperlink ref="B1508" r:id="rId4512"/>
-    <hyperlink ref="C1508" r:id="rId4513"/>
-    <hyperlink ref="E1508" r:id="rId4514"/>
-    <hyperlink ref="B1509" r:id="rId4515"/>
-    <hyperlink ref="C1509" r:id="rId4516"/>
-    <hyperlink ref="E1509" r:id="rId4517"/>
-    <hyperlink ref="B1510" r:id="rId4518"/>
-    <hyperlink ref="C1510" r:id="rId4519"/>
-    <hyperlink ref="E1510" r:id="rId4520"/>
-    <hyperlink ref="B1511" r:id="rId4521"/>
-    <hyperlink ref="C1511" r:id="rId4522"/>
-    <hyperlink ref="E1511" r:id="rId4523"/>
-    <hyperlink ref="B1512" r:id="rId4524"/>
-    <hyperlink ref="C1512" r:id="rId4525"/>
-    <hyperlink ref="E1512" r:id="rId4526"/>
-    <hyperlink ref="B1513" r:id="rId4527"/>
-    <hyperlink ref="C1513" r:id="rId4528"/>
-    <hyperlink ref="E1513" r:id="rId4529"/>
-    <hyperlink ref="B1514" r:id="rId4530"/>
-    <hyperlink ref="C1514" r:id="rId4531"/>
-    <hyperlink ref="E1514" r:id="rId4532"/>
-    <hyperlink ref="B1515" r:id="rId4533"/>
-    <hyperlink ref="C1515" r:id="rId4534"/>
-    <hyperlink ref="E1515" r:id="rId4535"/>
-    <hyperlink ref="B1516" r:id="rId4536"/>
-    <hyperlink ref="C1516" r:id="rId4537"/>
-    <hyperlink ref="E1516" r:id="rId4538"/>
-    <hyperlink ref="B1517" r:id="rId4539"/>
-    <hyperlink ref="C1517" r:id="rId4540"/>
-    <hyperlink ref="E1517" r:id="rId4541"/>
-    <hyperlink ref="B1518" r:id="rId4542"/>
-    <hyperlink ref="C1518" r:id="rId4543"/>
-    <hyperlink ref="E1518" r:id="rId4544"/>
-    <hyperlink ref="B1519" r:id="rId4545"/>
-    <hyperlink ref="C1519" r:id="rId4546"/>
-    <hyperlink ref="E1519" r:id="rId4547"/>
-    <hyperlink ref="B1520" r:id="rId4548"/>
-    <hyperlink ref="C1520" r:id="rId4549"/>
-    <hyperlink ref="E1520" r:id="rId4550"/>
-    <hyperlink ref="B1521" r:id="rId4551"/>
-    <hyperlink ref="C1521" r:id="rId4552"/>
-    <hyperlink ref="E1521" r:id="rId4553"/>
-    <hyperlink ref="B1522" r:id="rId4554"/>
-    <hyperlink ref="C1522" r:id="rId4555"/>
-    <hyperlink ref="E1522" r:id="rId4556"/>
-    <hyperlink ref="B1523" r:id="rId4557"/>
-    <hyperlink ref="C1523" r:id="rId4558"/>
-    <hyperlink ref="E1523" r:id="rId4559"/>
-    <hyperlink ref="B1524" r:id="rId4560"/>
-    <hyperlink ref="C1524" r:id="rId4561"/>
-    <hyperlink ref="E1524" r:id="rId4562"/>
-    <hyperlink ref="B1525" r:id="rId4563"/>
-    <hyperlink ref="C1525" r:id="rId4564"/>
-    <hyperlink ref="E1525" r:id="rId4565"/>
-    <hyperlink ref="B1526" r:id="rId4566"/>
-    <hyperlink ref="C1526" r:id="rId4567"/>
-    <hyperlink ref="E1526" r:id="rId4568"/>
-    <hyperlink ref="B1527" r:id="rId4569"/>
-    <hyperlink ref="C1527" r:id="rId4570"/>
-    <hyperlink ref="E1527" r:id="rId4571"/>
-    <hyperlink ref="B1528" r:id="rId4572"/>
-    <hyperlink ref="C1528" r:id="rId4573"/>
-    <hyperlink ref="E1528" r:id="rId4574"/>
-    <hyperlink ref="B1529" r:id="rId4575"/>
-    <hyperlink ref="C1529" r:id="rId4576"/>
-    <hyperlink ref="E1529" r:id="rId4577"/>
-    <hyperlink ref="B1530" r:id="rId4578"/>
-    <hyperlink ref="C1530" r:id="rId4579"/>
-    <hyperlink ref="E1530" r:id="rId4580"/>
-    <hyperlink ref="B1531" r:id="rId4581"/>
-    <hyperlink ref="C1531" r:id="rId4582"/>
-    <hyperlink ref="E1531" r:id="rId4583"/>
-    <hyperlink ref="B1532" r:id="rId4584"/>
-    <hyperlink ref="C1532" r:id="rId4585"/>
-    <hyperlink ref="E1532" r:id="rId4586"/>
-    <hyperlink ref="B1533" r:id="rId4587"/>
-    <hyperlink ref="C1533" r:id="rId4588"/>
-    <hyperlink ref="E1533" r:id="rId4589"/>
-    <hyperlink ref="B1534" r:id="rId4590"/>
-    <hyperlink ref="C1534" r:id="rId4591"/>
-    <hyperlink ref="E1534" r:id="rId4592"/>
-    <hyperlink ref="B1535" r:id="rId4593"/>
-    <hyperlink ref="C1535" r:id="rId4594"/>
-    <hyperlink ref="E1535" r:id="rId4595"/>
-    <hyperlink ref="B1536" r:id="rId4596"/>
-    <hyperlink ref="C1536" r:id="rId4597"/>
-    <hyperlink ref="E1536" r:id="rId4598"/>
-    <hyperlink ref="B1537" r:id="rId4599"/>
-    <hyperlink ref="C1537" r:id="rId4600"/>
-    <hyperlink ref="E1537" r:id="rId4601"/>
-    <hyperlink ref="B1538" r:id="rId4602"/>
-    <hyperlink ref="C1538" r:id="rId4603"/>
-    <hyperlink ref="E1538" r:id="rId4604"/>
-    <hyperlink ref="B1539" r:id="rId4605"/>
-    <hyperlink ref="C1539" r:id="rId4606"/>
-    <hyperlink ref="E1539" r:id="rId4607"/>
-    <hyperlink ref="B1540" r:id="rId4608"/>
-    <hyperlink ref="C1540" r:id="rId4609"/>
-    <hyperlink ref="E1540" r:id="rId4610"/>
-    <hyperlink ref="B1541" r:id="rId4611"/>
-    <hyperlink ref="C1541" r:id="rId4612"/>
-    <hyperlink ref="E1541" r:id="rId4613"/>
-    <hyperlink ref="B1542" r:id="rId4614"/>
-    <hyperlink ref="C1542" r:id="rId4615"/>
-    <hyperlink ref="E1542" r:id="rId4616"/>
-    <hyperlink ref="B1543" r:id="rId4617"/>
-    <hyperlink ref="C1543" r:id="rId4618"/>
-    <hyperlink ref="E1543" r:id="rId4619"/>
-    <hyperlink ref="B1544" r:id="rId4620"/>
-    <hyperlink ref="C1544" r:id="rId4621"/>
-    <hyperlink ref="E1544" r:id="rId4622"/>
-    <hyperlink ref="B1545" r:id="rId4623"/>
-    <hyperlink ref="C1545" r:id="rId4624"/>
-    <hyperlink ref="E1545" r:id="rId4625"/>
-    <hyperlink ref="B1546" r:id="rId4626"/>
-    <hyperlink ref="C1546" r:id="rId4627"/>
-    <hyperlink ref="E1546" r:id="rId4628"/>
-    <hyperlink ref="B1547" r:id="rId4629"/>
-    <hyperlink ref="C1547" r:id="rId4630"/>
-    <hyperlink ref="E1547" r:id="rId4631"/>
-    <hyperlink ref="B1548" r:id="rId4632"/>
-    <hyperlink ref="C1548" r:id="rId4633"/>
-    <hyperlink ref="E1548" r:id="rId4634"/>
-    <hyperlink ref="B1549" r:id="rId4635"/>
-    <hyperlink ref="C1549" r:id="rId4636"/>
-    <hyperlink ref="E1549" r:id="rId4637"/>
-    <hyperlink ref="B1550" r:id="rId4638"/>
-    <hyperlink ref="C1550" r:id="rId4639"/>
-    <hyperlink ref="E1550" r:id="rId4640"/>
-    <hyperlink ref="B1551" r:id="rId4641"/>
-    <hyperlink ref="C1551" r:id="rId4642"/>
-    <hyperlink ref="E1551" r:id="rId4643"/>
-    <hyperlink ref="B1552" r:id="rId4644"/>
-    <hyperlink ref="C1552" r:id="rId4645"/>
-    <hyperlink ref="E1552" r:id="rId4646"/>
-    <hyperlink ref="B1553" r:id="rId4647"/>
-    <hyperlink ref="C1553" r:id="rId4648"/>
-    <hyperlink ref="E1553" r:id="rId4649"/>
-    <hyperlink ref="B1554" r:id="rId4650"/>
-    <hyperlink ref="C1554" r:id="rId4651"/>
-    <hyperlink ref="E1554" r:id="rId4652" location="pullrequestreview-184181318"/>
-    <hyperlink ref="B1555" r:id="rId4653"/>
-    <hyperlink ref="C1555" r:id="rId4654"/>
-    <hyperlink ref="E1555" r:id="rId4655"/>
-    <hyperlink ref="B1556" r:id="rId4656"/>
-    <hyperlink ref="C1556" r:id="rId4657"/>
-    <hyperlink ref="E1556" r:id="rId4658"/>
-    <hyperlink ref="B1557" r:id="rId4659"/>
-    <hyperlink ref="C1557" r:id="rId4660"/>
-    <hyperlink ref="E1557" r:id="rId4661"/>
-    <hyperlink ref="B1558" r:id="rId4662"/>
-    <hyperlink ref="C1558" r:id="rId4663"/>
-    <hyperlink ref="E1558" r:id="rId4664"/>
-    <hyperlink ref="B1559" r:id="rId4665"/>
-    <hyperlink ref="C1559" r:id="rId4666"/>
-    <hyperlink ref="E1559" r:id="rId4667"/>
-    <hyperlink ref="B1560" r:id="rId4668"/>
-    <hyperlink ref="C1560" r:id="rId4669"/>
-    <hyperlink ref="E1560" r:id="rId4670"/>
-    <hyperlink ref="B1561" r:id="rId4671"/>
-    <hyperlink ref="C1561" r:id="rId4672"/>
-    <hyperlink ref="E1561" r:id="rId4673"/>
-    <hyperlink ref="B1562" r:id="rId4674"/>
-    <hyperlink ref="C1562" r:id="rId4675"/>
-    <hyperlink ref="E1562" r:id="rId4676"/>
-    <hyperlink ref="B1563" r:id="rId4677"/>
-    <hyperlink ref="C1563" r:id="rId4678"/>
-    <hyperlink ref="E1563" r:id="rId4679"/>
-    <hyperlink ref="B1564" r:id="rId4680"/>
-    <hyperlink ref="C1564" r:id="rId4681"/>
-    <hyperlink ref="E1564" r:id="rId4682"/>
-    <hyperlink ref="B1565" r:id="rId4683"/>
-    <hyperlink ref="C1565" r:id="rId4684"/>
-    <hyperlink ref="E1565" r:id="rId4685"/>
-    <hyperlink ref="B1566" r:id="rId4686"/>
-    <hyperlink ref="C1566" r:id="rId4687"/>
-    <hyperlink ref="E1566" r:id="rId4688"/>
-    <hyperlink ref="B1567" r:id="rId4689"/>
-    <hyperlink ref="C1567" r:id="rId4690"/>
-    <hyperlink ref="E1567" r:id="rId4691"/>
-    <hyperlink ref="B1568" r:id="rId4692"/>
-    <hyperlink ref="C1568" r:id="rId4693"/>
-    <hyperlink ref="E1568" r:id="rId4694"/>
-    <hyperlink ref="B1569" r:id="rId4695"/>
-    <hyperlink ref="C1569" r:id="rId4696"/>
-    <hyperlink ref="E1569" r:id="rId4697"/>
-    <hyperlink ref="B1570" r:id="rId4698"/>
-    <hyperlink ref="C1570" r:id="rId4699"/>
-    <hyperlink ref="E1570" r:id="rId4700" location="event-2016722433"/>
-    <hyperlink ref="B1571" r:id="rId4701"/>
-    <hyperlink ref="C1571" r:id="rId4702"/>
-    <hyperlink ref="E1571" r:id="rId4703"/>
-    <hyperlink ref="B1572" r:id="rId4704"/>
-    <hyperlink ref="C1572" r:id="rId4705"/>
-    <hyperlink ref="E1572" r:id="rId4706"/>
-    <hyperlink ref="B1573" r:id="rId4707"/>
-    <hyperlink ref="C1573" r:id="rId4708"/>
-    <hyperlink ref="E1573" r:id="rId4709"/>
-    <hyperlink ref="B1574" r:id="rId4710"/>
-    <hyperlink ref="C1574" r:id="rId4711"/>
-    <hyperlink ref="E1574" r:id="rId4712"/>
-    <hyperlink ref="B1575" r:id="rId4713"/>
-    <hyperlink ref="C1575" r:id="rId4714"/>
-    <hyperlink ref="E1575" r:id="rId4715"/>
-    <hyperlink ref="B1576" r:id="rId4716"/>
-    <hyperlink ref="C1576" r:id="rId4717"/>
-    <hyperlink ref="E1576" r:id="rId4718"/>
-    <hyperlink ref="B1577" r:id="rId4719"/>
-    <hyperlink ref="C1577" r:id="rId4720"/>
-    <hyperlink ref="E1577" r:id="rId4721"/>
-    <hyperlink ref="B1578" r:id="rId4722"/>
-    <hyperlink ref="C1578" r:id="rId4723"/>
-    <hyperlink ref="E1578" r:id="rId4724"/>
-    <hyperlink ref="B1579" r:id="rId4725"/>
-    <hyperlink ref="C1579" r:id="rId4726"/>
-    <hyperlink ref="E1579" r:id="rId4727"/>
-    <hyperlink ref="B1580" r:id="rId4728"/>
-    <hyperlink ref="C1580" r:id="rId4729"/>
-    <hyperlink ref="E1580" r:id="rId4730"/>
-    <hyperlink ref="B1581" r:id="rId4731"/>
-    <hyperlink ref="C1581" r:id="rId4732"/>
-    <hyperlink ref="E1581" r:id="rId4733"/>
-    <hyperlink ref="B1582" r:id="rId4734"/>
-    <hyperlink ref="C1582" r:id="rId4735"/>
-    <hyperlink ref="E1582" r:id="rId4736"/>
-    <hyperlink ref="B1583" r:id="rId4737"/>
-    <hyperlink ref="C1583" r:id="rId4738"/>
-    <hyperlink ref="E1583" r:id="rId4739"/>
-    <hyperlink ref="B1584" r:id="rId4740"/>
-    <hyperlink ref="C1584" r:id="rId4741"/>
-    <hyperlink ref="E1584" r:id="rId4742"/>
-    <hyperlink ref="B1585" r:id="rId4743"/>
-    <hyperlink ref="C1585" r:id="rId4744"/>
-    <hyperlink ref="E1585" r:id="rId4745"/>
-    <hyperlink ref="B1586" r:id="rId4746"/>
-    <hyperlink ref="C1586" r:id="rId4747"/>
-    <hyperlink ref="E1586" r:id="rId4748"/>
-    <hyperlink ref="B1587" r:id="rId4749"/>
-    <hyperlink ref="C1587" r:id="rId4750"/>
-    <hyperlink ref="E1587" r:id="rId4751"/>
-    <hyperlink ref="B1588" r:id="rId4752"/>
-    <hyperlink ref="C1588" r:id="rId4753"/>
-    <hyperlink ref="E1588" r:id="rId4754"/>
-    <hyperlink ref="B1589" r:id="rId4755"/>
-    <hyperlink ref="C1589" r:id="rId4756"/>
-    <hyperlink ref="E1589" r:id="rId4757"/>
-    <hyperlink ref="B1590" r:id="rId4758"/>
-    <hyperlink ref="C1590" r:id="rId4759"/>
-    <hyperlink ref="E1590" r:id="rId4760"/>
-    <hyperlink ref="B1591" r:id="rId4761"/>
-    <hyperlink ref="C1591" r:id="rId4762"/>
-    <hyperlink ref="E1591" r:id="rId4763"/>
-    <hyperlink ref="B1592" r:id="rId4764"/>
-    <hyperlink ref="C1592" r:id="rId4765"/>
-    <hyperlink ref="E1592" r:id="rId4766"/>
-    <hyperlink ref="B1593" r:id="rId4767"/>
-    <hyperlink ref="C1593" r:id="rId4768"/>
-    <hyperlink ref="E1593" r:id="rId4769"/>
-    <hyperlink ref="B1594" r:id="rId4770"/>
-    <hyperlink ref="C1594" r:id="rId4771"/>
-    <hyperlink ref="E1594" r:id="rId4772"/>
-    <hyperlink ref="B1595" r:id="rId4773"/>
-    <hyperlink ref="C1595" r:id="rId4774"/>
-    <hyperlink ref="E1595" r:id="rId4775"/>
-    <hyperlink ref="B1596" r:id="rId4776"/>
-    <hyperlink ref="C1596" r:id="rId4777"/>
-    <hyperlink ref="E1596" r:id="rId4778"/>
-    <hyperlink ref="B1597" r:id="rId4779"/>
-    <hyperlink ref="C1597" r:id="rId4780"/>
-    <hyperlink ref="E1597" r:id="rId4781"/>
-    <hyperlink ref="B1598" r:id="rId4782"/>
-    <hyperlink ref="C1598" r:id="rId4783"/>
-    <hyperlink ref="E1598" r:id="rId4784"/>
-    <hyperlink ref="B1599" r:id="rId4785"/>
-    <hyperlink ref="C1599" r:id="rId4786"/>
-    <hyperlink ref="E1599" r:id="rId4787"/>
-    <hyperlink ref="B1600" r:id="rId4788"/>
-    <hyperlink ref="C1600" r:id="rId4789"/>
-    <hyperlink ref="E1600" r:id="rId4790"/>
-    <hyperlink ref="B1601" r:id="rId4791"/>
-    <hyperlink ref="C1601" r:id="rId4792"/>
-    <hyperlink ref="E1601" r:id="rId4793"/>
-    <hyperlink ref="B1602" r:id="rId4794"/>
-    <hyperlink ref="C1602" r:id="rId4795"/>
-    <hyperlink ref="E1602" r:id="rId4796"/>
-    <hyperlink ref="B1603" r:id="rId4797"/>
-    <hyperlink ref="C1603" r:id="rId4798"/>
-    <hyperlink ref="E1603" r:id="rId4799"/>
-    <hyperlink ref="B1604" r:id="rId4800"/>
-    <hyperlink ref="C1604" r:id="rId4801"/>
-    <hyperlink ref="E1604" r:id="rId4802"/>
-    <hyperlink ref="B1605" r:id="rId4803"/>
-    <hyperlink ref="C1605" r:id="rId4804"/>
-    <hyperlink ref="E1605" r:id="rId4805"/>
-    <hyperlink ref="B1606" r:id="rId4806"/>
-    <hyperlink ref="C1606" r:id="rId4807"/>
-    <hyperlink ref="E1606" r:id="rId4808"/>
-    <hyperlink ref="B1607" r:id="rId4809"/>
-    <hyperlink ref="C1607" r:id="rId4810"/>
-    <hyperlink ref="E1607" r:id="rId4811"/>
-    <hyperlink ref="B1608" r:id="rId4812"/>
-    <hyperlink ref="C1608" r:id="rId4813"/>
-    <hyperlink ref="E1608" r:id="rId4814"/>
-    <hyperlink ref="B1609" r:id="rId4815"/>
-    <hyperlink ref="C1609" r:id="rId4816"/>
-    <hyperlink ref="E1609" r:id="rId4817"/>
-    <hyperlink ref="B1610" r:id="rId4818"/>
-    <hyperlink ref="C1610" r:id="rId4819"/>
-    <hyperlink ref="E1610" r:id="rId4820"/>
-    <hyperlink ref="B1611" r:id="rId4821"/>
-    <hyperlink ref="C1611" r:id="rId4822"/>
-    <hyperlink ref="E1611" r:id="rId4823"/>
-    <hyperlink ref="B1612" r:id="rId4824"/>
-    <hyperlink ref="C1612" r:id="rId4825"/>
-    <hyperlink ref="E1612" r:id="rId4826"/>
-    <hyperlink ref="B1613" r:id="rId4827"/>
-    <hyperlink ref="C1613" r:id="rId4828"/>
-    <hyperlink ref="E1613" r:id="rId4829"/>
-    <hyperlink ref="B1614" r:id="rId4830"/>
-    <hyperlink ref="C1614" r:id="rId4831"/>
-    <hyperlink ref="E1614" r:id="rId4832"/>
-    <hyperlink ref="B1615" r:id="rId4833"/>
-    <hyperlink ref="C1615" r:id="rId4834"/>
-    <hyperlink ref="E1615" r:id="rId4835" location="gid=0"/>
-    <hyperlink ref="B1616" r:id="rId4836"/>
-    <hyperlink ref="C1616" r:id="rId4837"/>
-    <hyperlink ref="E1616" r:id="rId4838" location="gid=0"/>
-    <hyperlink ref="B1617" r:id="rId4839"/>
-    <hyperlink ref="C1617" r:id="rId4840"/>
-    <hyperlink ref="E1617" r:id="rId4841" location="gid=0"/>
-    <hyperlink ref="B1618" r:id="rId4842"/>
-    <hyperlink ref="C1618" r:id="rId4843"/>
-    <hyperlink ref="E1618" r:id="rId4844" location="gid=0"/>
-    <hyperlink ref="B1619" r:id="rId4845"/>
-    <hyperlink ref="C1619" r:id="rId4846"/>
-    <hyperlink ref="E1619" r:id="rId4847"/>
-    <hyperlink ref="B1620" r:id="rId4848"/>
-    <hyperlink ref="C1620" r:id="rId4849"/>
-    <hyperlink ref="E1620" r:id="rId4850" location="gid=0"/>
-    <hyperlink ref="B1621" r:id="rId4851"/>
-    <hyperlink ref="C1621" r:id="rId4852"/>
-    <hyperlink ref="E1621" r:id="rId4853" location="gid=0"/>
-    <hyperlink ref="B1622" r:id="rId4854"/>
-    <hyperlink ref="C1622" r:id="rId4855"/>
-    <hyperlink ref="E1622" r:id="rId4856" location="gid=0"/>
-    <hyperlink ref="B1623" r:id="rId4857"/>
-    <hyperlink ref="C1623" r:id="rId4858"/>
-    <hyperlink ref="E1623" r:id="rId4859" location="gid=0"/>
-    <hyperlink ref="B1624" r:id="rId4860"/>
-    <hyperlink ref="C1624" r:id="rId4861"/>
-    <hyperlink ref="E1624" r:id="rId4862" location="gid=0"/>
-    <hyperlink ref="B1625" r:id="rId4863"/>
-    <hyperlink ref="C1625" r:id="rId4864"/>
-    <hyperlink ref="E1625" r:id="rId4865" location="gid=0"/>
-    <hyperlink ref="B1626" r:id="rId4866"/>
-    <hyperlink ref="C1626" r:id="rId4867"/>
-    <hyperlink ref="E1626" r:id="rId4868"/>
-    <hyperlink ref="B1627" r:id="rId4869"/>
-    <hyperlink ref="C1627" r:id="rId4870"/>
-    <hyperlink ref="E1627" r:id="rId4871"/>
-    <hyperlink ref="B1628" r:id="rId4872"/>
-    <hyperlink ref="C1628" r:id="rId4873"/>
-    <hyperlink ref="E1628" r:id="rId4874"/>
-    <hyperlink ref="B1629" r:id="rId4875"/>
-    <hyperlink ref="C1629" r:id="rId4876"/>
-    <hyperlink ref="E1629" r:id="rId4877"/>
-    <hyperlink ref="B1630" r:id="rId4878"/>
-    <hyperlink ref="C1630" r:id="rId4879"/>
-    <hyperlink ref="E1630" r:id="rId4880"/>
-    <hyperlink ref="B1631" r:id="rId4881"/>
-    <hyperlink ref="C1631" r:id="rId4882"/>
-    <hyperlink ref="E1631" r:id="rId4883"/>
-    <hyperlink ref="B1632" r:id="rId4884"/>
-    <hyperlink ref="C1632" r:id="rId4885"/>
-    <hyperlink ref="E1632" r:id="rId4886"/>
-    <hyperlink ref="B1633" r:id="rId4887"/>
-    <hyperlink ref="C1633" r:id="rId4888"/>
-    <hyperlink ref="E1633" r:id="rId4889"/>
-    <hyperlink ref="B1634" r:id="rId4890"/>
-    <hyperlink ref="C1634" r:id="rId4891"/>
-    <hyperlink ref="E1634" r:id="rId4892"/>
-    <hyperlink ref="B1635" r:id="rId4893"/>
-    <hyperlink ref="C1635" r:id="rId4894"/>
-    <hyperlink ref="E1635" r:id="rId4895"/>
-    <hyperlink ref="B1636" r:id="rId4896"/>
-    <hyperlink ref="C1636" r:id="rId4897"/>
-    <hyperlink ref="E1636" r:id="rId4898"/>
-    <hyperlink ref="B1637" r:id="rId4899"/>
-    <hyperlink ref="C1637" r:id="rId4900"/>
-    <hyperlink ref="E1637" r:id="rId4901"/>
-    <hyperlink ref="B1638" r:id="rId4902"/>
-    <hyperlink ref="C1638" r:id="rId4903"/>
-    <hyperlink ref="E1638" r:id="rId4904"/>
-    <hyperlink ref="B1639" r:id="rId4905"/>
-    <hyperlink ref="C1639" r:id="rId4906"/>
-    <hyperlink ref="E1639" r:id="rId4907"/>
-    <hyperlink ref="B1640" r:id="rId4908"/>
-    <hyperlink ref="C1640" r:id="rId4909"/>
-    <hyperlink ref="E1640" r:id="rId4910"/>
-    <hyperlink ref="B1641" r:id="rId4911"/>
-    <hyperlink ref="C1641" r:id="rId4912"/>
-    <hyperlink ref="E1641" r:id="rId4913"/>
-    <hyperlink ref="B1642" r:id="rId4914"/>
-    <hyperlink ref="C1642" r:id="rId4915"/>
-    <hyperlink ref="E1642" r:id="rId4916"/>
-    <hyperlink ref="B1643" r:id="rId4917"/>
-    <hyperlink ref="C1643" r:id="rId4918"/>
-    <hyperlink ref="E1643" r:id="rId4919"/>
-    <hyperlink ref="B1644" r:id="rId4920"/>
-    <hyperlink ref="C1644" r:id="rId4921"/>
-    <hyperlink ref="E1644" r:id="rId4922"/>
-    <hyperlink ref="B1645" r:id="rId4923"/>
-    <hyperlink ref="C1645" r:id="rId4924"/>
-    <hyperlink ref="E1645" r:id="rId4925"/>
-    <hyperlink ref="B1646" r:id="rId4926"/>
-    <hyperlink ref="C1646" r:id="rId4927"/>
-    <hyperlink ref="E1646" r:id="rId4928"/>
-    <hyperlink ref="B1647" r:id="rId4929"/>
-    <hyperlink ref="C1647" r:id="rId4930"/>
-    <hyperlink ref="E1647" r:id="rId4931"/>
-    <hyperlink ref="B1648" r:id="rId4932"/>
-    <hyperlink ref="C1648" r:id="rId4933"/>
-    <hyperlink ref="E1648" r:id="rId4934"/>
-    <hyperlink ref="B1649" r:id="rId4935"/>
-    <hyperlink ref="C1649" r:id="rId4936"/>
-    <hyperlink ref="E1649" r:id="rId4937"/>
-    <hyperlink ref="B1650" r:id="rId4938"/>
-    <hyperlink ref="C1650" r:id="rId4939"/>
-    <hyperlink ref="E1650" r:id="rId4940"/>
-    <hyperlink ref="B1651" r:id="rId4941"/>
-    <hyperlink ref="C1651" r:id="rId4942"/>
-    <hyperlink ref="E1651" r:id="rId4943"/>
-    <hyperlink ref="B1652" r:id="rId4944"/>
-    <hyperlink ref="C1652" r:id="rId4945"/>
-    <hyperlink ref="E1652" r:id="rId4946"/>
-    <hyperlink ref="B1653" r:id="rId4947"/>
-    <hyperlink ref="C1653" r:id="rId4948"/>
-    <hyperlink ref="E1653" r:id="rId4949"/>
-    <hyperlink ref="B1654" r:id="rId4950"/>
-    <hyperlink ref="C1654" r:id="rId4951"/>
-    <hyperlink ref="E1654" r:id="rId4952"/>
-    <hyperlink ref="B1655" r:id="rId4953"/>
-    <hyperlink ref="C1655" r:id="rId4954"/>
-    <hyperlink ref="E1655" r:id="rId4955"/>
-    <hyperlink ref="B1656" r:id="rId4956"/>
-    <hyperlink ref="C1656" r:id="rId4957"/>
-    <hyperlink ref="E1656" r:id="rId4958"/>
-    <hyperlink ref="B1657" r:id="rId4959"/>
-    <hyperlink ref="C1657" r:id="rId4960"/>
-    <hyperlink ref="E1657" r:id="rId4961"/>
-    <hyperlink ref="B1658" r:id="rId4962"/>
-    <hyperlink ref="C1658" r:id="rId4963"/>
-    <hyperlink ref="E1658" r:id="rId4964"/>
-    <hyperlink ref="B1659" r:id="rId4965"/>
-    <hyperlink ref="C1659" r:id="rId4966"/>
-    <hyperlink ref="E1659" r:id="rId4967"/>
-    <hyperlink ref="B1660" r:id="rId4968"/>
-    <hyperlink ref="C1660" r:id="rId4969"/>
-    <hyperlink ref="E1660" r:id="rId4970"/>
-    <hyperlink ref="B1661" r:id="rId4971"/>
-    <hyperlink ref="C1661" r:id="rId4972"/>
-    <hyperlink ref="E1661" r:id="rId4973"/>
-    <hyperlink ref="B1662" r:id="rId4974"/>
-    <hyperlink ref="C1662" r:id="rId4975"/>
-    <hyperlink ref="E1662" r:id="rId4976"/>
-    <hyperlink ref="B1663" r:id="rId4977"/>
-    <hyperlink ref="C1663" r:id="rId4978"/>
-    <hyperlink ref="E1663" r:id="rId4979"/>
-    <hyperlink ref="B1664" r:id="rId4980"/>
-    <hyperlink ref="C1664" r:id="rId4981"/>
-    <hyperlink ref="E1664" r:id="rId4982"/>
-    <hyperlink ref="B1665" r:id="rId4983"/>
-    <hyperlink ref="C1665" r:id="rId4984"/>
-    <hyperlink ref="E1665" r:id="rId4985"/>
-    <hyperlink ref="B1666" r:id="rId4986"/>
-    <hyperlink ref="C1666" r:id="rId4987"/>
-    <hyperlink ref="E1666" r:id="rId4988"/>
-    <hyperlink ref="B1667" r:id="rId4989"/>
-    <hyperlink ref="C1667" r:id="rId4990"/>
-    <hyperlink ref="E1667" r:id="rId4991"/>
-    <hyperlink ref="B1668" r:id="rId4992"/>
-    <hyperlink ref="C1668" r:id="rId4993"/>
-    <hyperlink ref="E1668" r:id="rId4994"/>
-    <hyperlink ref="B1669" r:id="rId4995"/>
-    <hyperlink ref="C1669" r:id="rId4996"/>
-    <hyperlink ref="E1669" r:id="rId4997"/>
-    <hyperlink ref="B1670" r:id="rId4998"/>
-    <hyperlink ref="C1670" r:id="rId4999"/>
-    <hyperlink ref="E1670" r:id="rId5000"/>
-    <hyperlink ref="B1671" r:id="rId5001"/>
-    <hyperlink ref="C1671" r:id="rId5002"/>
-    <hyperlink ref="E1671" r:id="rId5003"/>
-    <hyperlink ref="B1672" r:id="rId5004"/>
-    <hyperlink ref="C1672" r:id="rId5005"/>
-    <hyperlink ref="E1672" r:id="rId5006"/>
-    <hyperlink ref="B1673" r:id="rId5007"/>
-    <hyperlink ref="C1673" r:id="rId5008"/>
-    <hyperlink ref="E1673" r:id="rId5009"/>
-    <hyperlink ref="B1674" r:id="rId5010"/>
-    <hyperlink ref="C1674" r:id="rId5011"/>
-    <hyperlink ref="E1674" r:id="rId5012"/>
-    <hyperlink ref="B1675" r:id="rId5013"/>
-    <hyperlink ref="C1675" r:id="rId5014"/>
-    <hyperlink ref="E1675" r:id="rId5015"/>
-    <hyperlink ref="B1676" r:id="rId5016"/>
-    <hyperlink ref="C1676" r:id="rId5017"/>
-    <hyperlink ref="E1676" r:id="rId5018"/>
-    <hyperlink ref="B1677" r:id="rId5019"/>
-    <hyperlink ref="C1677" r:id="rId5020"/>
-    <hyperlink ref="E1677" r:id="rId5021"/>
-    <hyperlink ref="B1678" r:id="rId5022"/>
-    <hyperlink ref="C1678" r:id="rId5023"/>
-    <hyperlink ref="E1678" r:id="rId5024"/>
-    <hyperlink ref="B1679" r:id="rId5025"/>
-    <hyperlink ref="C1679" r:id="rId5026"/>
-    <hyperlink ref="E1679" r:id="rId5027"/>
-    <hyperlink ref="B1680" r:id="rId5028"/>
-    <hyperlink ref="C1680" r:id="rId5029"/>
-    <hyperlink ref="E1680" r:id="rId5030"/>
-    <hyperlink ref="B1681" r:id="rId5031"/>
-    <hyperlink ref="C1681" r:id="rId5032"/>
-    <hyperlink ref="E1681" r:id="rId5033"/>
-    <hyperlink ref="B1682" r:id="rId5034"/>
-    <hyperlink ref="C1682" r:id="rId5035"/>
-    <hyperlink ref="E1682" r:id="rId5036"/>
-    <hyperlink ref="B1683" r:id="rId5037"/>
-    <hyperlink ref="C1683" r:id="rId5038"/>
-    <hyperlink ref="E1683" r:id="rId5039"/>
-    <hyperlink ref="B1684" r:id="rId5040"/>
-    <hyperlink ref="C1684" r:id="rId5041"/>
-    <hyperlink ref="E1684" r:id="rId5042"/>
-    <hyperlink ref="B1685" r:id="rId5043"/>
-    <hyperlink ref="C1685" r:id="rId5044"/>
-    <hyperlink ref="E1685" r:id="rId5045"/>
-    <hyperlink ref="B1686" r:id="rId5046"/>
-    <hyperlink ref="C1686" r:id="rId5047"/>
-    <hyperlink ref="E1686" r:id="rId5048"/>
-    <hyperlink ref="B1687" r:id="rId5049"/>
-    <hyperlink ref="C1687" r:id="rId5050"/>
-    <hyperlink ref="E1687" r:id="rId5051"/>
-    <hyperlink ref="B1688" r:id="rId5052"/>
-    <hyperlink ref="C1688" r:id="rId5053"/>
-    <hyperlink ref="E1688" r:id="rId5054"/>
-    <hyperlink ref="B1689" r:id="rId5055"/>
-    <hyperlink ref="C1689" r:id="rId5056"/>
-    <hyperlink ref="E1689" r:id="rId5057"/>
-    <hyperlink ref="B1690" r:id="rId5058"/>
-    <hyperlink ref="C1690" r:id="rId5059"/>
-    <hyperlink ref="E1690" r:id="rId5060"/>
-    <hyperlink ref="B1691" r:id="rId5061"/>
-    <hyperlink ref="C1691" r:id="rId5062"/>
-    <hyperlink ref="E1691" r:id="rId5063"/>
-    <hyperlink ref="B1692" r:id="rId5064"/>
-    <hyperlink ref="C1692" r:id="rId5065"/>
-    <hyperlink ref="E1692" r:id="rId5066"/>
-    <hyperlink ref="B1693" r:id="rId5067"/>
-    <hyperlink ref="C1693" r:id="rId5068"/>
-    <hyperlink ref="E1693" r:id="rId5069"/>
-    <hyperlink ref="B1694" r:id="rId5070"/>
-    <hyperlink ref="C1694" r:id="rId5071"/>
-    <hyperlink ref="E1694" r:id="rId5072"/>
-    <hyperlink ref="B1695" r:id="rId5073"/>
-    <hyperlink ref="C1695" r:id="rId5074"/>
-    <hyperlink ref="E1695" r:id="rId5075"/>
-    <hyperlink ref="B1696" r:id="rId5076"/>
-    <hyperlink ref="C1696" r:id="rId5077"/>
-    <hyperlink ref="E1696" r:id="rId5078"/>
-    <hyperlink ref="B1697" r:id="rId5079"/>
-    <hyperlink ref="C1697" r:id="rId5080"/>
-    <hyperlink ref="E1697" r:id="rId5081"/>
-    <hyperlink ref="B1698" r:id="rId5082"/>
-    <hyperlink ref="C1698" r:id="rId5083"/>
-    <hyperlink ref="E1698" r:id="rId5084"/>
-    <hyperlink ref="B1699" r:id="rId5085"/>
-    <hyperlink ref="C1699" r:id="rId5086"/>
-    <hyperlink ref="E1699" r:id="rId5087"/>
-    <hyperlink ref="B1700" r:id="rId5088"/>
-    <hyperlink ref="C1700" r:id="rId5089"/>
-    <hyperlink ref="E1700" r:id="rId5090"/>
-    <hyperlink ref="B1701" r:id="rId5091"/>
-    <hyperlink ref="C1701" r:id="rId5092"/>
-    <hyperlink ref="E1701" r:id="rId5093"/>
-    <hyperlink ref="B1702" r:id="rId5094"/>
-    <hyperlink ref="C1702" r:id="rId5095"/>
-    <hyperlink ref="E1702" r:id="rId5096"/>
-    <hyperlink ref="B1703" r:id="rId5097"/>
-    <hyperlink ref="C1703" r:id="rId5098"/>
-    <hyperlink ref="E1703" r:id="rId5099"/>
-    <hyperlink ref="B1704" r:id="rId5100"/>
-    <hyperlink ref="C1704" r:id="rId5101"/>
-    <hyperlink ref="E1704" r:id="rId5102"/>
-    <hyperlink ref="B1705" r:id="rId5103"/>
-    <hyperlink ref="C1705" r:id="rId5104"/>
-    <hyperlink ref="E1705" r:id="rId5105"/>
-    <hyperlink ref="B1706" r:id="rId5106"/>
-    <hyperlink ref="C1706" r:id="rId5107"/>
-    <hyperlink ref="E1706" r:id="rId5108"/>
-    <hyperlink ref="B1707" r:id="rId5109"/>
-    <hyperlink ref="C1707" r:id="rId5110"/>
-    <hyperlink ref="E1707" r:id="rId5111"/>
-    <hyperlink ref="B1708" r:id="rId5112"/>
-    <hyperlink ref="C1708" r:id="rId5113"/>
-    <hyperlink ref="E1708" r:id="rId5114"/>
-    <hyperlink ref="B1709" r:id="rId5115"/>
-    <hyperlink ref="C1709" r:id="rId5116"/>
-    <hyperlink ref="E1709" r:id="rId5117"/>
-    <hyperlink ref="B1710" r:id="rId5118"/>
-    <hyperlink ref="C1710" r:id="rId5119"/>
-    <hyperlink ref="E1710" r:id="rId5120"/>
-    <hyperlink ref="B1711" r:id="rId5121"/>
-    <hyperlink ref="C1711" r:id="rId5122"/>
-    <hyperlink ref="E1711" r:id="rId5123"/>
-    <hyperlink ref="B1712" r:id="rId5124"/>
-    <hyperlink ref="C1712" r:id="rId5125"/>
-    <hyperlink ref="E1712" r:id="rId5126"/>
-    <hyperlink ref="B1713" r:id="rId5127"/>
-    <hyperlink ref="C1713" r:id="rId5128"/>
-    <hyperlink ref="E1713" r:id="rId5129"/>
-    <hyperlink ref="B1714" r:id="rId5130"/>
-    <hyperlink ref="C1714" r:id="rId5131"/>
-    <hyperlink ref="E1714" r:id="rId5132"/>
-    <hyperlink ref="B1715" r:id="rId5133"/>
-    <hyperlink ref="C1715" r:id="rId5134"/>
-    <hyperlink ref="E1715" r:id="rId5135"/>
-    <hyperlink ref="B1716" r:id="rId5136"/>
-    <hyperlink ref="C1716" r:id="rId5137"/>
-    <hyperlink ref="E1716" r:id="rId5138"/>
-    <hyperlink ref="B1717" r:id="rId5139"/>
-    <hyperlink ref="C1717" r:id="rId5140"/>
-    <hyperlink ref="E1717" r:id="rId5141"/>
-    <hyperlink ref="B1718" r:id="rId5142"/>
-    <hyperlink ref="C1718" r:id="rId5143"/>
-    <hyperlink ref="E1718" r:id="rId5144"/>
-    <hyperlink ref="B1719" r:id="rId5145"/>
-    <hyperlink ref="C1719" r:id="rId5146"/>
-    <hyperlink ref="E1719" r:id="rId5147"/>
-    <hyperlink ref="B1720" r:id="rId5148"/>
-    <hyperlink ref="C1720" r:id="rId5149"/>
-    <hyperlink ref="E1720" r:id="rId5150"/>
-    <hyperlink ref="B1721" r:id="rId5151"/>
-    <hyperlink ref="C1721" r:id="rId5152"/>
-    <hyperlink ref="E1721" r:id="rId5153"/>
-    <hyperlink ref="B1722" r:id="rId5154"/>
-    <hyperlink ref="C1722" r:id="rId5155"/>
-    <hyperlink ref="E1722" r:id="rId5156"/>
-    <hyperlink ref="B1723" r:id="rId5157"/>
-    <hyperlink ref="C1723" r:id="rId5158"/>
-    <hyperlink ref="E1723" r:id="rId5159"/>
-    <hyperlink ref="B1724" r:id="rId5160"/>
-    <hyperlink ref="C1724" r:id="rId5161"/>
-    <hyperlink ref="E1724" r:id="rId5162"/>
-    <hyperlink ref="B1725" r:id="rId5163"/>
-    <hyperlink ref="C1725" r:id="rId5164"/>
-    <hyperlink ref="E1725" r:id="rId5165"/>
-    <hyperlink ref="B1726" r:id="rId5166"/>
-    <hyperlink ref="C1726" r:id="rId5167"/>
-    <hyperlink ref="E1726" r:id="rId5168"/>
-    <hyperlink ref="B1727" r:id="rId5169"/>
-    <hyperlink ref="C1727" r:id="rId5170"/>
-    <hyperlink ref="E1727" r:id="rId5171"/>
-    <hyperlink ref="B1728" r:id="rId5172"/>
-    <hyperlink ref="C1728" r:id="rId5173"/>
-    <hyperlink ref="E1728" r:id="rId5174"/>
-    <hyperlink ref="B1729" r:id="rId5175"/>
-    <hyperlink ref="C1729" r:id="rId5176"/>
-    <hyperlink ref="E1729" r:id="rId5177"/>
-    <hyperlink ref="B1730" r:id="rId5178"/>
-    <hyperlink ref="C1730" r:id="rId5179"/>
-    <hyperlink ref="E1730" r:id="rId5180"/>
-    <hyperlink ref="B1731" r:id="rId5181"/>
-    <hyperlink ref="C1731" r:id="rId5182"/>
-    <hyperlink ref="E1731" r:id="rId5183"/>
-    <hyperlink ref="B1732" r:id="rId5184"/>
-    <hyperlink ref="C1732" r:id="rId5185"/>
-    <hyperlink ref="E1732" r:id="rId5186"/>
-    <hyperlink ref="B1733" r:id="rId5187"/>
-    <hyperlink ref="C1733" r:id="rId5188"/>
-    <hyperlink ref="E1733" r:id="rId5189"/>
-    <hyperlink ref="B1734" r:id="rId5190"/>
-    <hyperlink ref="C1734" r:id="rId5191"/>
-    <hyperlink ref="E1734" r:id="rId5192"/>
-    <hyperlink ref="B1735" r:id="rId5193"/>
-    <hyperlink ref="C1735" r:id="rId5194"/>
-    <hyperlink ref="E1735" r:id="rId5195"/>
-    <hyperlink ref="B1736" r:id="rId5196"/>
-    <hyperlink ref="C1736" r:id="rId5197"/>
-    <hyperlink ref="E1736" r:id="rId5198"/>
-    <hyperlink ref="B1737" r:id="rId5199"/>
-    <hyperlink ref="C1737" r:id="rId5200"/>
-    <hyperlink ref="E1737" r:id="rId5201"/>
-    <hyperlink ref="B1738" r:id="rId5202"/>
-    <hyperlink ref="C1738" r:id="rId5203"/>
-    <hyperlink ref="E1738" r:id="rId5204"/>
-    <hyperlink ref="B1739" r:id="rId5205"/>
-    <hyperlink ref="C1739" r:id="rId5206"/>
-    <hyperlink ref="E1739" r:id="rId5207"/>
-    <hyperlink ref="B1740" r:id="rId5208"/>
-    <hyperlink ref="C1740" r:id="rId5209"/>
-    <hyperlink ref="E1740" r:id="rId5210"/>
-    <hyperlink ref="B1741" r:id="rId5211"/>
-    <hyperlink ref="C1741" r:id="rId5212"/>
-    <hyperlink ref="E1741" r:id="rId5213"/>
-    <hyperlink ref="B1742" r:id="rId5214"/>
-    <hyperlink ref="C1742" r:id="rId5215"/>
-    <hyperlink ref="E1742" r:id="rId5216"/>
-    <hyperlink ref="B1743" r:id="rId5217"/>
-    <hyperlink ref="C1743" r:id="rId5218"/>
-    <hyperlink ref="E1743" r:id="rId5219"/>
-    <hyperlink ref="B1744" r:id="rId5220"/>
-    <hyperlink ref="C1744" r:id="rId5221"/>
-    <hyperlink ref="E1744" r:id="rId5222"/>
-    <hyperlink ref="B1745" r:id="rId5223"/>
-    <hyperlink ref="C1745" r:id="rId5224"/>
-    <hyperlink ref="E1745" r:id="rId5225"/>
-    <hyperlink ref="B1746" r:id="rId5226"/>
-    <hyperlink ref="C1746" r:id="rId5227"/>
-    <hyperlink ref="E1746" r:id="rId5228"/>
-    <hyperlink ref="B1747" r:id="rId5229"/>
-    <hyperlink ref="C1747" r:id="rId5230"/>
-    <hyperlink ref="E1747" r:id="rId5231"/>
-    <hyperlink ref="B1748" r:id="rId5232"/>
-    <hyperlink ref="C1748" r:id="rId5233"/>
-    <hyperlink ref="E1748" r:id="rId5234"/>
-    <hyperlink ref="B1749" r:id="rId5235"/>
-    <hyperlink ref="C1749" r:id="rId5236"/>
-    <hyperlink ref="E1749" r:id="rId5237"/>
-    <hyperlink ref="B1750" r:id="rId5238"/>
-    <hyperlink ref="C1750" r:id="rId5239"/>
-    <hyperlink ref="E1750" r:id="rId5240"/>
-    <hyperlink ref="B1751" r:id="rId5241"/>
-    <hyperlink ref="C1751" r:id="rId5242"/>
-    <hyperlink ref="E1751" r:id="rId5243"/>
-    <hyperlink ref="B1752" r:id="rId5244"/>
-    <hyperlink ref="C1752" r:id="rId5245"/>
-    <hyperlink ref="E1752" r:id="rId5246"/>
-    <hyperlink ref="B1753" r:id="rId5247"/>
-    <hyperlink ref="C1753" r:id="rId5248"/>
-    <hyperlink ref="E1753" r:id="rId5249"/>
-    <hyperlink ref="B1754" r:id="rId5250"/>
-    <hyperlink ref="C1754" r:id="rId5251"/>
-    <hyperlink ref="E1754" r:id="rId5252"/>
-    <hyperlink ref="B1755" r:id="rId5253"/>
-    <hyperlink ref="C1755" r:id="rId5254"/>
-    <hyperlink ref="E1755" r:id="rId5255"/>
-    <hyperlink ref="B1756" r:id="rId5256"/>
-    <hyperlink ref="C1756" r:id="rId5257"/>
-    <hyperlink ref="E1756" r:id="rId5258"/>
-    <hyperlink ref="B1757" r:id="rId5259"/>
-    <hyperlink ref="C1757" r:id="rId5260"/>
-    <hyperlink ref="E1757" r:id="rId5261"/>
-    <hyperlink ref="B1758" r:id="rId5262"/>
-    <hyperlink ref="C1758" r:id="rId5263"/>
-    <hyperlink ref="E1758" r:id="rId5264"/>
-    <hyperlink ref="B1759" r:id="rId5265"/>
-    <hyperlink ref="C1759" r:id="rId5266"/>
-    <hyperlink ref="E1759" r:id="rId5267"/>
-    <hyperlink ref="B1760" r:id="rId5268"/>
-    <hyperlink ref="C1760" r:id="rId5269"/>
-    <hyperlink ref="E1760" r:id="rId5270"/>
-    <hyperlink ref="B1761" r:id="rId5271"/>
-    <hyperlink ref="C1761" r:id="rId5272"/>
-    <hyperlink ref="E1761" r:id="rId5273"/>
-    <hyperlink ref="B1762" r:id="rId5274"/>
-    <hyperlink ref="C1762" r:id="rId5275"/>
-    <hyperlink ref="E1762" r:id="rId5276"/>
-    <hyperlink ref="B1763" r:id="rId5277"/>
-    <hyperlink ref="C1763" r:id="rId5278"/>
-    <hyperlink ref="E1763" r:id="rId5279"/>
-    <hyperlink ref="B1764" r:id="rId5280"/>
-    <hyperlink ref="C1764" r:id="rId5281"/>
-    <hyperlink ref="E1764" r:id="rId5282" location="pullrequestreview-187798954"/>
-    <hyperlink ref="B1765" r:id="rId5283"/>
-    <hyperlink ref="C1765" r:id="rId5284"/>
-    <hyperlink ref="E1765" r:id="rId5285"/>
-    <hyperlink ref="B1766" r:id="rId5286"/>
-    <hyperlink ref="C1766" r:id="rId5287"/>
-    <hyperlink ref="E1766" r:id="rId5288"/>
-    <hyperlink ref="B1767" r:id="rId5289"/>
-    <hyperlink ref="C1767" r:id="rId5290"/>
-    <hyperlink ref="E1767" r:id="rId5291"/>
-    <hyperlink ref="B1768" r:id="rId5292"/>
-    <hyperlink ref="C1768" r:id="rId5293"/>
-    <hyperlink ref="E1768" r:id="rId5294"/>
-    <hyperlink ref="B1769" r:id="rId5295"/>
-    <hyperlink ref="C1769" r:id="rId5296"/>
-    <hyperlink ref="E1769" r:id="rId5297"/>
-    <hyperlink ref="B1770" r:id="rId5298"/>
-    <hyperlink ref="C1770" r:id="rId5299"/>
-    <hyperlink ref="E1770" r:id="rId5300"/>
-    <hyperlink ref="B1771" r:id="rId5301"/>
-    <hyperlink ref="C1771" r:id="rId5302"/>
-    <hyperlink ref="E1771" r:id="rId5303"/>
-    <hyperlink ref="B1772" r:id="rId5304"/>
-    <hyperlink ref="C1772" r:id="rId5305"/>
-    <hyperlink ref="E1772" r:id="rId5306"/>
-    <hyperlink ref="B1773" r:id="rId5307"/>
-    <hyperlink ref="C1773" r:id="rId5308"/>
-    <hyperlink ref="E1773" r:id="rId5309" location="pullrequestreview-187808202"/>
-    <hyperlink ref="B1774" r:id="rId5310"/>
-    <hyperlink ref="C1774" r:id="rId5311"/>
-    <hyperlink ref="E1774" r:id="rId5312" location="pullrequestreview-187807953"/>
-    <hyperlink ref="B1775" r:id="rId5313"/>
-    <hyperlink ref="C1775" r:id="rId5314"/>
-    <hyperlink ref="E1775" r:id="rId5315"/>
-    <hyperlink ref="B1776" r:id="rId5316"/>
-    <hyperlink ref="C1776" r:id="rId5317"/>
-    <hyperlink ref="E1776" r:id="rId5318"/>
-    <hyperlink ref="B1777" r:id="rId5319"/>
-    <hyperlink ref="C1777" r:id="rId5320"/>
-    <hyperlink ref="E1777" r:id="rId5321"/>
-    <hyperlink ref="B1778" r:id="rId5322"/>
-    <hyperlink ref="C1778" r:id="rId5323"/>
-    <hyperlink ref="E1778" r:id="rId5324"/>
-    <hyperlink ref="B1779" r:id="rId5325"/>
-    <hyperlink ref="C1779" r:id="rId5326"/>
-    <hyperlink ref="E1779" r:id="rId5327"/>
-    <hyperlink ref="B1780" r:id="rId5328"/>
-    <hyperlink ref="C1780" r:id="rId5329"/>
-    <hyperlink ref="E1780" r:id="rId5330"/>
-    <hyperlink ref="B1781" r:id="rId5331"/>
-    <hyperlink ref="C1781" r:id="rId5332"/>
-    <hyperlink ref="E1781" r:id="rId5333"/>
-    <hyperlink ref="B1782" r:id="rId5334"/>
-    <hyperlink ref="C1782" r:id="rId5335"/>
-    <hyperlink ref="E1782" r:id="rId5336" location="pullrequestreview-187951346"/>
-    <hyperlink ref="B1783" r:id="rId5337"/>
-    <hyperlink ref="C1783" r:id="rId5338"/>
-    <hyperlink ref="E1783" r:id="rId5339" location="pullrequestreview-187951565"/>
-    <hyperlink ref="B1784" r:id="rId5340"/>
-    <hyperlink ref="C1784" r:id="rId5341"/>
-    <hyperlink ref="E1784" r:id="rId5342"/>
-    <hyperlink ref="B1785" r:id="rId5343"/>
-    <hyperlink ref="C1785" r:id="rId5344"/>
-    <hyperlink ref="E1785" r:id="rId5345"/>
-    <hyperlink ref="B1786" r:id="rId5346"/>
-    <hyperlink ref="C1786" r:id="rId5347"/>
-    <hyperlink ref="E1786" r:id="rId5348"/>
-    <hyperlink ref="B1787" r:id="rId5349"/>
-    <hyperlink ref="C1787" r:id="rId5350"/>
-    <hyperlink ref="E1787" r:id="rId5351"/>
-    <hyperlink ref="B1788" r:id="rId5352"/>
-    <hyperlink ref="C1788" r:id="rId5353"/>
-    <hyperlink ref="E1788" r:id="rId5354"/>
-    <hyperlink ref="B1789" r:id="rId5355"/>
-    <hyperlink ref="C1789" r:id="rId5356"/>
-    <hyperlink ref="E1789" r:id="rId5357"/>
-    <hyperlink ref="B1790" r:id="rId5358"/>
-    <hyperlink ref="C1790" r:id="rId5359"/>
-    <hyperlink ref="E1790" r:id="rId5360"/>
-    <hyperlink ref="B1791" r:id="rId5361"/>
-    <hyperlink ref="C1791" r:id="rId5362"/>
-    <hyperlink ref="E1791" r:id="rId5363"/>
-    <hyperlink ref="B1792" r:id="rId5364"/>
-    <hyperlink ref="C1792" r:id="rId5365"/>
-    <hyperlink ref="E1792" r:id="rId5366"/>
-    <hyperlink ref="B1793" r:id="rId5367"/>
-    <hyperlink ref="C1793" r:id="rId5368"/>
-    <hyperlink ref="E1793" r:id="rId5369"/>
-    <hyperlink ref="B1794" r:id="rId5370"/>
-    <hyperlink ref="C1794" r:id="rId5371"/>
-    <hyperlink ref="E1794" r:id="rId5372"/>
-    <hyperlink ref="B1795" r:id="rId5373"/>
-    <hyperlink ref="C1795" r:id="rId5374"/>
-    <hyperlink ref="E1795" r:id="rId5375"/>
-    <hyperlink ref="B1796" r:id="rId5376"/>
-    <hyperlink ref="C1796" r:id="rId5377"/>
-    <hyperlink ref="E1796" r:id="rId5378"/>
-    <hyperlink ref="B1797" r:id="rId5379"/>
-    <hyperlink ref="C1797" r:id="rId5380"/>
-    <hyperlink ref="E1797" r:id="rId5381"/>
-    <hyperlink ref="B1798" r:id="rId5382"/>
-    <hyperlink ref="C1798" r:id="rId5383"/>
-    <hyperlink ref="E1798" r:id="rId5384"/>
-    <hyperlink ref="B1799" r:id="rId5385"/>
-    <hyperlink ref="C1799" r:id="rId5386"/>
-    <hyperlink ref="E1799" r:id="rId5387"/>
-    <hyperlink ref="B1800" r:id="rId5388"/>
-    <hyperlink ref="C1800" r:id="rId5389"/>
-    <hyperlink ref="E1800" r:id="rId5390"/>
-    <hyperlink ref="B1801" r:id="rId5391"/>
-    <hyperlink ref="C1801" r:id="rId5392"/>
-    <hyperlink ref="E1801" r:id="rId5393"/>
-    <hyperlink ref="B1802" r:id="rId5394"/>
-    <hyperlink ref="C1802" r:id="rId5395"/>
-    <hyperlink ref="E1802" r:id="rId5396"/>
-    <hyperlink ref="B1803" r:id="rId5397"/>
-    <hyperlink ref="C1803" r:id="rId5398"/>
-    <hyperlink ref="E1803" r:id="rId5399"/>
-    <hyperlink ref="B1804" r:id="rId5400"/>
-    <hyperlink ref="C1804" r:id="rId5401"/>
-    <hyperlink ref="E1804" r:id="rId5402" location="pullrequestreview-188324780"/>
-    <hyperlink ref="B1805" r:id="rId5403"/>
-    <hyperlink ref="C1805" r:id="rId5404"/>
-    <hyperlink ref="E1805" r:id="rId5405"/>
-    <hyperlink ref="B1806" r:id="rId5406"/>
-    <hyperlink ref="C1806" r:id="rId5407"/>
-    <hyperlink ref="E1806" r:id="rId5408" location="pullrequestreview-188380836"/>
-    <hyperlink ref="B1807" r:id="rId5409"/>
-    <hyperlink ref="C1807" r:id="rId5410"/>
-    <hyperlink ref="E1807" r:id="rId5411"/>
-    <hyperlink ref="B1808" r:id="rId5412"/>
-    <hyperlink ref="C1808" r:id="rId5413"/>
-    <hyperlink ref="E1808" r:id="rId5414"/>
-    <hyperlink ref="B1809" r:id="rId5415"/>
-    <hyperlink ref="C1809" r:id="rId5416"/>
-    <hyperlink ref="E1809" r:id="rId5417"/>
-    <hyperlink ref="B1810" r:id="rId5418"/>
-    <hyperlink ref="C1810" r:id="rId5419"/>
-    <hyperlink ref="E1810" r:id="rId5420"/>
-    <hyperlink ref="B1811" r:id="rId5421"/>
-    <hyperlink ref="C1811" r:id="rId5422"/>
-    <hyperlink ref="E1811" r:id="rId5423"/>
-    <hyperlink ref="B1812" r:id="rId5424"/>
-    <hyperlink ref="C1812" r:id="rId5425"/>
-    <hyperlink ref="E1812" r:id="rId5426"/>
-    <hyperlink ref="B1813" r:id="rId5427"/>
-    <hyperlink ref="C1813" r:id="rId5428"/>
-    <hyperlink ref="E1813" r:id="rId5429"/>
-    <hyperlink ref="B1814" r:id="rId5430"/>
-    <hyperlink ref="C1814" r:id="rId5431"/>
-    <hyperlink ref="E1814" r:id="rId5432"/>
-    <hyperlink ref="B1815" r:id="rId5433"/>
-    <hyperlink ref="C1815" r:id="rId5434"/>
-    <hyperlink ref="E1815" r:id="rId5435"/>
-    <hyperlink ref="B1816" r:id="rId5436"/>
-    <hyperlink ref="C1816" r:id="rId5437"/>
-    <hyperlink ref="E1816" r:id="rId5438"/>
-    <hyperlink ref="B1817" r:id="rId5439"/>
-    <hyperlink ref="C1817" r:id="rId5440"/>
-    <hyperlink ref="E1817" r:id="rId5441"/>
-    <hyperlink ref="B1818" r:id="rId5442"/>
-    <hyperlink ref="C1818" r:id="rId5443"/>
-    <hyperlink ref="E1818" r:id="rId5444"/>
-    <hyperlink ref="B1819" r:id="rId5445"/>
-    <hyperlink ref="C1819" r:id="rId5446"/>
-    <hyperlink ref="E1819" r:id="rId5447"/>
-    <hyperlink ref="B1820" r:id="rId5448"/>
-    <hyperlink ref="C1820" r:id="rId5449"/>
-    <hyperlink ref="E1820" r:id="rId5450"/>
-    <hyperlink ref="B1821" r:id="rId5451"/>
-    <hyperlink ref="C1821" r:id="rId5452"/>
-    <hyperlink ref="E1821" r:id="rId5453"/>
-    <hyperlink ref="B1822" r:id="rId5454"/>
-    <hyperlink ref="C1822" r:id="rId5455"/>
-    <hyperlink ref="E1822" r:id="rId5456"/>
-    <hyperlink ref="B1823" r:id="rId5457"/>
-    <hyperlink ref="C1823" r:id="rId5458"/>
-    <hyperlink ref="E1823" r:id="rId5459"/>
-    <hyperlink ref="B1824" r:id="rId5460"/>
-    <hyperlink ref="C1824" r:id="rId5461"/>
-    <hyperlink ref="E1824" r:id="rId5462"/>
-    <hyperlink ref="B1825" r:id="rId5463"/>
-    <hyperlink ref="C1825" r:id="rId5464"/>
-    <hyperlink ref="E1825" r:id="rId5465"/>
-    <hyperlink ref="B1826" r:id="rId5466"/>
-    <hyperlink ref="C1826" r:id="rId5467"/>
-    <hyperlink ref="E1826" r:id="rId5468"/>
-    <hyperlink ref="B1827" r:id="rId5469"/>
-    <hyperlink ref="C1827" r:id="rId5470"/>
-    <hyperlink ref="E1827" r:id="rId5471"/>
-    <hyperlink ref="B1828" r:id="rId5472"/>
-    <hyperlink ref="C1828" r:id="rId5473"/>
-    <hyperlink ref="E1828" r:id="rId5474"/>
-    <hyperlink ref="B1829" r:id="rId5475"/>
-    <hyperlink ref="C1829" r:id="rId5476"/>
-    <hyperlink ref="E1829" r:id="rId5477"/>
-    <hyperlink ref="B1830" r:id="rId5478"/>
-    <hyperlink ref="C1830" r:id="rId5479"/>
-    <hyperlink ref="E1830" r:id="rId5480"/>
-    <hyperlink ref="B1831" r:id="rId5481"/>
-    <hyperlink ref="C1831" r:id="rId5482"/>
-    <hyperlink ref="E1831" r:id="rId5483"/>
-    <hyperlink ref="B1832" r:id="rId5484"/>
-    <hyperlink ref="C1832" r:id="rId5485"/>
-    <hyperlink ref="E1832" r:id="rId5486"/>
-    <hyperlink ref="B1833" r:id="rId5487"/>
-    <hyperlink ref="C1833" r:id="rId5488"/>
-    <hyperlink ref="E1833" r:id="rId5489"/>
-    <hyperlink ref="B1834" r:id="rId5490"/>
-    <hyperlink ref="C1834" r:id="rId5491"/>
-    <hyperlink ref="E1834" r:id="rId5492"/>
-    <hyperlink ref="B1835" r:id="rId5493"/>
-    <hyperlink ref="C1835" r:id="rId5494"/>
-    <hyperlink ref="E1835" r:id="rId5495"/>
-    <hyperlink ref="B1836" r:id="rId5496"/>
-    <hyperlink ref="C1836" r:id="rId5497"/>
-    <hyperlink ref="E1836" r:id="rId5498"/>
-    <hyperlink ref="B1837" r:id="rId5499"/>
-    <hyperlink ref="C1837" r:id="rId5500"/>
-    <hyperlink ref="E1837" r:id="rId5501"/>
-    <hyperlink ref="B1838" r:id="rId5502"/>
-    <hyperlink ref="C1838" r:id="rId5503"/>
-    <hyperlink ref="E1838" r:id="rId5504"/>
-    <hyperlink ref="B1839" r:id="rId5505"/>
-    <hyperlink ref="C1839" r:id="rId5506"/>
-    <hyperlink ref="E1839" r:id="rId5507"/>
-    <hyperlink ref="B1840" r:id="rId5508"/>
-    <hyperlink ref="C1840" r:id="rId5509"/>
-    <hyperlink ref="E1840" r:id="rId5510"/>
-    <hyperlink ref="B1841" r:id="rId5511"/>
-    <hyperlink ref="C1841" r:id="rId5512"/>
-    <hyperlink ref="E1841" r:id="rId5513"/>
-    <hyperlink ref="B1842" r:id="rId5514"/>
-    <hyperlink ref="C1842" r:id="rId5515"/>
-    <hyperlink ref="E1842" r:id="rId5516"/>
-    <hyperlink ref="B1843" r:id="rId5517"/>
-    <hyperlink ref="C1843" r:id="rId5518"/>
-    <hyperlink ref="E1843" r:id="rId5519"/>
-    <hyperlink ref="B1844" r:id="rId5520"/>
-    <hyperlink ref="C1844" r:id="rId5521"/>
-    <hyperlink ref="E1844" r:id="rId5522"/>
-    <hyperlink ref="B1845" r:id="rId5523"/>
-    <hyperlink ref="C1845" r:id="rId5524"/>
-    <hyperlink ref="E1845" r:id="rId5525"/>
-    <hyperlink ref="B1846" r:id="rId5526"/>
-    <hyperlink ref="C1846" r:id="rId5527"/>
-    <hyperlink ref="E1846" r:id="rId5528"/>
-    <hyperlink ref="B1847" r:id="rId5529"/>
-    <hyperlink ref="C1847" r:id="rId5530"/>
-    <hyperlink ref="E1847" r:id="rId5531"/>
-    <hyperlink ref="B1848" r:id="rId5532"/>
-    <hyperlink ref="C1848" r:id="rId5533"/>
-    <hyperlink ref="E1848" r:id="rId5534"/>
-    <hyperlink ref="B1849" r:id="rId5535"/>
-    <hyperlink ref="C1849" r:id="rId5536"/>
-    <hyperlink ref="E1849" r:id="rId5537"/>
-    <hyperlink ref="B1850" r:id="rId5538"/>
-    <hyperlink ref="C1850" r:id="rId5539"/>
-    <hyperlink ref="E1850" r:id="rId5540"/>
-    <hyperlink ref="B1851" r:id="rId5541"/>
-    <hyperlink ref="C1851" r:id="rId5542"/>
-    <hyperlink ref="E1851" r:id="rId5543"/>
-    <hyperlink ref="B1852" r:id="rId5544"/>
-    <hyperlink ref="C1852" r:id="rId5545"/>
-    <hyperlink ref="E1852" r:id="rId5546"/>
-    <hyperlink ref="B1853" r:id="rId5547"/>
-    <hyperlink ref="C1853" r:id="rId5548"/>
-    <hyperlink ref="E1853" r:id="rId5549"/>
-    <hyperlink ref="B1854" r:id="rId5550"/>
-    <hyperlink ref="C1854" r:id="rId5551"/>
-    <hyperlink ref="E1854" r:id="rId5552"/>
-    <hyperlink ref="B1855" r:id="rId5553"/>
-    <hyperlink ref="C1855" r:id="rId5554"/>
-    <hyperlink ref="E1855" r:id="rId5555"/>
-    <hyperlink ref="B1856" r:id="rId5556"/>
-    <hyperlink ref="C1856" r:id="rId5557"/>
-    <hyperlink ref="E1856" r:id="rId5558"/>
-    <hyperlink ref="B1857" r:id="rId5559"/>
-    <hyperlink ref="C1857" r:id="rId5560"/>
-    <hyperlink ref="E1857" r:id="rId5561"/>
-    <hyperlink ref="B1858" r:id="rId5562"/>
-    <hyperlink ref="C1858" r:id="rId5563"/>
-    <hyperlink ref="E1858" r:id="rId5564"/>
-    <hyperlink ref="B1859" r:id="rId5565"/>
-    <hyperlink ref="C1859" r:id="rId5566"/>
-    <hyperlink ref="E1859" r:id="rId5567"/>
-    <hyperlink ref="B1860" r:id="rId5568"/>
-    <hyperlink ref="C1860" r:id="rId5569"/>
-    <hyperlink ref="E1860" r:id="rId5570"/>
-    <hyperlink ref="B1861" r:id="rId5571"/>
-    <hyperlink ref="C1861" r:id="rId5572"/>
-    <hyperlink ref="E1861" r:id="rId5573"/>
-    <hyperlink ref="B1862" r:id="rId5574"/>
-    <hyperlink ref="C1862" r:id="rId5575"/>
-    <hyperlink ref="E1862" r:id="rId5576"/>
-    <hyperlink ref="B1863" r:id="rId5577"/>
-    <hyperlink ref="C1863" r:id="rId5578"/>
-    <hyperlink ref="E1863" r:id="rId5579"/>
-    <hyperlink ref="B1864" r:id="rId5580"/>
-    <hyperlink ref="C1864" r:id="rId5581"/>
-    <hyperlink ref="E1864" r:id="rId5582"/>
-    <hyperlink ref="B1865" r:id="rId5583"/>
-    <hyperlink ref="C1865" r:id="rId5584"/>
-    <hyperlink ref="E1865" r:id="rId5585"/>
+    <hyperlink ref="B1301" r:id="rId3887"/>
+    <hyperlink ref="C1301" r:id="rId3888"/>
+    <hyperlink ref="E1301" r:id="rId3889"/>
+    <hyperlink ref="B1302" r:id="rId3890"/>
+    <hyperlink ref="C1302" r:id="rId3891"/>
+    <hyperlink ref="E1302" r:id="rId3892"/>
+    <hyperlink ref="B1303" r:id="rId3893"/>
+    <hyperlink ref="C1303" r:id="rId3894"/>
+    <hyperlink ref="E1303" r:id="rId3895" location="pullrequestreview-180535268"/>
+    <hyperlink ref="B1304" r:id="rId3896"/>
+    <hyperlink ref="C1304" r:id="rId3897"/>
+    <hyperlink ref="E1304" r:id="rId3898" location="pullrequestreview-180527806"/>
+    <hyperlink ref="B1305" r:id="rId3899"/>
+    <hyperlink ref="C1305" r:id="rId3900"/>
+    <hyperlink ref="E1305" r:id="rId3901" location="pullrequestreview-180537012"/>
+    <hyperlink ref="B1306" r:id="rId3902"/>
+    <hyperlink ref="C1306" r:id="rId3903"/>
+    <hyperlink ref="E1306" r:id="rId3904"/>
+    <hyperlink ref="B1307" r:id="rId3905"/>
+    <hyperlink ref="C1307" r:id="rId3906"/>
+    <hyperlink ref="E1307" r:id="rId3907"/>
+    <hyperlink ref="B1308" r:id="rId3908"/>
+    <hyperlink ref="C1308" r:id="rId3909"/>
+    <hyperlink ref="E1308" r:id="rId3910"/>
+    <hyperlink ref="B1309" r:id="rId3911"/>
+    <hyperlink ref="C1309" r:id="rId3912"/>
+    <hyperlink ref="E1309" r:id="rId3913"/>
+    <hyperlink ref="B1310" r:id="rId3914"/>
+    <hyperlink ref="C1310" r:id="rId3915"/>
+    <hyperlink ref="E1310" r:id="rId3916"/>
+    <hyperlink ref="B1311" r:id="rId3917"/>
+    <hyperlink ref="C1311" r:id="rId3918"/>
+    <hyperlink ref="E1311" r:id="rId3919"/>
+    <hyperlink ref="B1312" r:id="rId3920"/>
+    <hyperlink ref="C1312" r:id="rId3921"/>
+    <hyperlink ref="E1312" r:id="rId3922"/>
+    <hyperlink ref="B1313" r:id="rId3923"/>
+    <hyperlink ref="C1313" r:id="rId3924"/>
+    <hyperlink ref="E1313" r:id="rId3925"/>
+    <hyperlink ref="B1314" r:id="rId3926"/>
+    <hyperlink ref="C1314" r:id="rId3927"/>
+    <hyperlink ref="E1314" r:id="rId3928"/>
+    <hyperlink ref="B1315" r:id="rId3929"/>
+    <hyperlink ref="C1315" r:id="rId3930"/>
+    <hyperlink ref="E1315" r:id="rId3931"/>
+    <hyperlink ref="B1316" r:id="rId3932"/>
+    <hyperlink ref="C1316" r:id="rId3933"/>
+    <hyperlink ref="E1316" r:id="rId3934"/>
+    <hyperlink ref="B1317" r:id="rId3935"/>
+    <hyperlink ref="C1317" r:id="rId3936"/>
+    <hyperlink ref="E1317" r:id="rId3937"/>
+    <hyperlink ref="B1318" r:id="rId3938"/>
+    <hyperlink ref="C1318" r:id="rId3939"/>
+    <hyperlink ref="E1318" r:id="rId3940"/>
+    <hyperlink ref="B1319" r:id="rId3941"/>
+    <hyperlink ref="C1319" r:id="rId3942"/>
+    <hyperlink ref="E1319" r:id="rId3943"/>
+    <hyperlink ref="B1320" r:id="rId3944"/>
+    <hyperlink ref="C1320" r:id="rId3945"/>
+    <hyperlink ref="E1320" r:id="rId3946"/>
+    <hyperlink ref="B1321" r:id="rId3947"/>
+    <hyperlink ref="C1321" r:id="rId3948"/>
+    <hyperlink ref="E1321" r:id="rId3949"/>
+    <hyperlink ref="B1322" r:id="rId3950"/>
+    <hyperlink ref="C1322" r:id="rId3951"/>
+    <hyperlink ref="E1322" r:id="rId3952"/>
+    <hyperlink ref="B1323" r:id="rId3953"/>
+    <hyperlink ref="C1323" r:id="rId3954"/>
+    <hyperlink ref="E1323" r:id="rId3955"/>
+    <hyperlink ref="B1324" r:id="rId3956"/>
+    <hyperlink ref="C1324" r:id="rId3957"/>
+    <hyperlink ref="E1324" r:id="rId3958"/>
+    <hyperlink ref="B1325" r:id="rId3959"/>
+    <hyperlink ref="C1325" r:id="rId3960"/>
+    <hyperlink ref="E1325" r:id="rId3961"/>
+    <hyperlink ref="B1326" r:id="rId3962"/>
+    <hyperlink ref="C1326" r:id="rId3963"/>
+    <hyperlink ref="E1326" r:id="rId3964"/>
+    <hyperlink ref="B1327" r:id="rId3965"/>
+    <hyperlink ref="C1327" r:id="rId3966"/>
+    <hyperlink ref="E1327" r:id="rId3967"/>
+    <hyperlink ref="B1328" r:id="rId3968"/>
+    <hyperlink ref="C1328" r:id="rId3969"/>
+    <hyperlink ref="E1328" r:id="rId3970"/>
+    <hyperlink ref="B1329" r:id="rId3971"/>
+    <hyperlink ref="C1329" r:id="rId3972"/>
+    <hyperlink ref="E1329" r:id="rId3973"/>
+    <hyperlink ref="B1330" r:id="rId3974"/>
+    <hyperlink ref="C1330" r:id="rId3975"/>
+    <hyperlink ref="E1330" r:id="rId3976"/>
+    <hyperlink ref="B1331" r:id="rId3977"/>
+    <hyperlink ref="C1331" r:id="rId3978"/>
+    <hyperlink ref="E1331" r:id="rId3979"/>
+    <hyperlink ref="B1332" r:id="rId3980"/>
+    <hyperlink ref="C1332" r:id="rId3981"/>
+    <hyperlink ref="E1332" r:id="rId3982"/>
+    <hyperlink ref="B1333" r:id="rId3983"/>
+    <hyperlink ref="C1333" r:id="rId3984"/>
+    <hyperlink ref="E1333" r:id="rId3985"/>
+    <hyperlink ref="B1334" r:id="rId3986"/>
+    <hyperlink ref="C1334" r:id="rId3987"/>
+    <hyperlink ref="E1334" r:id="rId3988"/>
+    <hyperlink ref="B1335" r:id="rId3989"/>
+    <hyperlink ref="C1335" r:id="rId3990"/>
+    <hyperlink ref="E1335" r:id="rId3991"/>
+    <hyperlink ref="B1336" r:id="rId3992"/>
+    <hyperlink ref="C1336" r:id="rId3993"/>
+    <hyperlink ref="E1336" r:id="rId3994"/>
+    <hyperlink ref="B1337" r:id="rId3995"/>
+    <hyperlink ref="C1337" r:id="rId3996"/>
+    <hyperlink ref="E1337" r:id="rId3997"/>
+    <hyperlink ref="B1338" r:id="rId3998"/>
+    <hyperlink ref="C1338" r:id="rId3999"/>
+    <hyperlink ref="E1338" r:id="rId4000"/>
+    <hyperlink ref="B1339" r:id="rId4001"/>
+    <hyperlink ref="C1339" r:id="rId4002"/>
+    <hyperlink ref="E1339" r:id="rId4003"/>
+    <hyperlink ref="B1340" r:id="rId4004"/>
+    <hyperlink ref="C1340" r:id="rId4005"/>
+    <hyperlink ref="E1340" r:id="rId4006"/>
+    <hyperlink ref="B1341" r:id="rId4007"/>
+    <hyperlink ref="C1341" r:id="rId4008"/>
+    <hyperlink ref="E1341" r:id="rId4009"/>
+    <hyperlink ref="B1342" r:id="rId4010"/>
+    <hyperlink ref="C1342" r:id="rId4011"/>
+    <hyperlink ref="E1342" r:id="rId4012"/>
+    <hyperlink ref="B1343" r:id="rId4013"/>
+    <hyperlink ref="C1343" r:id="rId4014"/>
+    <hyperlink ref="E1343" r:id="rId4015"/>
+    <hyperlink ref="B1344" r:id="rId4016"/>
+    <hyperlink ref="C1344" r:id="rId4017"/>
+    <hyperlink ref="E1344" r:id="rId4018"/>
+    <hyperlink ref="B1345" r:id="rId4019"/>
+    <hyperlink ref="C1345" r:id="rId4020"/>
+    <hyperlink ref="E1345" r:id="rId4021"/>
+    <hyperlink ref="B1346" r:id="rId4022"/>
+    <hyperlink ref="C1346" r:id="rId4023"/>
+    <hyperlink ref="E1346" r:id="rId4024"/>
+    <hyperlink ref="B1347" r:id="rId4025"/>
+    <hyperlink ref="C1347" r:id="rId4026"/>
+    <hyperlink ref="E1347" r:id="rId4027"/>
+    <hyperlink ref="B1348" r:id="rId4028"/>
+    <hyperlink ref="C1348" r:id="rId4029"/>
+    <hyperlink ref="E1348" r:id="rId4030"/>
+    <hyperlink ref="B1349" r:id="rId4031"/>
+    <hyperlink ref="C1349" r:id="rId4032"/>
+    <hyperlink ref="E1349" r:id="rId4033"/>
+    <hyperlink ref="B1350" r:id="rId4034"/>
+    <hyperlink ref="C1350" r:id="rId4035"/>
+    <hyperlink ref="E1350" r:id="rId4036"/>
+    <hyperlink ref="B1351" r:id="rId4037"/>
+    <hyperlink ref="C1351" r:id="rId4038"/>
+    <hyperlink ref="E1351" r:id="rId4039"/>
+    <hyperlink ref="B1352" r:id="rId4040"/>
+    <hyperlink ref="C1352" r:id="rId4041"/>
+    <hyperlink ref="E1352" r:id="rId4042"/>
+    <hyperlink ref="B1353" r:id="rId4043"/>
+    <hyperlink ref="C1353" r:id="rId4044"/>
+    <hyperlink ref="E1353" r:id="rId4045"/>
+    <hyperlink ref="B1354" r:id="rId4046"/>
+    <hyperlink ref="C1354" r:id="rId4047"/>
+    <hyperlink ref="E1354" r:id="rId4048"/>
+    <hyperlink ref="B1355" r:id="rId4049"/>
+    <hyperlink ref="C1355" r:id="rId4050"/>
+    <hyperlink ref="E1355" r:id="rId4051"/>
+    <hyperlink ref="B1356" r:id="rId4052"/>
+    <hyperlink ref="C1356" r:id="rId4053"/>
+    <hyperlink ref="E1356" r:id="rId4054"/>
+    <hyperlink ref="G1356" r:id="rId4055"/>
+    <hyperlink ref="B1357" r:id="rId4056"/>
+    <hyperlink ref="C1357" r:id="rId4057"/>
+    <hyperlink ref="E1357" r:id="rId4058"/>
+    <hyperlink ref="B1358" r:id="rId4059"/>
+    <hyperlink ref="C1358" r:id="rId4060"/>
+    <hyperlink ref="E1358" r:id="rId4061"/>
+    <hyperlink ref="B1359" r:id="rId4062"/>
+    <hyperlink ref="C1359" r:id="rId4063"/>
+    <hyperlink ref="E1359" r:id="rId4064"/>
+    <hyperlink ref="B1360" r:id="rId4065"/>
+    <hyperlink ref="C1360" r:id="rId4066"/>
+    <hyperlink ref="E1360" r:id="rId4067"/>
+    <hyperlink ref="B1361" r:id="rId4068"/>
+    <hyperlink ref="C1361" r:id="rId4069"/>
+    <hyperlink ref="E1361" r:id="rId4070"/>
+    <hyperlink ref="B1362" r:id="rId4071"/>
+    <hyperlink ref="C1362" r:id="rId4072"/>
+    <hyperlink ref="E1362" r:id="rId4073"/>
+    <hyperlink ref="B1363" r:id="rId4074"/>
+    <hyperlink ref="C1363" r:id="rId4075"/>
+    <hyperlink ref="E1363" r:id="rId4076"/>
+    <hyperlink ref="B1364" r:id="rId4077"/>
+    <hyperlink ref="C1364" r:id="rId4078"/>
+    <hyperlink ref="E1364" r:id="rId4079"/>
+    <hyperlink ref="B1365" r:id="rId4080"/>
+    <hyperlink ref="C1365" r:id="rId4081"/>
+    <hyperlink ref="E1365" r:id="rId4082"/>
+    <hyperlink ref="B1366" r:id="rId4083"/>
+    <hyperlink ref="C1366" r:id="rId4084"/>
+    <hyperlink ref="E1366" r:id="rId4085"/>
+    <hyperlink ref="B1367" r:id="rId4086"/>
+    <hyperlink ref="C1367" r:id="rId4087"/>
+    <hyperlink ref="E1367" r:id="rId4088"/>
+    <hyperlink ref="B1368" r:id="rId4089"/>
+    <hyperlink ref="C1368" r:id="rId4090"/>
+    <hyperlink ref="E1368" r:id="rId4091"/>
+    <hyperlink ref="B1369" r:id="rId4092"/>
+    <hyperlink ref="C1369" r:id="rId4093"/>
+    <hyperlink ref="E1369" r:id="rId4094"/>
+    <hyperlink ref="B1370" r:id="rId4095"/>
+    <hyperlink ref="C1370" r:id="rId4096"/>
+    <hyperlink ref="E1370" r:id="rId4097"/>
+    <hyperlink ref="B1371" r:id="rId4098"/>
+    <hyperlink ref="C1371" r:id="rId4099"/>
+    <hyperlink ref="E1371" r:id="rId4100"/>
+    <hyperlink ref="B1372" r:id="rId4101"/>
+    <hyperlink ref="C1372" r:id="rId4102"/>
+    <hyperlink ref="E1372" r:id="rId4103"/>
+    <hyperlink ref="B1373" r:id="rId4104"/>
+    <hyperlink ref="C1373" r:id="rId4105"/>
+    <hyperlink ref="E1373" r:id="rId4106"/>
+    <hyperlink ref="B1374" r:id="rId4107"/>
+    <hyperlink ref="C1374" r:id="rId4108"/>
+    <hyperlink ref="E1374" r:id="rId4109"/>
+    <hyperlink ref="B1375" r:id="rId4110"/>
+    <hyperlink ref="C1375" r:id="rId4111"/>
+    <hyperlink ref="E1375" r:id="rId4112"/>
+    <hyperlink ref="B1376" r:id="rId4113"/>
+    <hyperlink ref="C1376" r:id="rId4114"/>
+    <hyperlink ref="E1376" r:id="rId4115"/>
+    <hyperlink ref="B1377" r:id="rId4116"/>
+    <hyperlink ref="C1377" r:id="rId4117"/>
+    <hyperlink ref="E1377" r:id="rId4118" location="pullrequestreview-181806388"/>
+    <hyperlink ref="B1378" r:id="rId4119"/>
+    <hyperlink ref="C1378" r:id="rId4120"/>
+    <hyperlink ref="E1378" r:id="rId4121"/>
+    <hyperlink ref="B1379" r:id="rId4122"/>
+    <hyperlink ref="C1379" r:id="rId4123"/>
+    <hyperlink ref="E1379" r:id="rId4124"/>
+    <hyperlink ref="B1380" r:id="rId4125"/>
+    <hyperlink ref="C1380" r:id="rId4126"/>
+    <hyperlink ref="E1380" r:id="rId4127"/>
+    <hyperlink ref="B1381" r:id="rId4128"/>
+    <hyperlink ref="C1381" r:id="rId4129"/>
+    <hyperlink ref="E1381" r:id="rId4130"/>
+    <hyperlink ref="B1382" r:id="rId4131"/>
+    <hyperlink ref="C1382" r:id="rId4132"/>
+    <hyperlink ref="E1382" r:id="rId4133"/>
+    <hyperlink ref="B1383" r:id="rId4134"/>
+    <hyperlink ref="C1383" r:id="rId4135"/>
+    <hyperlink ref="E1383" r:id="rId4136"/>
+    <hyperlink ref="B1384" r:id="rId4137"/>
+    <hyperlink ref="C1384" r:id="rId4138"/>
+    <hyperlink ref="E1384" r:id="rId4139"/>
+    <hyperlink ref="B1385" r:id="rId4140"/>
+    <hyperlink ref="C1385" r:id="rId4141"/>
+    <hyperlink ref="E1385" r:id="rId4142"/>
+    <hyperlink ref="B1386" r:id="rId4143"/>
+    <hyperlink ref="C1386" r:id="rId4144"/>
+    <hyperlink ref="E1386" r:id="rId4145"/>
+    <hyperlink ref="B1387" r:id="rId4146"/>
+    <hyperlink ref="C1387" r:id="rId4147"/>
+    <hyperlink ref="E1387" r:id="rId4148"/>
+    <hyperlink ref="B1388" r:id="rId4149"/>
+    <hyperlink ref="C1388" r:id="rId4150"/>
+    <hyperlink ref="E1388" r:id="rId4151"/>
+    <hyperlink ref="B1389" r:id="rId4152"/>
+    <hyperlink ref="C1389" r:id="rId4153"/>
+    <hyperlink ref="E1389" r:id="rId4154"/>
+    <hyperlink ref="B1390" r:id="rId4155"/>
+    <hyperlink ref="C1390" r:id="rId4156"/>
+    <hyperlink ref="E1390" r:id="rId4157"/>
+    <hyperlink ref="B1391" r:id="rId4158"/>
+    <hyperlink ref="C1391" r:id="rId4159"/>
+    <hyperlink ref="E1391" r:id="rId4160"/>
+    <hyperlink ref="B1392" r:id="rId4161"/>
+    <hyperlink ref="C1392" r:id="rId4162"/>
+    <hyperlink ref="E1392" r:id="rId4163"/>
+    <hyperlink ref="B1393" r:id="rId4164"/>
+    <hyperlink ref="C1393" r:id="rId4165"/>
+    <hyperlink ref="E1393" r:id="rId4166"/>
+    <hyperlink ref="B1394" r:id="rId4167"/>
+    <hyperlink ref="C1394" r:id="rId4168"/>
+    <hyperlink ref="E1394" r:id="rId4169"/>
+    <hyperlink ref="B1395" r:id="rId4170"/>
+    <hyperlink ref="C1395" r:id="rId4171"/>
+    <hyperlink ref="E1395" r:id="rId4172"/>
+    <hyperlink ref="B1396" r:id="rId4173"/>
+    <hyperlink ref="C1396" r:id="rId4174"/>
+    <hyperlink ref="E1396" r:id="rId4175"/>
+    <hyperlink ref="B1397" r:id="rId4176"/>
+    <hyperlink ref="C1397" r:id="rId4177"/>
+    <hyperlink ref="E1397" r:id="rId4178"/>
+    <hyperlink ref="B1398" r:id="rId4179"/>
+    <hyperlink ref="C1398" r:id="rId4180"/>
+    <hyperlink ref="E1398" r:id="rId4181"/>
+    <hyperlink ref="B1399" r:id="rId4182"/>
+    <hyperlink ref="C1399" r:id="rId4183"/>
+    <hyperlink ref="E1399" r:id="rId4184"/>
+    <hyperlink ref="B1400" r:id="rId4185"/>
+    <hyperlink ref="C1400" r:id="rId4186"/>
+    <hyperlink ref="E1400" r:id="rId4187"/>
+    <hyperlink ref="B1401" r:id="rId4188"/>
+    <hyperlink ref="C1401" r:id="rId4189"/>
+    <hyperlink ref="E1401" r:id="rId4190"/>
+    <hyperlink ref="B1402" r:id="rId4191"/>
+    <hyperlink ref="C1402" r:id="rId4192"/>
+    <hyperlink ref="E1402" r:id="rId4193"/>
+    <hyperlink ref="B1403" r:id="rId4194"/>
+    <hyperlink ref="C1403" r:id="rId4195"/>
+    <hyperlink ref="E1403" r:id="rId4196"/>
+    <hyperlink ref="B1404" r:id="rId4197"/>
+    <hyperlink ref="C1404" r:id="rId4198"/>
+    <hyperlink ref="E1404" r:id="rId4199"/>
+    <hyperlink ref="B1405" r:id="rId4200"/>
+    <hyperlink ref="C1405" r:id="rId4201"/>
+    <hyperlink ref="E1405" r:id="rId4202"/>
+    <hyperlink ref="B1406" r:id="rId4203"/>
+    <hyperlink ref="C1406" r:id="rId4204"/>
+    <hyperlink ref="E1406" r:id="rId4205"/>
+    <hyperlink ref="B1407" r:id="rId4206"/>
+    <hyperlink ref="C1407" r:id="rId4207"/>
+    <hyperlink ref="E1407" r:id="rId4208"/>
+    <hyperlink ref="B1408" r:id="rId4209"/>
+    <hyperlink ref="C1408" r:id="rId4210"/>
+    <hyperlink ref="E1408" r:id="rId4211"/>
+    <hyperlink ref="B1409" r:id="rId4212"/>
+    <hyperlink ref="C1409" r:id="rId4213"/>
+    <hyperlink ref="E1409" r:id="rId4214"/>
+    <hyperlink ref="B1410" r:id="rId4215"/>
+    <hyperlink ref="C1410" r:id="rId4216"/>
+    <hyperlink ref="E1410" r:id="rId4217"/>
+    <hyperlink ref="B1411" r:id="rId4218"/>
+    <hyperlink ref="C1411" r:id="rId4219"/>
+    <hyperlink ref="E1411" r:id="rId4220"/>
+    <hyperlink ref="B1412" r:id="rId4221"/>
+    <hyperlink ref="C1412" r:id="rId4222"/>
+    <hyperlink ref="E1412" r:id="rId4223"/>
+    <hyperlink ref="B1413" r:id="rId4224"/>
+    <hyperlink ref="C1413" r:id="rId4225"/>
+    <hyperlink ref="E1413" r:id="rId4226"/>
+    <hyperlink ref="B1414" r:id="rId4227"/>
+    <hyperlink ref="C1414" r:id="rId4228"/>
+    <hyperlink ref="E1414" r:id="rId4229"/>
+    <hyperlink ref="B1415" r:id="rId4230"/>
+    <hyperlink ref="C1415" r:id="rId4231"/>
+    <hyperlink ref="E1415" r:id="rId4232"/>
+    <hyperlink ref="B1416" r:id="rId4233"/>
+    <hyperlink ref="C1416" r:id="rId4234"/>
+    <hyperlink ref="E1416" r:id="rId4235"/>
+    <hyperlink ref="B1417" r:id="rId4236"/>
+    <hyperlink ref="C1417" r:id="rId4237"/>
+    <hyperlink ref="E1417" r:id="rId4238"/>
+    <hyperlink ref="B1418" r:id="rId4239"/>
+    <hyperlink ref="C1418" r:id="rId4240"/>
+    <hyperlink ref="E1418" r:id="rId4241"/>
+    <hyperlink ref="B1419" r:id="rId4242"/>
+    <hyperlink ref="C1419" r:id="rId4243"/>
+    <hyperlink ref="E1419" r:id="rId4244"/>
+    <hyperlink ref="B1420" r:id="rId4245"/>
+    <hyperlink ref="C1420" r:id="rId4246"/>
+    <hyperlink ref="E1420" r:id="rId4247"/>
+    <hyperlink ref="B1421" r:id="rId4248"/>
+    <hyperlink ref="C1421" r:id="rId4249"/>
+    <hyperlink ref="E1421" r:id="rId4250"/>
+    <hyperlink ref="B1422" r:id="rId4251"/>
+    <hyperlink ref="C1422" r:id="rId4252"/>
+    <hyperlink ref="E1422" r:id="rId4253"/>
+    <hyperlink ref="B1423" r:id="rId4254"/>
+    <hyperlink ref="C1423" r:id="rId4255"/>
+    <hyperlink ref="E1423" r:id="rId4256"/>
+    <hyperlink ref="B1424" r:id="rId4257"/>
+    <hyperlink ref="C1424" r:id="rId4258"/>
+    <hyperlink ref="E1424" r:id="rId4259"/>
+    <hyperlink ref="B1425" r:id="rId4260"/>
+    <hyperlink ref="C1425" r:id="rId4261"/>
+    <hyperlink ref="E1425" r:id="rId4262"/>
+    <hyperlink ref="B1426" r:id="rId4263"/>
+    <hyperlink ref="C1426" r:id="rId4264"/>
+    <hyperlink ref="E1426" r:id="rId4265"/>
+    <hyperlink ref="B1427" r:id="rId4266"/>
+    <hyperlink ref="C1427" r:id="rId4267"/>
+    <hyperlink ref="E1427" r:id="rId4268"/>
+    <hyperlink ref="B1428" r:id="rId4269"/>
+    <hyperlink ref="C1428" r:id="rId4270"/>
+    <hyperlink ref="E1428" r:id="rId4271"/>
+    <hyperlink ref="B1429" r:id="rId4272"/>
+    <hyperlink ref="C1429" r:id="rId4273"/>
+    <hyperlink ref="E1429" r:id="rId4274"/>
+    <hyperlink ref="B1430" r:id="rId4275"/>
+    <hyperlink ref="C1430" r:id="rId4276"/>
+    <hyperlink ref="E1430" r:id="rId4277"/>
+    <hyperlink ref="B1431" r:id="rId4278"/>
+    <hyperlink ref="C1431" r:id="rId4279"/>
+    <hyperlink ref="E1431" r:id="rId4280"/>
+    <hyperlink ref="B1432" r:id="rId4281"/>
+    <hyperlink ref="C1432" r:id="rId4282"/>
+    <hyperlink ref="E1432" r:id="rId4283"/>
+    <hyperlink ref="B1433" r:id="rId4284"/>
+    <hyperlink ref="C1433" r:id="rId4285"/>
+    <hyperlink ref="E1433" r:id="rId4286"/>
+    <hyperlink ref="B1434" r:id="rId4287"/>
+    <hyperlink ref="C1434" r:id="rId4288"/>
+    <hyperlink ref="E1434" r:id="rId4289"/>
+    <hyperlink ref="B1435" r:id="rId4290"/>
+    <hyperlink ref="C1435" r:id="rId4291"/>
+    <hyperlink ref="E1435" r:id="rId4292"/>
+    <hyperlink ref="B1436" r:id="rId4293"/>
+    <hyperlink ref="C1436" r:id="rId4294"/>
+    <hyperlink ref="E1436" r:id="rId4295"/>
+    <hyperlink ref="B1437" r:id="rId4296"/>
+    <hyperlink ref="C1437" r:id="rId4297"/>
+    <hyperlink ref="E1437" r:id="rId4298"/>
+    <hyperlink ref="B1438" r:id="rId4299"/>
+    <hyperlink ref="C1438" r:id="rId4300"/>
+    <hyperlink ref="E1438" r:id="rId4301"/>
+    <hyperlink ref="B1439" r:id="rId4302"/>
+    <hyperlink ref="C1439" r:id="rId4303"/>
+    <hyperlink ref="E1439" r:id="rId4304"/>
+    <hyperlink ref="B1440" r:id="rId4305"/>
+    <hyperlink ref="C1440" r:id="rId4306"/>
+    <hyperlink ref="E1440" r:id="rId4307"/>
+    <hyperlink ref="B1441" r:id="rId4308"/>
+    <hyperlink ref="C1441" r:id="rId4309"/>
+    <hyperlink ref="E1441" r:id="rId4310"/>
+    <hyperlink ref="B1442" r:id="rId4311"/>
+    <hyperlink ref="C1442" r:id="rId4312"/>
+    <hyperlink ref="E1442" r:id="rId4313"/>
+    <hyperlink ref="B1443" r:id="rId4314"/>
+    <hyperlink ref="C1443" r:id="rId4315"/>
+    <hyperlink ref="E1443" r:id="rId4316"/>
+    <hyperlink ref="B1444" r:id="rId4317"/>
+    <hyperlink ref="C1444" r:id="rId4318"/>
+    <hyperlink ref="E1444" r:id="rId4319"/>
+    <hyperlink ref="B1445" r:id="rId4320"/>
+    <hyperlink ref="C1445" r:id="rId4321"/>
+    <hyperlink ref="E1445" r:id="rId4322"/>
+    <hyperlink ref="B1446" r:id="rId4323"/>
+    <hyperlink ref="C1446" r:id="rId4324"/>
+    <hyperlink ref="E1446" r:id="rId4325"/>
+    <hyperlink ref="B1447" r:id="rId4326"/>
+    <hyperlink ref="C1447" r:id="rId4327"/>
+    <hyperlink ref="E1447" r:id="rId4328"/>
+    <hyperlink ref="B1448" r:id="rId4329"/>
+    <hyperlink ref="C1448" r:id="rId4330"/>
+    <hyperlink ref="E1448" r:id="rId4331"/>
+    <hyperlink ref="B1449" r:id="rId4332"/>
+    <hyperlink ref="C1449" r:id="rId4333"/>
+    <hyperlink ref="E1449" r:id="rId4334"/>
+    <hyperlink ref="B1450" r:id="rId4335"/>
+    <hyperlink ref="C1450" r:id="rId4336"/>
+    <hyperlink ref="E1450" r:id="rId4337"/>
+    <hyperlink ref="B1451" r:id="rId4338"/>
+    <hyperlink ref="C1451" r:id="rId4339"/>
+    <hyperlink ref="E1451" r:id="rId4340"/>
+    <hyperlink ref="B1452" r:id="rId4341"/>
+    <hyperlink ref="C1452" r:id="rId4342"/>
+    <hyperlink ref="E1452" r:id="rId4343"/>
+    <hyperlink ref="B1453" r:id="rId4344"/>
+    <hyperlink ref="C1453" r:id="rId4345"/>
+    <hyperlink ref="E1453" r:id="rId4346"/>
+    <hyperlink ref="B1454" r:id="rId4347"/>
+    <hyperlink ref="C1454" r:id="rId4348"/>
+    <hyperlink ref="E1454" r:id="rId4349"/>
+    <hyperlink ref="B1455" r:id="rId4350"/>
+    <hyperlink ref="C1455" r:id="rId4351"/>
+    <hyperlink ref="E1455" r:id="rId4352"/>
+    <hyperlink ref="B1456" r:id="rId4353"/>
+    <hyperlink ref="C1456" r:id="rId4354"/>
+    <hyperlink ref="E1456" r:id="rId4355"/>
+    <hyperlink ref="B1457" r:id="rId4356"/>
+    <hyperlink ref="C1457" r:id="rId4357"/>
+    <hyperlink ref="E1457" r:id="rId4358"/>
+    <hyperlink ref="B1458" r:id="rId4359"/>
+    <hyperlink ref="C1458" r:id="rId4360"/>
+    <hyperlink ref="E1458" r:id="rId4361"/>
+    <hyperlink ref="B1459" r:id="rId4362"/>
+    <hyperlink ref="C1459" r:id="rId4363"/>
+    <hyperlink ref="E1459" r:id="rId4364"/>
+    <hyperlink ref="B1460" r:id="rId4365"/>
+    <hyperlink ref="C1460" r:id="rId4366"/>
+    <hyperlink ref="E1460" r:id="rId4367"/>
+    <hyperlink ref="B1461" r:id="rId4368"/>
+    <hyperlink ref="C1461" r:id="rId4369"/>
+    <hyperlink ref="E1461" r:id="rId4370"/>
+    <hyperlink ref="B1462" r:id="rId4371"/>
+    <hyperlink ref="C1462" r:id="rId4372"/>
+    <hyperlink ref="E1462" r:id="rId4373"/>
+    <hyperlink ref="B1463" r:id="rId4374"/>
+    <hyperlink ref="C1463" r:id="rId4375"/>
+    <hyperlink ref="E1463" r:id="rId4376"/>
+    <hyperlink ref="B1464" r:id="rId4377"/>
+    <hyperlink ref="C1464" r:id="rId4378"/>
+    <hyperlink ref="E1464" r:id="rId4379"/>
+    <hyperlink ref="B1465" r:id="rId4380"/>
+    <hyperlink ref="C1465" r:id="rId4381"/>
+    <hyperlink ref="E1465" r:id="rId4382"/>
+    <hyperlink ref="B1466" r:id="rId4383"/>
+    <hyperlink ref="C1466" r:id="rId4384"/>
+    <hyperlink ref="E1466" r:id="rId4385"/>
+    <hyperlink ref="B1467" r:id="rId4386"/>
+    <hyperlink ref="C1467" r:id="rId4387"/>
+    <hyperlink ref="E1467" r:id="rId4388"/>
+    <hyperlink ref="B1468" r:id="rId4389"/>
+    <hyperlink ref="C1468" r:id="rId4390"/>
+    <hyperlink ref="E1468" r:id="rId4391"/>
+    <hyperlink ref="B1469" r:id="rId4392"/>
+    <hyperlink ref="C1469" r:id="rId4393"/>
+    <hyperlink ref="E1469" r:id="rId4394"/>
+    <hyperlink ref="B1470" r:id="rId4395"/>
+    <hyperlink ref="C1470" r:id="rId4396"/>
+    <hyperlink ref="E1470" r:id="rId4397"/>
+    <hyperlink ref="B1471" r:id="rId4398"/>
+    <hyperlink ref="C1471" r:id="rId4399"/>
+    <hyperlink ref="E1471" r:id="rId4400"/>
+    <hyperlink ref="B1472" r:id="rId4401"/>
+    <hyperlink ref="C1472" r:id="rId4402"/>
+    <hyperlink ref="E1472" r:id="rId4403"/>
+    <hyperlink ref="B1473" r:id="rId4404"/>
+    <hyperlink ref="C1473" r:id="rId4405"/>
+    <hyperlink ref="E1473" r:id="rId4406"/>
+    <hyperlink ref="B1474" r:id="rId4407"/>
+    <hyperlink ref="C1474" r:id="rId4408"/>
+    <hyperlink ref="E1474" r:id="rId4409"/>
+    <hyperlink ref="B1475" r:id="rId4410"/>
+    <hyperlink ref="C1475" r:id="rId4411"/>
+    <hyperlink ref="E1475" r:id="rId4412"/>
+    <hyperlink ref="B1476" r:id="rId4413"/>
+    <hyperlink ref="C1476" r:id="rId4414"/>
+    <hyperlink ref="E1476" r:id="rId4415"/>
+    <hyperlink ref="B1477" r:id="rId4416"/>
+    <hyperlink ref="C1477" r:id="rId4417"/>
+    <hyperlink ref="E1477" r:id="rId4418"/>
+    <hyperlink ref="B1478" r:id="rId4419"/>
+    <hyperlink ref="C1478" r:id="rId4420"/>
+    <hyperlink ref="E1478" r:id="rId4421"/>
+    <hyperlink ref="B1479" r:id="rId4422"/>
+    <hyperlink ref="C1479" r:id="rId4423"/>
+    <hyperlink ref="E1479" r:id="rId4424"/>
+    <hyperlink ref="B1480" r:id="rId4425"/>
+    <hyperlink ref="C1480" r:id="rId4426"/>
+    <hyperlink ref="E1480" r:id="rId4427"/>
+    <hyperlink ref="B1481" r:id="rId4428"/>
+    <hyperlink ref="C1481" r:id="rId4429"/>
+    <hyperlink ref="E1481" r:id="rId4430"/>
+    <hyperlink ref="B1482" r:id="rId4431"/>
+    <hyperlink ref="C1482" r:id="rId4432"/>
+    <hyperlink ref="E1482" r:id="rId4433"/>
+    <hyperlink ref="B1483" r:id="rId4434"/>
+    <hyperlink ref="C1483" r:id="rId4435"/>
+    <hyperlink ref="E1483" r:id="rId4436"/>
+    <hyperlink ref="B1484" r:id="rId4437"/>
+    <hyperlink ref="C1484" r:id="rId4438"/>
+    <hyperlink ref="E1484" r:id="rId4439"/>
+    <hyperlink ref="B1485" r:id="rId4440"/>
+    <hyperlink ref="C1485" r:id="rId4441"/>
+    <hyperlink ref="E1485" r:id="rId4442"/>
+    <hyperlink ref="B1486" r:id="rId4443"/>
+    <hyperlink ref="C1486" r:id="rId4444"/>
+    <hyperlink ref="E1486" r:id="rId4445"/>
+    <hyperlink ref="B1487" r:id="rId4446"/>
+    <hyperlink ref="C1487" r:id="rId4447"/>
+    <hyperlink ref="E1487" r:id="rId4448"/>
+    <hyperlink ref="B1488" r:id="rId4449"/>
+    <hyperlink ref="C1488" r:id="rId4450"/>
+    <hyperlink ref="E1488" r:id="rId4451" location="/"/>
+    <hyperlink ref="B1489" r:id="rId4452"/>
+    <hyperlink ref="C1489" r:id="rId4453"/>
+    <hyperlink ref="E1489" r:id="rId4454"/>
+    <hyperlink ref="B1490" r:id="rId4455"/>
+    <hyperlink ref="C1490" r:id="rId4456"/>
+    <hyperlink ref="E1490" r:id="rId4457"/>
+    <hyperlink ref="B1491" r:id="rId4458"/>
+    <hyperlink ref="C1491" r:id="rId4459"/>
+    <hyperlink ref="E1491" r:id="rId4460"/>
+    <hyperlink ref="B1492" r:id="rId4461"/>
+    <hyperlink ref="C1492" r:id="rId4462"/>
+    <hyperlink ref="E1492" r:id="rId4463"/>
+    <hyperlink ref="B1493" r:id="rId4464"/>
+    <hyperlink ref="C1493" r:id="rId4465"/>
+    <hyperlink ref="E1493" r:id="rId4466"/>
+    <hyperlink ref="B1494" r:id="rId4467"/>
+    <hyperlink ref="C1494" r:id="rId4468"/>
+    <hyperlink ref="E1494" r:id="rId4469"/>
+    <hyperlink ref="B1495" r:id="rId4470"/>
+    <hyperlink ref="C1495" r:id="rId4471"/>
+    <hyperlink ref="E1495" r:id="rId4472"/>
+    <hyperlink ref="B1496" r:id="rId4473"/>
+    <hyperlink ref="C1496" r:id="rId4474"/>
+    <hyperlink ref="E1496" r:id="rId4475"/>
+    <hyperlink ref="B1497" r:id="rId4476"/>
+    <hyperlink ref="C1497" r:id="rId4477"/>
+    <hyperlink ref="E1497" r:id="rId4478"/>
+    <hyperlink ref="B1498" r:id="rId4479"/>
+    <hyperlink ref="C1498" r:id="rId4480"/>
+    <hyperlink ref="E1498" r:id="rId4481"/>
+    <hyperlink ref="B1499" r:id="rId4482"/>
+    <hyperlink ref="C1499" r:id="rId4483"/>
+    <hyperlink ref="E1499" r:id="rId4484"/>
+    <hyperlink ref="B1500" r:id="rId4485"/>
+    <hyperlink ref="C1500" r:id="rId4486"/>
+    <hyperlink ref="E1500" r:id="rId4487"/>
+    <hyperlink ref="B1501" r:id="rId4488"/>
+    <hyperlink ref="C1501" r:id="rId4489"/>
+    <hyperlink ref="E1501" r:id="rId4490"/>
+    <hyperlink ref="B1502" r:id="rId4491"/>
+    <hyperlink ref="C1502" r:id="rId4492"/>
+    <hyperlink ref="E1502" r:id="rId4493"/>
+    <hyperlink ref="B1503" r:id="rId4494"/>
+    <hyperlink ref="C1503" r:id="rId4495"/>
+    <hyperlink ref="E1503" r:id="rId4496"/>
+    <hyperlink ref="B1504" r:id="rId4497"/>
+    <hyperlink ref="C1504" r:id="rId4498"/>
+    <hyperlink ref="E1504" r:id="rId4499"/>
+    <hyperlink ref="B1505" r:id="rId4500"/>
+    <hyperlink ref="C1505" r:id="rId4501"/>
+    <hyperlink ref="E1505" r:id="rId4502"/>
+    <hyperlink ref="B1506" r:id="rId4503"/>
+    <hyperlink ref="C1506" r:id="rId4504"/>
+    <hyperlink ref="E1506" r:id="rId4505"/>
+    <hyperlink ref="B1507" r:id="rId4506"/>
+    <hyperlink ref="C1507" r:id="rId4507"/>
+    <hyperlink ref="E1507" r:id="rId4508"/>
+    <hyperlink ref="B1508" r:id="rId4509"/>
+    <hyperlink ref="C1508" r:id="rId4510"/>
+    <hyperlink ref="E1508" r:id="rId4511"/>
+    <hyperlink ref="B1509" r:id="rId4512"/>
+    <hyperlink ref="C1509" r:id="rId4513"/>
+    <hyperlink ref="E1509" r:id="rId4514"/>
+    <hyperlink ref="B1510" r:id="rId4515"/>
+    <hyperlink ref="C1510" r:id="rId4516"/>
+    <hyperlink ref="E1510" r:id="rId4517"/>
+    <hyperlink ref="B1511" r:id="rId4518"/>
+    <hyperlink ref="C1511" r:id="rId4519"/>
+    <hyperlink ref="E1511" r:id="rId4520"/>
+    <hyperlink ref="B1512" r:id="rId4521"/>
+    <hyperlink ref="C1512" r:id="rId4522"/>
+    <hyperlink ref="E1512" r:id="rId4523"/>
+    <hyperlink ref="B1513" r:id="rId4524"/>
+    <hyperlink ref="C1513" r:id="rId4525"/>
+    <hyperlink ref="E1513" r:id="rId4526"/>
+    <hyperlink ref="B1514" r:id="rId4527"/>
+    <hyperlink ref="C1514" r:id="rId4528"/>
+    <hyperlink ref="E1514" r:id="rId4529"/>
+    <hyperlink ref="B1515" r:id="rId4530"/>
+    <hyperlink ref="C1515" r:id="rId4531"/>
+    <hyperlink ref="E1515" r:id="rId4532"/>
+    <hyperlink ref="B1516" r:id="rId4533"/>
+    <hyperlink ref="C1516" r:id="rId4534"/>
+    <hyperlink ref="E1516" r:id="rId4535"/>
+    <hyperlink ref="B1517" r:id="rId4536"/>
+    <hyperlink ref="C1517" r:id="rId4537"/>
+    <hyperlink ref="E1517" r:id="rId4538"/>
+    <hyperlink ref="B1518" r:id="rId4539"/>
+    <hyperlink ref="C1518" r:id="rId4540"/>
+    <hyperlink ref="E1518" r:id="rId4541"/>
+    <hyperlink ref="B1519" r:id="rId4542"/>
+    <hyperlink ref="C1519" r:id="rId4543"/>
+    <hyperlink ref="E1519" r:id="rId4544"/>
+    <hyperlink ref="B1520" r:id="rId4545"/>
+    <hyperlink ref="C1520" r:id="rId4546"/>
+    <hyperlink ref="E1520" r:id="rId4547"/>
+    <hyperlink ref="B1521" r:id="rId4548"/>
+    <hyperlink ref="C1521" r:id="rId4549"/>
+    <hyperlink ref="E1521" r:id="rId4550"/>
+    <hyperlink ref="B1522" r:id="rId4551"/>
+    <hyperlink ref="C1522" r:id="rId4552"/>
+    <hyperlink ref="E1522" r:id="rId4553"/>
+    <hyperlink ref="B1523" r:id="rId4554"/>
+    <hyperlink ref="C1523" r:id="rId4555"/>
+    <hyperlink ref="E1523" r:id="rId4556"/>
+    <hyperlink ref="B1524" r:id="rId4557"/>
+    <hyperlink ref="C1524" r:id="rId4558"/>
+    <hyperlink ref="E1524" r:id="rId4559"/>
+    <hyperlink ref="B1525" r:id="rId4560"/>
+    <hyperlink ref="C1525" r:id="rId4561"/>
+    <hyperlink ref="E1525" r:id="rId4562"/>
+    <hyperlink ref="B1526" r:id="rId4563"/>
+    <hyperlink ref="C1526" r:id="rId4564"/>
+    <hyperlink ref="E1526" r:id="rId4565"/>
+    <hyperlink ref="B1527" r:id="rId4566"/>
+    <hyperlink ref="C1527" r:id="rId4567"/>
+    <hyperlink ref="E1527" r:id="rId4568"/>
+    <hyperlink ref="B1528" r:id="rId4569"/>
+    <hyperlink ref="C1528" r:id="rId4570"/>
+    <hyperlink ref="E1528" r:id="rId4571"/>
+    <hyperlink ref="B1529" r:id="rId4572"/>
+    <hyperlink ref="C1529" r:id="rId4573"/>
+    <hyperlink ref="E1529" r:id="rId4574"/>
+    <hyperlink ref="B1530" r:id="rId4575"/>
+    <hyperlink ref="C1530" r:id="rId4576"/>
+    <hyperlink ref="E1530" r:id="rId4577"/>
+    <hyperlink ref="B1531" r:id="rId4578"/>
+    <hyperlink ref="C1531" r:id="rId4579"/>
+    <hyperlink ref="E1531" r:id="rId4580"/>
+    <hyperlink ref="B1532" r:id="rId4581"/>
+    <hyperlink ref="C1532" r:id="rId4582"/>
+    <hyperlink ref="E1532" r:id="rId4583"/>
+    <hyperlink ref="B1533" r:id="rId4584"/>
+    <hyperlink ref="C1533" r:id="rId4585"/>
+    <hyperlink ref="E1533" r:id="rId4586"/>
+    <hyperlink ref="B1534" r:id="rId4587"/>
+    <hyperlink ref="C1534" r:id="rId4588"/>
+    <hyperlink ref="E1534" r:id="rId4589"/>
+    <hyperlink ref="B1535" r:id="rId4590"/>
+    <hyperlink ref="C1535" r:id="rId4591"/>
+    <hyperlink ref="E1535" r:id="rId4592"/>
+    <hyperlink ref="B1536" r:id="rId4593"/>
+    <hyperlink ref="C1536" r:id="rId4594"/>
+    <hyperlink ref="E1536" r:id="rId4595"/>
+    <hyperlink ref="B1537" r:id="rId4596"/>
+    <hyperlink ref="C1537" r:id="rId4597"/>
+    <hyperlink ref="E1537" r:id="rId4598"/>
+    <hyperlink ref="B1538" r:id="rId4599"/>
+    <hyperlink ref="C1538" r:id="rId4600"/>
+    <hyperlink ref="E1538" r:id="rId4601"/>
+    <hyperlink ref="B1539" r:id="rId4602"/>
+    <hyperlink ref="C1539" r:id="rId4603"/>
+    <hyperlink ref="E1539" r:id="rId4604"/>
+    <hyperlink ref="B1540" r:id="rId4605"/>
+    <hyperlink ref="C1540" r:id="rId4606"/>
+    <hyperlink ref="E1540" r:id="rId4607"/>
+    <hyperlink ref="B1541" r:id="rId4608"/>
+    <hyperlink ref="C1541" r:id="rId4609"/>
+    <hyperlink ref="E1541" r:id="rId4610"/>
+    <hyperlink ref="B1542" r:id="rId4611"/>
+    <hyperlink ref="C1542" r:id="rId4612"/>
+    <hyperlink ref="E1542" r:id="rId4613"/>
+    <hyperlink ref="B1543" r:id="rId4614"/>
+    <hyperlink ref="C1543" r:id="rId4615"/>
+    <hyperlink ref="E1543" r:id="rId4616"/>
+    <hyperlink ref="B1544" r:id="rId4617"/>
+    <hyperlink ref="C1544" r:id="rId4618"/>
+    <hyperlink ref="E1544" r:id="rId4619"/>
+    <hyperlink ref="B1545" r:id="rId4620"/>
+    <hyperlink ref="C1545" r:id="rId4621"/>
+    <hyperlink ref="E1545" r:id="rId4622"/>
+    <hyperlink ref="B1546" r:id="rId4623"/>
+    <hyperlink ref="C1546" r:id="rId4624"/>
+    <hyperlink ref="E1546" r:id="rId4625"/>
+    <hyperlink ref="B1547" r:id="rId4626"/>
+    <hyperlink ref="C1547" r:id="rId4627"/>
+    <hyperlink ref="E1547" r:id="rId4628"/>
+    <hyperlink ref="B1548" r:id="rId4629"/>
+    <hyperlink ref="C1548" r:id="rId4630"/>
+    <hyperlink ref="E1548" r:id="rId4631"/>
+    <hyperlink ref="B1549" r:id="rId4632"/>
+    <hyperlink ref="C1549" r:id="rId4633"/>
+    <hyperlink ref="E1549" r:id="rId4634"/>
+    <hyperlink ref="B1550" r:id="rId4635"/>
+    <hyperlink ref="C1550" r:id="rId4636"/>
+    <hyperlink ref="E1550" r:id="rId4637"/>
+    <hyperlink ref="B1551" r:id="rId4638"/>
+    <hyperlink ref="C1551" r:id="rId4639"/>
+    <hyperlink ref="E1551" r:id="rId4640"/>
+    <hyperlink ref="B1552" r:id="rId4641"/>
+    <hyperlink ref="C1552" r:id="rId4642"/>
+    <hyperlink ref="E1552" r:id="rId4643"/>
+    <hyperlink ref="B1553" r:id="rId4644"/>
+    <hyperlink ref="C1553" r:id="rId4645"/>
+    <hyperlink ref="E1553" r:id="rId4646"/>
+    <hyperlink ref="B1554" r:id="rId4647"/>
+    <hyperlink ref="C1554" r:id="rId4648"/>
+    <hyperlink ref="E1554" r:id="rId4649" location="pullrequestreview-184181318"/>
+    <hyperlink ref="B1555" r:id="rId4650"/>
+    <hyperlink ref="C1555" r:id="rId4651"/>
+    <hyperlink ref="E1555" r:id="rId4652"/>
+    <hyperlink ref="B1556" r:id="rId4653"/>
+    <hyperlink ref="C1556" r:id="rId4654"/>
+    <hyperlink ref="E1556" r:id="rId4655"/>
+    <hyperlink ref="B1557" r:id="rId4656"/>
+    <hyperlink ref="C1557" r:id="rId4657"/>
+    <hyperlink ref="E1557" r:id="rId4658"/>
+    <hyperlink ref="B1558" r:id="rId4659"/>
+    <hyperlink ref="C1558" r:id="rId4660"/>
+    <hyperlink ref="E1558" r:id="rId4661"/>
+    <hyperlink ref="B1559" r:id="rId4662"/>
+    <hyperlink ref="C1559" r:id="rId4663"/>
+    <hyperlink ref="E1559" r:id="rId4664"/>
+    <hyperlink ref="B1560" r:id="rId4665"/>
+    <hyperlink ref="C1560" r:id="rId4666"/>
+    <hyperlink ref="E1560" r:id="rId4667"/>
+    <hyperlink ref="B1561" r:id="rId4668"/>
+    <hyperlink ref="C1561" r:id="rId4669"/>
+    <hyperlink ref="E1561" r:id="rId4670"/>
+    <hyperlink ref="B1562" r:id="rId4671"/>
+    <hyperlink ref="C1562" r:id="rId4672"/>
+    <hyperlink ref="E1562" r:id="rId4673"/>
+    <hyperlink ref="B1563" r:id="rId4674"/>
+    <hyperlink ref="C1563" r:id="rId4675"/>
+    <hyperlink ref="E1563" r:id="rId4676"/>
+    <hyperlink ref="B1564" r:id="rId4677"/>
+    <hyperlink ref="C1564" r:id="rId4678"/>
+    <hyperlink ref="E1564" r:id="rId4679"/>
+    <hyperlink ref="B1565" r:id="rId4680"/>
+    <hyperlink ref="C1565" r:id="rId4681"/>
+    <hyperlink ref="E1565" r:id="rId4682"/>
+    <hyperlink ref="B1566" r:id="rId4683"/>
+    <hyperlink ref="C1566" r:id="rId4684"/>
+    <hyperlink ref="E1566" r:id="rId4685"/>
+    <hyperlink ref="B1567" r:id="rId4686"/>
+    <hyperlink ref="C1567" r:id="rId4687"/>
+    <hyperlink ref="E1567" r:id="rId4688"/>
+    <hyperlink ref="B1568" r:id="rId4689"/>
+    <hyperlink ref="C1568" r:id="rId4690"/>
+    <hyperlink ref="E1568" r:id="rId4691"/>
+    <hyperlink ref="B1569" r:id="rId4692"/>
+    <hyperlink ref="C1569" r:id="rId4693"/>
+    <hyperlink ref="E1569" r:id="rId4694"/>
+    <hyperlink ref="B1570" r:id="rId4695"/>
+    <hyperlink ref="C1570" r:id="rId4696"/>
+    <hyperlink ref="E1570" r:id="rId4697" location="event-2016722433"/>
+    <hyperlink ref="B1571" r:id="rId4698"/>
+    <hyperlink ref="C1571" r:id="rId4699"/>
+    <hyperlink ref="E1571" r:id="rId4700"/>
+    <hyperlink ref="B1572" r:id="rId4701"/>
+    <hyperlink ref="C1572" r:id="rId4702"/>
+    <hyperlink ref="E1572" r:id="rId4703"/>
+    <hyperlink ref="B1573" r:id="rId4704"/>
+    <hyperlink ref="C1573" r:id="rId4705"/>
+    <hyperlink ref="E1573" r:id="rId4706"/>
+    <hyperlink ref="B1574" r:id="rId4707"/>
+    <hyperlink ref="C1574" r:id="rId4708"/>
+    <hyperlink ref="E1574" r:id="rId4709"/>
+    <hyperlink ref="B1575" r:id="rId4710"/>
+    <hyperlink ref="C1575" r:id="rId4711"/>
+    <hyperlink ref="E1575" r:id="rId4712"/>
+    <hyperlink ref="B1576" r:id="rId4713"/>
+    <hyperlink ref="C1576" r:id="rId4714"/>
+    <hyperlink ref="E1576" r:id="rId4715"/>
+    <hyperlink ref="B1577" r:id="rId4716"/>
+    <hyperlink ref="C1577" r:id="rId4717"/>
+    <hyperlink ref="E1577" r:id="rId4718"/>
+    <hyperlink ref="B1578" r:id="rId4719"/>
+    <hyperlink ref="C1578" r:id="rId4720"/>
+    <hyperlink ref="E1578" r:id="rId4721"/>
+    <hyperlink ref="B1579" r:id="rId4722"/>
+    <hyperlink ref="C1579" r:id="rId4723"/>
+    <hyperlink ref="E1579" r:id="rId4724"/>
+    <hyperlink ref="B1580" r:id="rId4725"/>
+    <hyperlink ref="C1580" r:id="rId4726"/>
+    <hyperlink ref="E1580" r:id="rId4727"/>
+    <hyperlink ref="B1581" r:id="rId4728"/>
+    <hyperlink ref="C1581" r:id="rId4729"/>
+    <hyperlink ref="E1581" r:id="rId4730"/>
+    <hyperlink ref="B1582" r:id="rId4731"/>
+    <hyperlink ref="C1582" r:id="rId4732"/>
+    <hyperlink ref="E1582" r:id="rId4733"/>
+    <hyperlink ref="B1583" r:id="rId4734"/>
+    <hyperlink ref="C1583" r:id="rId4735"/>
+    <hyperlink ref="E1583" r:id="rId4736"/>
+    <hyperlink ref="B1584" r:id="rId4737"/>
+    <hyperlink ref="C1584" r:id="rId4738"/>
+    <hyperlink ref="E1584" r:id="rId4739"/>
+    <hyperlink ref="B1585" r:id="rId4740"/>
+    <hyperlink ref="C1585" r:id="rId4741"/>
+    <hyperlink ref="E1585" r:id="rId4742"/>
+    <hyperlink ref="B1586" r:id="rId4743"/>
+    <hyperlink ref="C1586" r:id="rId4744"/>
+    <hyperlink ref="E1586" r:id="rId4745"/>
+    <hyperlink ref="B1587" r:id="rId4746"/>
+    <hyperlink ref="C1587" r:id="rId4747"/>
+    <hyperlink ref="E1587" r:id="rId4748"/>
+    <hyperlink ref="B1588" r:id="rId4749"/>
+    <hyperlink ref="C1588" r:id="rId4750"/>
+    <hyperlink ref="E1588" r:id="rId4751"/>
+    <hyperlink ref="B1589" r:id="rId4752"/>
+    <hyperlink ref="C1589" r:id="rId4753"/>
+    <hyperlink ref="E1589" r:id="rId4754"/>
+    <hyperlink ref="B1590" r:id="rId4755"/>
+    <hyperlink ref="C1590" r:id="rId4756"/>
+    <hyperlink ref="E1590" r:id="rId4757"/>
+    <hyperlink ref="B1591" r:id="rId4758"/>
+    <hyperlink ref="C1591" r:id="rId4759"/>
+    <hyperlink ref="E1591" r:id="rId4760"/>
+    <hyperlink ref="B1592" r:id="rId4761"/>
+    <hyperlink ref="C1592" r:id="rId4762"/>
+    <hyperlink ref="E1592" r:id="rId4763"/>
+    <hyperlink ref="B1593" r:id="rId4764"/>
+    <hyperlink ref="C1593" r:id="rId4765"/>
+    <hyperlink ref="E1593" r:id="rId4766"/>
+    <hyperlink ref="B1594" r:id="rId4767"/>
+    <hyperlink ref="C1594" r:id="rId4768"/>
+    <hyperlink ref="E1594" r:id="rId4769"/>
+    <hyperlink ref="B1595" r:id="rId4770"/>
+    <hyperlink ref="C1595" r:id="rId4771"/>
+    <hyperlink ref="E1595" r:id="rId4772"/>
+    <hyperlink ref="B1596" r:id="rId4773"/>
+    <hyperlink ref="C1596" r:id="rId4774"/>
+    <hyperlink ref="E1596" r:id="rId4775"/>
+    <hyperlink ref="B1597" r:id="rId4776"/>
+    <hyperlink ref="C1597" r:id="rId4777"/>
+    <hyperlink ref="E1597" r:id="rId4778"/>
+    <hyperlink ref="B1598" r:id="rId4779"/>
+    <hyperlink ref="C1598" r:id="rId4780"/>
+    <hyperlink ref="E1598" r:id="rId4781"/>
+    <hyperlink ref="B1599" r:id="rId4782"/>
+    <hyperlink ref="C1599" r:id="rId4783"/>
+    <hyperlink ref="E1599" r:id="rId4784"/>
+    <hyperlink ref="B1600" r:id="rId4785"/>
+    <hyperlink ref="C1600" r:id="rId4786"/>
+    <hyperlink ref="E1600" r:id="rId4787"/>
+    <hyperlink ref="B1601" r:id="rId4788"/>
+    <hyperlink ref="C1601" r:id="rId4789"/>
+    <hyperlink ref="E1601" r:id="rId4790"/>
+    <hyperlink ref="B1602" r:id="rId4791"/>
+    <hyperlink ref="C1602" r:id="rId4792"/>
+    <hyperlink ref="E1602" r:id="rId4793"/>
+    <hyperlink ref="B1603" r:id="rId4794"/>
+    <hyperlink ref="C1603" r:id="rId4795"/>
+    <hyperlink ref="E1603" r:id="rId4796"/>
+    <hyperlink ref="B1604" r:id="rId4797"/>
+    <hyperlink ref="C1604" r:id="rId4798"/>
+    <hyperlink ref="E1604" r:id="rId4799"/>
+    <hyperlink ref="B1605" r:id="rId4800"/>
+    <hyperlink ref="C1605" r:id="rId4801"/>
+    <hyperlink ref="E1605" r:id="rId4802"/>
+    <hyperlink ref="B1606" r:id="rId4803"/>
+    <hyperlink ref="C1606" r:id="rId4804"/>
+    <hyperlink ref="E1606" r:id="rId4805"/>
+    <hyperlink ref="B1607" r:id="rId4806"/>
+    <hyperlink ref="C1607" r:id="rId4807"/>
+    <hyperlink ref="E1607" r:id="rId4808"/>
+    <hyperlink ref="B1608" r:id="rId4809"/>
+    <hyperlink ref="C1608" r:id="rId4810"/>
+    <hyperlink ref="E1608" r:id="rId4811"/>
+    <hyperlink ref="B1609" r:id="rId4812"/>
+    <hyperlink ref="C1609" r:id="rId4813"/>
+    <hyperlink ref="E1609" r:id="rId4814"/>
+    <hyperlink ref="B1610" r:id="rId4815"/>
+    <hyperlink ref="C1610" r:id="rId4816"/>
+    <hyperlink ref="E1610" r:id="rId4817"/>
+    <hyperlink ref="B1611" r:id="rId4818"/>
+    <hyperlink ref="C1611" r:id="rId4819"/>
+    <hyperlink ref="E1611" r:id="rId4820"/>
+    <hyperlink ref="B1612" r:id="rId4821"/>
+    <hyperlink ref="C1612" r:id="rId4822"/>
+    <hyperlink ref="E1612" r:id="rId4823"/>
+    <hyperlink ref="B1613" r:id="rId4824"/>
+    <hyperlink ref="C1613" r:id="rId4825"/>
+    <hyperlink ref="E1613" r:id="rId4826"/>
+    <hyperlink ref="B1614" r:id="rId4827"/>
+    <hyperlink ref="C1614" r:id="rId4828"/>
+    <hyperlink ref="E1614" r:id="rId4829"/>
+    <hyperlink ref="B1615" r:id="rId4830"/>
+    <hyperlink ref="C1615" r:id="rId4831"/>
+    <hyperlink ref="E1615" r:id="rId4832" location="gid=0"/>
+    <hyperlink ref="B1616" r:id="rId4833"/>
+    <hyperlink ref="C1616" r:id="rId4834"/>
+    <hyperlink ref="E1616" r:id="rId4835" location="gid=0"/>
+    <hyperlink ref="B1617" r:id="rId4836"/>
+    <hyperlink ref="C1617" r:id="rId4837"/>
+    <hyperlink ref="E1617" r:id="rId4838" location="gid=0"/>
+    <hyperlink ref="B1618" r:id="rId4839"/>
+    <hyperlink ref="C1618" r:id="rId4840"/>
+    <hyperlink ref="E1618" r:id="rId4841" location="gid=0"/>
+    <hyperlink ref="B1619" r:id="rId4842"/>
+    <hyperlink ref="C1619" r:id="rId4843"/>
+    <hyperlink ref="E1619" r:id="rId4844"/>
+    <hyperlink ref="B1620" r:id="rId4845"/>
+    <hyperlink ref="C1620" r:id="rId4846"/>
+    <hyperlink ref="E1620" r:id="rId4847" location="gid=0"/>
+    <hyperlink ref="B1621" r:id="rId4848"/>
+    <hyperlink ref="C1621" r:id="rId4849"/>
+    <hyperlink ref="E1621" r:id="rId4850" location="gid=0"/>
+    <hyperlink ref="B1622" r:id="rId4851"/>
+    <hyperlink ref="C1622" r:id="rId4852"/>
+    <hyperlink ref="E1622" r:id="rId4853" location="gid=0"/>
+    <hyperlink ref="B1623" r:id="rId4854"/>
+    <hyperlink ref="C1623" r:id="rId4855"/>
+    <hyperlink ref="E1623" r:id="rId4856" location="gid=0"/>
+    <hyperlink ref="B1624" r:id="rId4857"/>
+    <hyperlink ref="C1624" r:id="rId4858"/>
+    <hyperlink ref="E1624" r:id="rId4859" location="gid=0"/>
+    <hyperlink ref="B1625" r:id="rId4860"/>
+    <hyperlink ref="C1625" r:id="rId4861"/>
+    <hyperlink ref="E1625" r:id="rId4862" location="gid=0"/>
+    <hyperlink ref="B1626" r:id="rId4863"/>
+    <hyperlink ref="C1626" r:id="rId4864"/>
+    <hyperlink ref="E1626" r:id="rId4865"/>
+    <hyperlink ref="B1627" r:id="rId4866"/>
+    <hyperlink ref="C1627" r:id="rId4867"/>
+    <hyperlink ref="E1627" r:id="rId4868"/>
+    <hyperlink ref="B1628" r:id="rId4869"/>
+    <hyperlink ref="C1628" r:id="rId4870"/>
+    <hyperlink ref="E1628" r:id="rId4871"/>
+    <hyperlink ref="B1629" r:id="rId4872"/>
+    <hyperlink ref="C1629" r:id="rId4873"/>
+    <hyperlink ref="E1629" r:id="rId4874"/>
+    <hyperlink ref="B1630" r:id="rId4875"/>
+    <hyperlink ref="C1630" r:id="rId4876"/>
+    <hyperlink ref="E1630" r:id="rId4877"/>
+    <hyperlink ref="B1631" r:id="rId4878"/>
+    <hyperlink ref="C1631" r:id="rId4879"/>
+    <hyperlink ref="E1631" r:id="rId4880"/>
+    <hyperlink ref="B1632" r:id="rId4881"/>
+    <hyperlink ref="C1632" r:id="rId4882"/>
+    <hyperlink ref="E1632" r:id="rId4883"/>
+    <hyperlink ref="B1633" r:id="rId4884"/>
+    <hyperlink ref="C1633" r:id="rId4885"/>
+    <hyperlink ref="E1633" r:id="rId4886"/>
+    <hyperlink ref="B1634" r:id="rId4887"/>
+    <hyperlink ref="C1634" r:id="rId4888"/>
+    <hyperlink ref="E1634" r:id="rId4889"/>
+    <hyperlink ref="B1635" r:id="rId4890"/>
+    <hyperlink ref="C1635" r:id="rId4891"/>
+    <hyperlink ref="E1635" r:id="rId4892"/>
+    <hyperlink ref="B1636" r:id="rId4893"/>
+    <hyperlink ref="C1636" r:id="rId4894"/>
+    <hyperlink ref="E1636" r:id="rId4895"/>
+    <hyperlink ref="B1637" r:id="rId4896"/>
+    <hyperlink ref="C1637" r:id="rId4897"/>
+    <hyperlink ref="E1637" r:id="rId4898"/>
+    <hyperlink ref="B1638" r:id="rId4899"/>
+    <hyperlink ref="C1638" r:id="rId4900"/>
+    <hyperlink ref="E1638" r:id="rId4901"/>
+    <hyperlink ref="B1639" r:id="rId4902"/>
+    <hyperlink ref="C1639" r:id="rId4903"/>
+    <hyperlink ref="E1639" r:id="rId4904"/>
+    <hyperlink ref="B1640" r:id="rId4905"/>
+    <hyperlink ref="C1640" r:id="rId4906"/>
+    <hyperlink ref="E1640" r:id="rId4907"/>
+    <hyperlink ref="B1641" r:id="rId4908"/>
+    <hyperlink ref="C1641" r:id="rId4909"/>
+    <hyperlink ref="E1641" r:id="rId4910"/>
+    <hyperlink ref="B1642" r:id="rId4911"/>
+    <hyperlink ref="C1642" r:id="rId4912"/>
+    <hyperlink ref="E1642" r:id="rId4913"/>
+    <hyperlink ref="B1643" r:id="rId4914"/>
+    <hyperlink ref="C1643" r:id="rId4915"/>
+    <hyperlink ref="E1643" r:id="rId4916"/>
+    <hyperlink ref="B1644" r:id="rId4917"/>
+    <hyperlink ref="C1644" r:id="rId4918"/>
+    <hyperlink ref="E1644" r:id="rId4919"/>
+    <hyperlink ref="B1645" r:id="rId4920"/>
+    <hyperlink ref="C1645" r:id="rId4921"/>
+    <hyperlink ref="E1645" r:id="rId4922"/>
+    <hyperlink ref="B1646" r:id="rId4923"/>
+    <hyperlink ref="C1646" r:id="rId4924"/>
+    <hyperlink ref="E1646" r:id="rId4925"/>
+    <hyperlink ref="B1647" r:id="rId4926"/>
+    <hyperlink ref="C1647" r:id="rId4927"/>
+    <hyperlink ref="E1647" r:id="rId4928"/>
+    <hyperlink ref="B1648" r:id="rId4929"/>
+    <hyperlink ref="C1648" r:id="rId4930"/>
+    <hyperlink ref="E1648" r:id="rId4931"/>
+    <hyperlink ref="B1649" r:id="rId4932"/>
+    <hyperlink ref="C1649" r:id="rId4933"/>
+    <hyperlink ref="E1649" r:id="rId4934"/>
+    <hyperlink ref="B1650" r:id="rId4935"/>
+    <hyperlink ref="C1650" r:id="rId4936"/>
+    <hyperlink ref="E1650" r:id="rId4937"/>
+    <hyperlink ref="B1651" r:id="rId4938"/>
+    <hyperlink ref="C1651" r:id="rId4939"/>
+    <hyperlink ref="E1651" r:id="rId4940"/>
+    <hyperlink ref="B1652" r:id="rId4941"/>
+    <hyperlink ref="C1652" r:id="rId4942"/>
+    <hyperlink ref="E1652" r:id="rId4943"/>
+    <hyperlink ref="B1653" r:id="rId4944"/>
+    <hyperlink ref="C1653" r:id="rId4945"/>
+    <hyperlink ref="E1653" r:id="rId4946"/>
+    <hyperlink ref="B1654" r:id="rId4947"/>
+    <hyperlink ref="C1654" r:id="rId4948"/>
+    <hyperlink ref="E1654" r:id="rId4949"/>
+    <hyperlink ref="B1655" r:id="rId4950"/>
+    <hyperlink ref="C1655" r:id="rId4951"/>
+    <hyperlink ref="E1655" r:id="rId4952"/>
+    <hyperlink ref="B1656" r:id="rId4953"/>
+    <hyperlink ref="C1656" r:id="rId4954"/>
+    <hyperlink ref="E1656" r:id="rId4955"/>
+    <hyperlink ref="B1657" r:id="rId4956"/>
+    <hyperlink ref="C1657" r:id="rId4957"/>
+    <hyperlink ref="E1657" r:id="rId4958"/>
+    <hyperlink ref="B1658" r:id="rId4959"/>
+    <hyperlink ref="C1658" r:id="rId4960"/>
+    <hyperlink ref="E1658" r:id="rId4961"/>
+    <hyperlink ref="B1659" r:id="rId4962"/>
+    <hyperlink ref="C1659" r:id="rId4963"/>
+    <hyperlink ref="E1659" r:id="rId4964"/>
+    <hyperlink ref="B1660" r:id="rId4965"/>
+    <hyperlink ref="C1660" r:id="rId4966"/>
+    <hyperlink ref="E1660" r:id="rId4967"/>
+    <hyperlink ref="B1661" r:id="rId4968"/>
+    <hyperlink ref="C1661" r:id="rId4969"/>
+    <hyperlink ref="E1661" r:id="rId4970"/>
+    <hyperlink ref="B1662" r:id="rId4971"/>
+    <hyperlink ref="C1662" r:id="rId4972"/>
+    <hyperlink ref="E1662" r:id="rId4973"/>
+    <hyperlink ref="B1663" r:id="rId4974"/>
+    <hyperlink ref="C1663" r:id="rId4975"/>
+    <hyperlink ref="E1663" r:id="rId4976"/>
+    <hyperlink ref="B1664" r:id="rId4977"/>
+    <hyperlink ref="C1664" r:id="rId4978"/>
+    <hyperlink ref="E1664" r:id="rId4979"/>
+    <hyperlink ref="B1665" r:id="rId4980"/>
+    <hyperlink ref="C1665" r:id="rId4981"/>
+    <hyperlink ref="E1665" r:id="rId4982"/>
+    <hyperlink ref="B1666" r:id="rId4983"/>
+    <hyperlink ref="C1666" r:id="rId4984"/>
+    <hyperlink ref="E1666" r:id="rId4985"/>
+    <hyperlink ref="B1667" r:id="rId4986"/>
+    <hyperlink ref="C1667" r:id="rId4987"/>
+    <hyperlink ref="E1667" r:id="rId4988"/>
+    <hyperlink ref="B1668" r:id="rId4989"/>
+    <hyperlink ref="C1668" r:id="rId4990"/>
+    <hyperlink ref="E1668" r:id="rId4991"/>
+    <hyperlink ref="B1669" r:id="rId4992"/>
+    <hyperlink ref="C1669" r:id="rId4993"/>
+    <hyperlink ref="E1669" r:id="rId4994"/>
+    <hyperlink ref="B1670" r:id="rId4995"/>
+    <hyperlink ref="C1670" r:id="rId4996"/>
+    <hyperlink ref="E1670" r:id="rId4997"/>
+    <hyperlink ref="B1671" r:id="rId4998"/>
+    <hyperlink ref="C1671" r:id="rId4999"/>
+    <hyperlink ref="E1671" r:id="rId5000"/>
+    <hyperlink ref="B1672" r:id="rId5001"/>
+    <hyperlink ref="C1672" r:id="rId5002"/>
+    <hyperlink ref="E1672" r:id="rId5003"/>
+    <hyperlink ref="B1673" r:id="rId5004"/>
+    <hyperlink ref="C1673" r:id="rId5005"/>
+    <hyperlink ref="E1673" r:id="rId5006"/>
+    <hyperlink ref="B1674" r:id="rId5007"/>
+    <hyperlink ref="C1674" r:id="rId5008"/>
+    <hyperlink ref="E1674" r:id="rId5009"/>
+    <hyperlink ref="B1675" r:id="rId5010"/>
+    <hyperlink ref="C1675" r:id="rId5011"/>
+    <hyperlink ref="E1675" r:id="rId5012"/>
+    <hyperlink ref="B1676" r:id="rId5013"/>
+    <hyperlink ref="C1676" r:id="rId5014"/>
+    <hyperlink ref="E1676" r:id="rId5015"/>
+    <hyperlink ref="B1677" r:id="rId5016"/>
+    <hyperlink ref="C1677" r:id="rId5017"/>
+    <hyperlink ref="E1677" r:id="rId5018"/>
+    <hyperlink ref="B1678" r:id="rId5019"/>
+    <hyperlink ref="C1678" r:id="rId5020"/>
+    <hyperlink ref="E1678" r:id="rId5021"/>
+    <hyperlink ref="B1679" r:id="rId5022"/>
+    <hyperlink ref="C1679" r:id="rId5023"/>
+    <hyperlink ref="E1679" r:id="rId5024"/>
+    <hyperlink ref="B1680" r:id="rId5025"/>
+    <hyperlink ref="C1680" r:id="rId5026"/>
+    <hyperlink ref="E1680" r:id="rId5027"/>
+    <hyperlink ref="B1681" r:id="rId5028"/>
+    <hyperlink ref="C1681" r:id="rId5029"/>
+    <hyperlink ref="E1681" r:id="rId5030"/>
+    <hyperlink ref="B1682" r:id="rId5031"/>
+    <hyperlink ref="C1682" r:id="rId5032"/>
+    <hyperlink ref="E1682" r:id="rId5033"/>
+    <hyperlink ref="B1683" r:id="rId5034"/>
+    <hyperlink ref="C1683" r:id="rId5035"/>
+    <hyperlink ref="E1683" r:id="rId5036"/>
+    <hyperlink ref="B1684" r:id="rId5037"/>
+    <hyperlink ref="C1684" r:id="rId5038"/>
+    <hyperlink ref="E1684" r:id="rId5039"/>
+    <hyperlink ref="B1685" r:id="rId5040"/>
+    <hyperlink ref="C1685" r:id="rId5041"/>
+    <hyperlink ref="E1685" r:id="rId5042"/>
+    <hyperlink ref="B1686" r:id="rId5043"/>
+    <hyperlink ref="C1686" r:id="rId5044"/>
+    <hyperlink ref="E1686" r:id="rId5045"/>
+    <hyperlink ref="B1687" r:id="rId5046"/>
+    <hyperlink ref="C1687" r:id="rId5047"/>
+    <hyperlink ref="E1687" r:id="rId5048"/>
+    <hyperlink ref="B1688" r:id="rId5049"/>
+    <hyperlink ref="C1688" r:id="rId5050"/>
+    <hyperlink ref="E1688" r:id="rId5051"/>
+    <hyperlink ref="B1689" r:id="rId5052"/>
+    <hyperlink ref="C1689" r:id="rId5053"/>
+    <hyperlink ref="E1689" r:id="rId5054"/>
+    <hyperlink ref="B1690" r:id="rId5055"/>
+    <hyperlink ref="C1690" r:id="rId5056"/>
+    <hyperlink ref="E1690" r:id="rId5057"/>
+    <hyperlink ref="B1691" r:id="rId5058"/>
+    <hyperlink ref="C1691" r:id="rId5059"/>
+    <hyperlink ref="E1691" r:id="rId5060"/>
+    <hyperlink ref="B1692" r:id="rId5061"/>
+    <hyperlink ref="C1692" r:id="rId5062"/>
+    <hyperlink ref="E1692" r:id="rId5063"/>
+    <hyperlink ref="B1693" r:id="rId5064"/>
+    <hyperlink ref="C1693" r:id="rId5065"/>
+    <hyperlink ref="E1693" r:id="rId5066"/>
+    <hyperlink ref="B1694" r:id="rId5067"/>
+    <hyperlink ref="C1694" r:id="rId5068"/>
+    <hyperlink ref="E1694" r:id="rId5069"/>
+    <hyperlink ref="B1695" r:id="rId5070"/>
+    <hyperlink ref="C1695" r:id="rId5071"/>
+    <hyperlink ref="E1695" r:id="rId5072"/>
+    <hyperlink ref="B1696" r:id="rId5073"/>
+    <hyperlink ref="C1696" r:id="rId5074"/>
+    <hyperlink ref="E1696" r:id="rId5075"/>
+    <hyperlink ref="B1697" r:id="rId5076"/>
+    <hyperlink ref="C1697" r:id="rId5077"/>
+    <hyperlink ref="E1697" r:id="rId5078"/>
+    <hyperlink ref="B1698" r:id="rId5079"/>
+    <hyperlink ref="C1698" r:id="rId5080"/>
+    <hyperlink ref="E1698" r:id="rId5081"/>
+    <hyperlink ref="B1699" r:id="rId5082"/>
+    <hyperlink ref="C1699" r:id="rId5083"/>
+    <hyperlink ref="E1699" r:id="rId5084"/>
+    <hyperlink ref="B1700" r:id="rId5085"/>
+    <hyperlink ref="C1700" r:id="rId5086"/>
+    <hyperlink ref="E1700" r:id="rId5087"/>
+    <hyperlink ref="B1701" r:id="rId5088"/>
+    <hyperlink ref="C1701" r:id="rId5089"/>
+    <hyperlink ref="E1701" r:id="rId5090"/>
+    <hyperlink ref="B1702" r:id="rId5091"/>
+    <hyperlink ref="C1702" r:id="rId5092"/>
+    <hyperlink ref="E1702" r:id="rId5093"/>
+    <hyperlink ref="B1703" r:id="rId5094"/>
+    <hyperlink ref="C1703" r:id="rId5095"/>
+    <hyperlink ref="E1703" r:id="rId5096"/>
+    <hyperlink ref="B1704" r:id="rId5097"/>
+    <hyperlink ref="C1704" r:id="rId5098"/>
+    <hyperlink ref="E1704" r:id="rId5099"/>
+    <hyperlink ref="B1705" r:id="rId5100"/>
+    <hyperlink ref="C1705" r:id="rId5101"/>
+    <hyperlink ref="E1705" r:id="rId5102"/>
+    <hyperlink ref="B1706" r:id="rId5103"/>
+    <hyperlink ref="C1706" r:id="rId5104"/>
+    <hyperlink ref="E1706" r:id="rId5105"/>
+    <hyperlink ref="B1707" r:id="rId5106"/>
+    <hyperlink ref="C1707" r:id="rId5107"/>
+    <hyperlink ref="E1707" r:id="rId5108"/>
+    <hyperlink ref="B1708" r:id="rId5109"/>
+    <hyperlink ref="C1708" r:id="rId5110"/>
+    <hyperlink ref="E1708" r:id="rId5111"/>
+    <hyperlink ref="B1709" r:id="rId5112"/>
+    <hyperlink ref="C1709" r:id="rId5113"/>
+    <hyperlink ref="E1709" r:id="rId5114"/>
+    <hyperlink ref="B1710" r:id="rId5115"/>
+    <hyperlink ref="C1710" r:id="rId5116"/>
+    <hyperlink ref="E1710" r:id="rId5117"/>
+    <hyperlink ref="B1711" r:id="rId5118"/>
+    <hyperlink ref="C1711" r:id="rId5119"/>
+    <hyperlink ref="E1711" r:id="rId5120"/>
+    <hyperlink ref="B1712" r:id="rId5121"/>
+    <hyperlink ref="C1712" r:id="rId5122"/>
+    <hyperlink ref="E1712" r:id="rId5123"/>
+    <hyperlink ref="B1713" r:id="rId5124"/>
+    <hyperlink ref="C1713" r:id="rId5125"/>
+    <hyperlink ref="E1713" r:id="rId5126"/>
+    <hyperlink ref="B1714" r:id="rId5127"/>
+    <hyperlink ref="C1714" r:id="rId5128"/>
+    <hyperlink ref="E1714" r:id="rId5129"/>
+    <hyperlink ref="B1715" r:id="rId5130"/>
+    <hyperlink ref="C1715" r:id="rId5131"/>
+    <hyperlink ref="E1715" r:id="rId5132"/>
+    <hyperlink ref="B1716" r:id="rId5133"/>
+    <hyperlink ref="C1716" r:id="rId5134"/>
+    <hyperlink ref="E1716" r:id="rId5135"/>
+    <hyperlink ref="B1717" r:id="rId5136"/>
+    <hyperlink ref="C1717" r:id="rId5137"/>
+    <hyperlink ref="E1717" r:id="rId5138"/>
+    <hyperlink ref="B1718" r:id="rId5139"/>
+    <hyperlink ref="C1718" r:id="rId5140"/>
+    <hyperlink ref="E1718" r:id="rId5141"/>
+    <hyperlink ref="B1719" r:id="rId5142"/>
+    <hyperlink ref="C1719" r:id="rId5143"/>
+    <hyperlink ref="E1719" r:id="rId5144"/>
+    <hyperlink ref="B1720" r:id="rId5145"/>
+    <hyperlink ref="C1720" r:id="rId5146"/>
+    <hyperlink ref="E1720" r:id="rId5147"/>
+    <hyperlink ref="B1721" r:id="rId5148"/>
+    <hyperlink ref="C1721" r:id="rId5149"/>
+    <hyperlink ref="E1721" r:id="rId5150"/>
+    <hyperlink ref="B1722" r:id="rId5151"/>
+    <hyperlink ref="C1722" r:id="rId5152"/>
+    <hyperlink ref="E1722" r:id="rId5153"/>
+    <hyperlink ref="B1723" r:id="rId5154"/>
+    <hyperlink ref="C1723" r:id="rId5155"/>
+    <hyperlink ref="E1723" r:id="rId5156"/>
+    <hyperlink ref="B1724" r:id="rId5157"/>
+    <hyperlink ref="C1724" r:id="rId5158"/>
+    <hyperlink ref="E1724" r:id="rId5159"/>
+    <hyperlink ref="B1725" r:id="rId5160"/>
+    <hyperlink ref="C1725" r:id="rId5161"/>
+    <hyperlink ref="E1725" r:id="rId5162"/>
+    <hyperlink ref="B1726" r:id="rId5163"/>
+    <hyperlink ref="C1726" r:id="rId5164"/>
+    <hyperlink ref="E1726" r:id="rId5165"/>
+    <hyperlink ref="B1727" r:id="rId5166"/>
+    <hyperlink ref="C1727" r:id="rId5167"/>
+    <hyperlink ref="E1727" r:id="rId5168"/>
+    <hyperlink ref="B1728" r:id="rId5169"/>
+    <hyperlink ref="C1728" r:id="rId5170"/>
+    <hyperlink ref="E1728" r:id="rId5171"/>
+    <hyperlink ref="B1729" r:id="rId5172"/>
+    <hyperlink ref="C1729" r:id="rId5173"/>
+    <hyperlink ref="E1729" r:id="rId5174"/>
+    <hyperlink ref="B1730" r:id="rId5175"/>
+    <hyperlink ref="C1730" r:id="rId5176"/>
+    <hyperlink ref="E1730" r:id="rId5177"/>
+    <hyperlink ref="B1731" r:id="rId5178"/>
+    <hyperlink ref="C1731" r:id="rId5179"/>
+    <hyperlink ref="E1731" r:id="rId5180"/>
+    <hyperlink ref="B1732" r:id="rId5181"/>
+    <hyperlink ref="C1732" r:id="rId5182"/>
+    <hyperlink ref="E1732" r:id="rId5183"/>
+    <hyperlink ref="B1733" r:id="rId5184"/>
+    <hyperlink ref="C1733" r:id="rId5185"/>
+    <hyperlink ref="E1733" r:id="rId5186"/>
+    <hyperlink ref="B1734" r:id="rId5187"/>
+    <hyperlink ref="C1734" r:id="rId5188"/>
+    <hyperlink ref="E1734" r:id="rId5189"/>
+    <hyperlink ref="B1735" r:id="rId5190"/>
+    <hyperlink ref="C1735" r:id="rId5191"/>
+    <hyperlink ref="E1735" r:id="rId5192"/>
+    <hyperlink ref="B1736" r:id="rId5193"/>
+    <hyperlink ref="C1736" r:id="rId5194"/>
+    <hyperlink ref="E1736" r:id="rId5195"/>
+    <hyperlink ref="B1737" r:id="rId5196"/>
+    <hyperlink ref="C1737" r:id="rId5197"/>
+    <hyperlink ref="E1737" r:id="rId5198"/>
+    <hyperlink ref="B1738" r:id="rId5199"/>
+    <hyperlink ref="C1738" r:id="rId5200"/>
+    <hyperlink ref="E1738" r:id="rId5201"/>
+    <hyperlink ref="B1739" r:id="rId5202"/>
+    <hyperlink ref="C1739" r:id="rId5203"/>
+    <hyperlink ref="E1739" r:id="rId5204"/>
+    <hyperlink ref="B1740" r:id="rId5205"/>
+    <hyperlink ref="C1740" r:id="rId5206"/>
+    <hyperlink ref="E1740" r:id="rId5207"/>
+    <hyperlink ref="B1741" r:id="rId5208"/>
+    <hyperlink ref="C1741" r:id="rId5209"/>
+    <hyperlink ref="E1741" r:id="rId5210"/>
+    <hyperlink ref="B1742" r:id="rId5211"/>
+    <hyperlink ref="C1742" r:id="rId5212"/>
+    <hyperlink ref="E1742" r:id="rId5213"/>
+    <hyperlink ref="B1743" r:id="rId5214"/>
+    <hyperlink ref="C1743" r:id="rId5215"/>
+    <hyperlink ref="E1743" r:id="rId5216"/>
+    <hyperlink ref="B1744" r:id="rId5217"/>
+    <hyperlink ref="C1744" r:id="rId5218"/>
+    <hyperlink ref="E1744" r:id="rId5219"/>
+    <hyperlink ref="B1745" r:id="rId5220"/>
+    <hyperlink ref="C1745" r:id="rId5221"/>
+    <hyperlink ref="E1745" r:id="rId5222"/>
+    <hyperlink ref="B1746" r:id="rId5223"/>
+    <hyperlink ref="C1746" r:id="rId5224"/>
+    <hyperlink ref="E1746" r:id="rId5225"/>
+    <hyperlink ref="B1747" r:id="rId5226"/>
+    <hyperlink ref="C1747" r:id="rId5227"/>
+    <hyperlink ref="E1747" r:id="rId5228"/>
+    <hyperlink ref="B1748" r:id="rId5229"/>
+    <hyperlink ref="C1748" r:id="rId5230"/>
+    <hyperlink ref="E1748" r:id="rId5231"/>
+    <hyperlink ref="B1749" r:id="rId5232"/>
+    <hyperlink ref="C1749" r:id="rId5233"/>
+    <hyperlink ref="E1749" r:id="rId5234"/>
+    <hyperlink ref="B1750" r:id="rId5235"/>
+    <hyperlink ref="C1750" r:id="rId5236"/>
+    <hyperlink ref="E1750" r:id="rId5237"/>
+    <hyperlink ref="B1751" r:id="rId5238"/>
+    <hyperlink ref="C1751" r:id="rId5239"/>
+    <hyperlink ref="E1751" r:id="rId5240"/>
+    <hyperlink ref="B1752" r:id="rId5241"/>
+    <hyperlink ref="C1752" r:id="rId5242"/>
+    <hyperlink ref="E1752" r:id="rId5243"/>
+    <hyperlink ref="B1753" r:id="rId5244"/>
+    <hyperlink ref="C1753" r:id="rId5245"/>
+    <hyperlink ref="E1753" r:id="rId5246"/>
+    <hyperlink ref="B1754" r:id="rId5247"/>
+    <hyperlink ref="C1754" r:id="rId5248"/>
+    <hyperlink ref="E1754" r:id="rId5249"/>
+    <hyperlink ref="B1755" r:id="rId5250"/>
+    <hyperlink ref="C1755" r:id="rId5251"/>
+    <hyperlink ref="E1755" r:id="rId5252"/>
+    <hyperlink ref="B1756" r:id="rId5253"/>
+    <hyperlink ref="C1756" r:id="rId5254"/>
+    <hyperlink ref="E1756" r:id="rId5255"/>
+    <hyperlink ref="B1757" r:id="rId5256"/>
+    <hyperlink ref="C1757" r:id="rId5257"/>
+    <hyperlink ref="E1757" r:id="rId5258"/>
+    <hyperlink ref="B1758" r:id="rId5259"/>
+    <hyperlink ref="C1758" r:id="rId5260"/>
+    <hyperlink ref="E1758" r:id="rId5261"/>
+    <hyperlink ref="B1759" r:id="rId5262"/>
+    <hyperlink ref="C1759" r:id="rId5263"/>
+    <hyperlink ref="E1759" r:id="rId5264"/>
+    <hyperlink ref="B1760" r:id="rId5265"/>
+    <hyperlink ref="C1760" r:id="rId5266"/>
+    <hyperlink ref="E1760" r:id="rId5267"/>
+    <hyperlink ref="B1761" r:id="rId5268"/>
+    <hyperlink ref="C1761" r:id="rId5269"/>
+    <hyperlink ref="E1761" r:id="rId5270"/>
+    <hyperlink ref="B1762" r:id="rId5271"/>
+    <hyperlink ref="C1762" r:id="rId5272"/>
+    <hyperlink ref="E1762" r:id="rId5273"/>
+    <hyperlink ref="B1763" r:id="rId5274"/>
+    <hyperlink ref="C1763" r:id="rId5275"/>
+    <hyperlink ref="E1763" r:id="rId5276"/>
+    <hyperlink ref="B1764" r:id="rId5277"/>
+    <hyperlink ref="C1764" r:id="rId5278"/>
+    <hyperlink ref="E1764" r:id="rId5279" location="pullrequestreview-187798954"/>
+    <hyperlink ref="B1765" r:id="rId5280"/>
+    <hyperlink ref="C1765" r:id="rId5281"/>
+    <hyperlink ref="E1765" r:id="rId5282"/>
+    <hyperlink ref="B1766" r:id="rId5283"/>
+    <hyperlink ref="C1766" r:id="rId5284"/>
+    <hyperlink ref="E1766" r:id="rId5285"/>
+    <hyperlink ref="B1767" r:id="rId5286"/>
+    <hyperlink ref="C1767" r:id="rId5287"/>
+    <hyperlink ref="E1767" r:id="rId5288"/>
+    <hyperlink ref="B1768" r:id="rId5289"/>
+    <hyperlink ref="C1768" r:id="rId5290"/>
+    <hyperlink ref="E1768" r:id="rId5291"/>
+    <hyperlink ref="B1769" r:id="rId5292"/>
+    <hyperlink ref="C1769" r:id="rId5293"/>
+    <hyperlink ref="E1769" r:id="rId5294"/>
+    <hyperlink ref="B1770" r:id="rId5295"/>
+    <hyperlink ref="C1770" r:id="rId5296"/>
+    <hyperlink ref="E1770" r:id="rId5297"/>
+    <hyperlink ref="B1771" r:id="rId5298"/>
+    <hyperlink ref="C1771" r:id="rId5299"/>
+    <hyperlink ref="E1771" r:id="rId5300"/>
+    <hyperlink ref="B1772" r:id="rId5301"/>
+    <hyperlink ref="C1772" r:id="rId5302"/>
+    <hyperlink ref="E1772" r:id="rId5303"/>
+    <hyperlink ref="B1773" r:id="rId5304"/>
+    <hyperlink ref="C1773" r:id="rId5305"/>
+    <hyperlink ref="E1773" r:id="rId5306" location="pullrequestreview-187808202"/>
+    <hyperlink ref="B1774" r:id="rId5307"/>
+    <hyperlink ref="C1774" r:id="rId5308"/>
+    <hyperlink ref="E1774" r:id="rId5309" location="pullrequestreview-187807953"/>
+    <hyperlink ref="B1775" r:id="rId5310"/>
+    <hyperlink ref="C1775" r:id="rId5311"/>
+    <hyperlink ref="E1775" r:id="rId5312"/>
+    <hyperlink ref="B1776" r:id="rId5313"/>
+    <hyperlink ref="C1776" r:id="rId5314"/>
+    <hyperlink ref="E1776" r:id="rId5315"/>
+    <hyperlink ref="B1777" r:id="rId5316"/>
+    <hyperlink ref="C1777" r:id="rId5317"/>
+    <hyperlink ref="E1777" r:id="rId5318"/>
+    <hyperlink ref="B1778" r:id="rId5319"/>
+    <hyperlink ref="C1778" r:id="rId5320"/>
+    <hyperlink ref="E1778" r:id="rId5321"/>
+    <hyperlink ref="B1779" r:id="rId5322"/>
+    <hyperlink ref="C1779" r:id="rId5323"/>
+    <hyperlink ref="E1779" r:id="rId5324"/>
+    <hyperlink ref="B1780" r:id="rId5325"/>
+    <hyperlink ref="C1780" r:id="rId5326"/>
+    <hyperlink ref="E1780" r:id="rId5327"/>
+    <hyperlink ref="B1781" r:id="rId5328"/>
+    <hyperlink ref="C1781" r:id="rId5329"/>
+    <hyperlink ref="E1781" r:id="rId5330"/>
+    <hyperlink ref="B1782" r:id="rId5331"/>
+    <hyperlink ref="C1782" r:id="rId5332"/>
+    <hyperlink ref="E1782" r:id="rId5333" location="pullrequestreview-187951346"/>
+    <hyperlink ref="B1783" r:id="rId5334"/>
+    <hyperlink ref="C1783" r:id="rId5335"/>
+    <hyperlink ref="E1783" r:id="rId5336" location="pullrequestreview-187951565"/>
+    <hyperlink ref="B1784" r:id="rId5337"/>
+    <hyperlink ref="C1784" r:id="rId5338"/>
+    <hyperlink ref="E1784" r:id="rId5339"/>
+    <hyperlink ref="B1785" r:id="rId5340"/>
+    <hyperlink ref="C1785" r:id="rId5341"/>
+    <hyperlink ref="E1785" r:id="rId5342"/>
+    <hyperlink ref="B1786" r:id="rId5343"/>
+    <hyperlink ref="C1786" r:id="rId5344"/>
+    <hyperlink ref="E1786" r:id="rId5345"/>
+    <hyperlink ref="B1787" r:id="rId5346"/>
+    <hyperlink ref="C1787" r:id="rId5347"/>
+    <hyperlink ref="E1787" r:id="rId5348"/>
+    <hyperlink ref="B1788" r:id="rId5349"/>
+    <hyperlink ref="C1788" r:id="rId5350"/>
+    <hyperlink ref="E1788" r:id="rId5351"/>
+    <hyperlink ref="B1789" r:id="rId5352"/>
+    <hyperlink ref="C1789" r:id="rId5353"/>
+    <hyperlink ref="E1789" r:id="rId5354"/>
+    <hyperlink ref="B1790" r:id="rId5355"/>
+    <hyperlink ref="C1790" r:id="rId5356"/>
+    <hyperlink ref="E1790" r:id="rId5357"/>
+    <hyperlink ref="B1791" r:id="rId5358"/>
+    <hyperlink ref="C1791" r:id="rId5359"/>
+    <hyperlink ref="E1791" r:id="rId5360"/>
+    <hyperlink ref="B1792" r:id="rId5361"/>
+    <hyperlink ref="C1792" r:id="rId5362"/>
+    <hyperlink ref="E1792" r:id="rId5363"/>
+    <hyperlink ref="B1793" r:id="rId5364"/>
+    <hyperlink ref="C1793" r:id="rId5365"/>
+    <hyperlink ref="E1793" r:id="rId5366"/>
+    <hyperlink ref="B1794" r:id="rId5367"/>
+    <hyperlink ref="C1794" r:id="rId5368"/>
+    <hyperlink ref="E1794" r:id="rId5369"/>
+    <hyperlink ref="B1795" r:id="rId5370"/>
+    <hyperlink ref="C1795" r:id="rId5371"/>
+    <hyperlink ref="E1795" r:id="rId5372"/>
+    <hyperlink ref="B1796" r:id="rId5373"/>
+    <hyperlink ref="C1796" r:id="rId5374"/>
+    <hyperlink ref="E1796" r:id="rId5375"/>
+    <hyperlink ref="B1797" r:id="rId5376"/>
+    <hyperlink ref="C1797" r:id="rId5377"/>
+    <hyperlink ref="E1797" r:id="rId5378"/>
+    <hyperlink ref="B1798" r:id="rId5379"/>
+    <hyperlink ref="C1798" r:id="rId5380"/>
+    <hyperlink ref="E1798" r:id="rId5381"/>
+    <hyperlink ref="B1799" r:id="rId5382"/>
+    <hyperlink ref="C1799" r:id="rId5383"/>
+    <hyperlink ref="E1799" r:id="rId5384"/>
+    <hyperlink ref="B1800" r:id="rId5385"/>
+    <hyperlink ref="C1800" r:id="rId5386"/>
+    <hyperlink ref="E1800" r:id="rId5387"/>
+    <hyperlink ref="B1801" r:id="rId5388"/>
+    <hyperlink ref="C1801" r:id="rId5389"/>
+    <hyperlink ref="E1801" r:id="rId5390"/>
+    <hyperlink ref="B1802" r:id="rId5391"/>
+    <hyperlink ref="C1802" r:id="rId5392"/>
+    <hyperlink ref="E1802" r:id="rId5393"/>
+    <hyperlink ref="B1803" r:id="rId5394"/>
+    <hyperlink ref="C1803" r:id="rId5395"/>
+    <hyperlink ref="E1803" r:id="rId5396"/>
+    <hyperlink ref="B1804" r:id="rId5397"/>
+    <hyperlink ref="C1804" r:id="rId5398"/>
+    <hyperlink ref="E1804" r:id="rId5399" location="pullrequestreview-188324780"/>
+    <hyperlink ref="B1805" r:id="rId5400"/>
+    <hyperlink ref="C1805" r:id="rId5401"/>
+    <hyperlink ref="E1805" r:id="rId5402"/>
+    <hyperlink ref="B1806" r:id="rId5403"/>
+    <hyperlink ref="C1806" r:id="rId5404"/>
+    <hyperlink ref="E1806" r:id="rId5405" location="pullrequestreview-188380836"/>
+    <hyperlink ref="B1807" r:id="rId5406"/>
+    <hyperlink ref="C1807" r:id="rId5407"/>
+    <hyperlink ref="E1807" r:id="rId5408"/>
+    <hyperlink ref="B1808" r:id="rId5409"/>
+    <hyperlink ref="C1808" r:id="rId5410"/>
+    <hyperlink ref="E1808" r:id="rId5411"/>
+    <hyperlink ref="B1809" r:id="rId5412"/>
+    <hyperlink ref="C1809" r:id="rId5413"/>
+    <hyperlink ref="E1809" r:id="rId5414"/>
+    <hyperlink ref="B1810" r:id="rId5415"/>
+    <hyperlink ref="C1810" r:id="rId5416"/>
+    <hyperlink ref="E1810" r:id="rId5417"/>
+    <hyperlink ref="B1811" r:id="rId5418"/>
+    <hyperlink ref="C1811" r:id="rId5419"/>
+    <hyperlink ref="E1811" r:id="rId5420"/>
+    <hyperlink ref="B1812" r:id="rId5421"/>
+    <hyperlink ref="C1812" r:id="rId5422"/>
+    <hyperlink ref="E1812" r:id="rId5423"/>
+    <hyperlink ref="B1813" r:id="rId5424"/>
+    <hyperlink ref="C1813" r:id="rId5425"/>
+    <hyperlink ref="E1813" r:id="rId5426"/>
+    <hyperlink ref="B1814" r:id="rId5427"/>
+    <hyperlink ref="C1814" r:id="rId5428"/>
+    <hyperlink ref="E1814" r:id="rId5429"/>
+    <hyperlink ref="B1815" r:id="rId5430"/>
+    <hyperlink ref="C1815" r:id="rId5431"/>
+    <hyperlink ref="E1815" r:id="rId5432"/>
+    <hyperlink ref="B1816" r:id="rId5433"/>
+    <hyperlink ref="C1816" r:id="rId5434"/>
+    <hyperlink ref="E1816" r:id="rId5435"/>
+    <hyperlink ref="B1817" r:id="rId5436"/>
+    <hyperlink ref="C1817" r:id="rId5437"/>
+    <hyperlink ref="E1817" r:id="rId5438"/>
+    <hyperlink ref="B1818" r:id="rId5439"/>
+    <hyperlink ref="C1818" r:id="rId5440"/>
+    <hyperlink ref="E1818" r:id="rId5441"/>
+    <hyperlink ref="B1819" r:id="rId5442"/>
+    <hyperlink ref="C1819" r:id="rId5443"/>
+    <hyperlink ref="E1819" r:id="rId5444"/>
+    <hyperlink ref="B1820" r:id="rId5445"/>
+    <hyperlink ref="C1820" r:id="rId5446"/>
+    <hyperlink ref="E1820" r:id="rId5447"/>
+    <hyperlink ref="B1821" r:id="rId5448"/>
+    <hyperlink ref="C1821" r:id="rId5449"/>
+    <hyperlink ref="E1821" r:id="rId5450"/>
+    <hyperlink ref="B1822" r:id="rId5451"/>
+    <hyperlink ref="C1822" r:id="rId5452"/>
+    <hyperlink ref="E1822" r:id="rId5453"/>
+    <hyperlink ref="B1823" r:id="rId5454"/>
+    <hyperlink ref="C1823" r:id="rId5455"/>
+    <hyperlink ref="E1823" r:id="rId5456"/>
+    <hyperlink ref="B1824" r:id="rId5457"/>
+    <hyperlink ref="C1824" r:id="rId5458"/>
+    <hyperlink ref="E1824" r:id="rId5459"/>
+    <hyperlink ref="B1825" r:id="rId5460"/>
+    <hyperlink ref="C1825" r:id="rId5461"/>
+    <hyperlink ref="E1825" r:id="rId5462"/>
+    <hyperlink ref="B1826" r:id="rId5463"/>
+    <hyperlink ref="C1826" r:id="rId5464"/>
+    <hyperlink ref="E1826" r:id="rId5465"/>
+    <hyperlink ref="B1827" r:id="rId5466"/>
+    <hyperlink ref="C1827" r:id="rId5467"/>
+    <hyperlink ref="E1827" r:id="rId5468"/>
+    <hyperlink ref="B1828" r:id="rId5469"/>
+    <hyperlink ref="C1828" r:id="rId5470"/>
+    <hyperlink ref="E1828" r:id="rId5471"/>
+    <hyperlink ref="B1829" r:id="rId5472"/>
+    <hyperlink ref="C1829" r:id="rId5473"/>
+    <hyperlink ref="E1829" r:id="rId5474"/>
+    <hyperlink ref="B1830" r:id="rId5475"/>
+    <hyperlink ref="C1830" r:id="rId5476"/>
+    <hyperlink ref="E1830" r:id="rId5477"/>
+    <hyperlink ref="B1831" r:id="rId5478"/>
+    <hyperlink ref="C1831" r:id="rId5479"/>
+    <hyperlink ref="E1831" r:id="rId5480"/>
+    <hyperlink ref="B1832" r:id="rId5481"/>
+    <hyperlink ref="C1832" r:id="rId5482"/>
+    <hyperlink ref="E1832" r:id="rId5483"/>
+    <hyperlink ref="B1833" r:id="rId5484"/>
+    <hyperlink ref="C1833" r:id="rId5485"/>
+    <hyperlink ref="E1833" r:id="rId5486"/>
+    <hyperlink ref="B1834" r:id="rId5487"/>
+    <hyperlink ref="C1834" r:id="rId5488"/>
+    <hyperlink ref="E1834" r:id="rId5489"/>
+    <hyperlink ref="B1835" r:id="rId5490"/>
+    <hyperlink ref="C1835" r:id="rId5491"/>
+    <hyperlink ref="E1835" r:id="rId5492"/>
+    <hyperlink ref="B1836" r:id="rId5493"/>
+    <hyperlink ref="C1836" r:id="rId5494"/>
+    <hyperlink ref="E1836" r:id="rId5495"/>
+    <hyperlink ref="B1837" r:id="rId5496"/>
+    <hyperlink ref="C1837" r:id="rId5497"/>
+    <hyperlink ref="E1837" r:id="rId5498"/>
+    <hyperlink ref="B1838" r:id="rId5499"/>
+    <hyperlink ref="C1838" r:id="rId5500"/>
+    <hyperlink ref="E1838" r:id="rId5501"/>
+    <hyperlink ref="B1839" r:id="rId5502"/>
+    <hyperlink ref="C1839" r:id="rId5503"/>
+    <hyperlink ref="E1839" r:id="rId5504"/>
+    <hyperlink ref="B1840" r:id="rId5505"/>
+    <hyperlink ref="C1840" r:id="rId5506"/>
+    <hyperlink ref="E1840" r:id="rId5507"/>
+    <hyperlink ref="B1841" r:id="rId5508"/>
+    <hyperlink ref="C1841" r:id="rId5509"/>
+    <hyperlink ref="E1841" r:id="rId5510"/>
+    <hyperlink ref="B1842" r:id="rId5511"/>
+    <hyperlink ref="C1842" r:id="rId5512"/>
+    <hyperlink ref="E1842" r:id="rId5513"/>
+    <hyperlink ref="B1843" r:id="rId5514"/>
+    <hyperlink ref="C1843" r:id="rId5515"/>
+    <hyperlink ref="E1843" r:id="rId5516"/>
+    <hyperlink ref="B1844" r:id="rId5517"/>
+    <hyperlink ref="C1844" r:id="rId5518"/>
+    <hyperlink ref="E1844" r:id="rId5519"/>
+    <hyperlink ref="B1845" r:id="rId5520"/>
+    <hyperlink ref="C1845" r:id="rId5521"/>
+    <hyperlink ref="E1845" r:id="rId5522"/>
+    <hyperlink ref="B1846" r:id="rId5523"/>
+    <hyperlink ref="C1846" r:id="rId5524"/>
+    <hyperlink ref="E1846" r:id="rId5525"/>
+    <hyperlink ref="B1847" r:id="rId5526"/>
+    <hyperlink ref="C1847" r:id="rId5527"/>
+    <hyperlink ref="E1847" r:id="rId5528"/>
+    <hyperlink ref="B1848" r:id="rId5529"/>
+    <hyperlink ref="C1848" r:id="rId5530"/>
+    <hyperlink ref="E1848" r:id="rId5531"/>
+    <hyperlink ref="B1849" r:id="rId5532"/>
+    <hyperlink ref="C1849" r:id="rId5533"/>
+    <hyperlink ref="E1849" r:id="rId5534"/>
+    <hyperlink ref="B1850" r:id="rId5535"/>
+    <hyperlink ref="C1850" r:id="rId5536"/>
+    <hyperlink ref="E1850" r:id="rId5537"/>
+    <hyperlink ref="B1851" r:id="rId5538"/>
+    <hyperlink ref="C1851" r:id="rId5539"/>
+    <hyperlink ref="E1851" r:id="rId5540"/>
+    <hyperlink ref="B1852" r:id="rId5541"/>
+    <hyperlink ref="C1852" r:id="rId5542"/>
+    <hyperlink ref="E1852" r:id="rId5543"/>
+    <hyperlink ref="B1853" r:id="rId5544"/>
+    <hyperlink ref="C1853" r:id="rId5545"/>
+    <hyperlink ref="E1853" r:id="rId5546"/>
+    <hyperlink ref="B1854" r:id="rId5547"/>
+    <hyperlink ref="C1854" r:id="rId5548"/>
+    <hyperlink ref="E1854" r:id="rId5549"/>
+    <hyperlink ref="B1855" r:id="rId5550"/>
+    <hyperlink ref="C1855" r:id="rId5551"/>
+    <hyperlink ref="E1855" r:id="rId5552"/>
+    <hyperlink ref="B1856" r:id="rId5553"/>
+    <hyperlink ref="C1856" r:id="rId5554"/>
+    <hyperlink ref="E1856" r:id="rId5555"/>
+    <hyperlink ref="B1857" r:id="rId5556"/>
+    <hyperlink ref="C1857" r:id="rId5557"/>
+    <hyperlink ref="E1857" r:id="rId5558"/>
+    <hyperlink ref="B1858" r:id="rId5559"/>
+    <hyperlink ref="C1858" r:id="rId5560"/>
+    <hyperlink ref="E1858" r:id="rId5561"/>
+    <hyperlink ref="B1859" r:id="rId5562"/>
+    <hyperlink ref="C1859" r:id="rId5563"/>
+    <hyperlink ref="E1859" r:id="rId5564"/>
+    <hyperlink ref="B1860" r:id="rId5565"/>
+    <hyperlink ref="C1860" r:id="rId5566"/>
+    <hyperlink ref="E1860" r:id="rId5567"/>
+    <hyperlink ref="B1861" r:id="rId5568"/>
+    <hyperlink ref="C1861" r:id="rId5569"/>
+    <hyperlink ref="E1861" r:id="rId5570"/>
+    <hyperlink ref="B1862" r:id="rId5571"/>
+    <hyperlink ref="C1862" r:id="rId5572"/>
+    <hyperlink ref="E1862" r:id="rId5573"/>
+    <hyperlink ref="B1863" r:id="rId5574"/>
+    <hyperlink ref="C1863" r:id="rId5575"/>
+    <hyperlink ref="E1863" r:id="rId5576"/>
+    <hyperlink ref="B1864" r:id="rId5577"/>
+    <hyperlink ref="C1864" r:id="rId5578"/>
+    <hyperlink ref="E1864" r:id="rId5579"/>
+    <hyperlink ref="B1865" r:id="rId5580"/>
+    <hyperlink ref="C1865" r:id="rId5581"/>
+    <hyperlink ref="E1865" r:id="rId5582"/>
+    <hyperlink ref="B1300" r:id="rId5583"/>
+    <hyperlink ref="C1300" r:id="rId5584"/>
+    <hyperlink ref="E1300" r:id="rId5585" display="https://github.com/rolling-scopes-school/svyatlo-2018Q3/pull/3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>